<commit_message>
Added data directory with vocab and images
</commit_message>
<xml_diff>
--- a/data/vocab.xlsx
+++ b/data/vocab.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\Czech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CzechTutor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A67828-6B63-448F-A800-CE25E075DC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985D9962-F419-48D8-8523-162A0F78B85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
   </bookViews>
@@ -3548,13 +3548,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3893,27 +3893,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>562</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>563</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>558</v>
       </c>
@@ -3938,16 +3938,16 @@
       <c r="I2" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="J2" s="8"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>556</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>557</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="8"/>
       <c r="D3" t="s">
         <v>564</v>
       </c>
@@ -3957,10 +3957,10 @@
       <c r="F3" t="s">
         <v>566</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="8"/>
       <c r="I3" t="s">
         <v>564</v>
       </c>
@@ -3972,10 +3972,10 @@
       <c r="A4" t="s">
         <v>568</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="8"/>
       <c r="D4" t="s">
         <v>571</v>
       </c>
@@ -3985,10 +3985,10 @@
       <c r="F4" t="s">
         <v>573</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>572</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>571</v>
       </c>
@@ -4000,10 +4000,10 @@
       <c r="A5" t="s">
         <v>670</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>671</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>672</v>
       </c>
@@ -4013,10 +4013,10 @@
       <c r="F5" t="s">
         <v>674</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>672</v>
       </c>
@@ -4028,10 +4028,10 @@
       <c r="A6" t="s">
         <v>676</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>677</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>678</v>
       </c>
@@ -4041,10 +4041,10 @@
       <c r="F6" t="s">
         <v>680</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>678</v>
       </c>
@@ -4056,10 +4056,10 @@
       <c r="A7" t="s">
         <v>681</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>683</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="8"/>
       <c r="D7" t="s">
         <v>684</v>
       </c>
@@ -4069,10 +4069,10 @@
       <c r="F7" t="s">
         <v>686</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>685</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>684</v>
       </c>
@@ -4084,10 +4084,10 @@
       <c r="A8" t="s">
         <v>689</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>688</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="8"/>
       <c r="D8" t="s">
         <v>690</v>
       </c>
@@ -4097,10 +4097,10 @@
       <c r="F8" t="s">
         <v>692</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="8"/>
       <c r="I8" t="s">
         <v>690</v>
       </c>
@@ -4112,10 +4112,10 @@
       <c r="A9" t="s">
         <v>694</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="8"/>
       <c r="D9" t="s">
         <v>696</v>
       </c>
@@ -4125,10 +4125,10 @@
       <c r="F9" t="s">
         <v>698</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="8" t="s">
         <v>697</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="8"/>
       <c r="I9" t="s">
         <v>696</v>
       </c>
@@ -4140,10 +4140,10 @@
       <c r="A10" t="s">
         <v>703</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>700</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="8"/>
       <c r="D10" t="s">
         <v>701</v>
       </c>
@@ -4153,10 +4153,10 @@
       <c r="F10" t="s">
         <v>704</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="8" t="s">
         <v>702</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="8"/>
       <c r="I10" t="s">
         <v>701</v>
       </c>
@@ -4168,10 +4168,10 @@
       <c r="A11" t="s">
         <v>706</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="8"/>
       <c r="D11" t="s">
         <v>705</v>
       </c>
@@ -4181,10 +4181,10 @@
       <c r="F11" t="s">
         <v>705</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="8"/>
       <c r="I11" t="s">
         <v>705</v>
       </c>
@@ -4196,10 +4196,10 @@
       <c r="A12" t="s">
         <v>708</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>709</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="8"/>
       <c r="D12" t="s">
         <v>711</v>
       </c>
@@ -4209,10 +4209,10 @@
       <c r="F12" t="s">
         <v>713</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="8" t="s">
         <v>712</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="8"/>
       <c r="I12" t="s">
         <v>711</v>
       </c>
@@ -4224,10 +4224,10 @@
       <c r="A13" t="s">
         <v>714</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>715</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="8"/>
       <c r="D13" t="s">
         <v>717</v>
       </c>
@@ -4237,10 +4237,10 @@
       <c r="F13" t="s">
         <v>719</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>718</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="8"/>
       <c r="I13" t="s">
         <v>717</v>
       </c>
@@ -4249,134 +4249,114 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="B19:C19"/>
@@ -4393,17 +4373,37 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" location="Czech" xr:uid="{5941DCB9-FDEB-4587-B027-375759EB9DA4}"/>
@@ -6059,7 +6059,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed bug for hamster plural, and added image urls for city topic
</commit_message>
<xml_diff>
--- a/data/vocab.xlsx
+++ b/data/vocab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CzechTutor\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\Czech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985D9962-F419-48D8-8523-162A0F78B85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063F8E31-A399-4A67-B71E-0EFC038C65CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
   </bookViews>
   <sheets>
     <sheet name="Adjectives" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1656" uniqueCount="1184">
   <si>
     <t>English</t>
   </si>
@@ -3485,6 +3485,123 @@
   </si>
   <si>
     <t>https://free-images.com/lg/b48a/lamb_sheep_young_animal.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/376b/airport_aviation_safety_413817.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/0eab/apartments_city_high_rise.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/42c9/bakery_sweets_candy_chocolate.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d91f/national_bank_belgium_371288.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/8db7/meat_butchery_red_meat.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b177/castle_castle_castle_knight_9.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/98f8/chester_cathedral_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/8d2a/church_high_tower.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/410e/city_streets_skyline_buildings.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1d75/night_festival_club_music.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b2cb/club_house_golf_country.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b2ca/hospital_fire_training_to.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3ea0/beds_youth_hostel_bunk.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/dd55/hotel_room_bed_hotel.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/502a/house_8.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/c27c/south_library_shelves.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/074d/market_vegetable_market_1558658.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/cc57/office_office_complex_glass.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1049/metro_metro_station_transport.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d8b0/park_walkway.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/ede1/medical_medicine_pharmacy_1454513.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/fb06/port_container_gantry_crane.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/2607/russia_post_office_post.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/098d/pub_pool_table_entertainment.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/defa/restaurant_cafe_einstein_restaurant.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/267e/classroom_chinese_education_room.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/c9d2/candy_shop_shop_goods.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d2b0/fountain_zary_town_square_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/e33f/station_light_station_s.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b44d/statue_liberty_skyline_962263.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3765/bus_stop_waiting_bus.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/47cc/street_urban_part_town.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a07e/thatchedroof_house_settlement_with.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/24b8/supermarket_shelves_shopping_507295.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/9afe/swimming_pool_indoor_swimming.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/5d60/tower_pe_c3_b1erudes.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/14fb/old_town_town_center.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/f937/tram_sarajevo_former_wiener.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/2ddf/universit_c3_a4tsklinikum_ulm.jpg</t>
   </si>
 </sst>
 </file>
@@ -6058,8 +6175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A83DE8-6398-4B6D-9AFD-F64AA71A004A}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6919,10 +7036,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4FF4F7-C7FC-4558-887A-7BA51F1283D1}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6932,9 +7049,10 @@
     <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6950,8 +7068,11 @@
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>363</v>
       </c>
@@ -6967,8 +7088,11 @@
       <c r="E2" s="1" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>288</v>
       </c>
@@ -6984,8 +7108,11 @@
       <c r="E3" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>283</v>
       </c>
@@ -7001,8 +7128,11 @@
       <c r="E4" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>312</v>
       </c>
@@ -7018,8 +7148,11 @@
       <c r="E5" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>313</v>
       </c>
@@ -7035,8 +7168,11 @@
       <c r="E6" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>296</v>
       </c>
@@ -7052,8 +7188,11 @@
       <c r="E7" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1027</v>
       </c>
@@ -7069,8 +7208,11 @@
       <c r="E8" s="1" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>277</v>
       </c>
@@ -7086,8 +7228,11 @@
       <c r="E9" s="1" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>252</v>
       </c>
@@ -7103,8 +7248,11 @@
       <c r="E10" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>372</v>
       </c>
@@ -7120,8 +7268,11 @@
       <c r="E11" s="1" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1004</v>
       </c>
@@ -7131,8 +7282,11 @@
       <c r="D12" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>344</v>
       </c>
@@ -7148,8 +7302,11 @@
       <c r="E13" s="1" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>384</v>
       </c>
@@ -7165,8 +7322,11 @@
       <c r="E14" s="1" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>380</v>
       </c>
@@ -7182,8 +7342,11 @@
       <c r="E15" s="1" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>262</v>
       </c>
@@ -7199,8 +7362,11 @@
       <c r="E16" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>321</v>
       </c>
@@ -7216,8 +7382,11 @@
       <c r="E17" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>316</v>
       </c>
@@ -7233,8 +7402,11 @@
       <c r="E18" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>337</v>
       </c>
@@ -7250,8 +7422,11 @@
       <c r="E19" s="1" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>655</v>
       </c>
@@ -7267,8 +7442,11 @@
       <c r="E20" s="1" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>359</v>
       </c>
@@ -7284,8 +7462,11 @@
       <c r="E21" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>299</v>
       </c>
@@ -7301,8 +7482,11 @@
       <c r="E22" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>364</v>
       </c>
@@ -7318,8 +7502,11 @@
       <c r="E23" s="1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>284</v>
       </c>
@@ -7335,8 +7522,11 @@
       <c r="E24" s="1" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>368</v>
       </c>
@@ -7352,8 +7542,11 @@
       <c r="E25" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>377</v>
       </c>
@@ -7369,8 +7562,11 @@
       <c r="E26" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="1" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>348</v>
       </c>
@@ -7386,8 +7582,11 @@
       <c r="E27" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="1" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>273</v>
       </c>
@@ -7403,8 +7602,11 @@
       <c r="E28" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="1" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>270</v>
       </c>
@@ -7420,8 +7622,11 @@
       <c r="E29" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" s="1" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>307</v>
       </c>
@@ -7437,8 +7642,11 @@
       <c r="E30" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" s="1" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>392</v>
       </c>
@@ -7454,8 +7662,11 @@
       <c r="E31" s="1" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="1" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>332</v>
       </c>
@@ -7471,8 +7682,11 @@
       <c r="E32" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="1" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>268</v>
       </c>
@@ -7488,8 +7702,11 @@
       <c r="E33" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="1" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>394</v>
       </c>
@@ -7505,8 +7722,11 @@
       <c r="E34" s="1" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="1" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>304</v>
       </c>
@@ -7522,8 +7742,11 @@
       <c r="E35" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" s="1" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>355</v>
       </c>
@@ -7539,8 +7762,11 @@
       <c r="E36" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" s="1" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>325</v>
       </c>
@@ -7556,8 +7782,11 @@
       <c r="E37" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" s="1" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>255</v>
       </c>
@@ -7573,8 +7802,11 @@
       <c r="E38" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" s="1" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>340</v>
       </c>
@@ -7590,8 +7822,11 @@
       <c r="E39" s="1" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" s="1" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>350</v>
       </c>
@@ -7606,6 +7841,9 @@
       </c>
       <c r="E40" s="1" t="s">
         <v>352</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>1183</v>
       </c>
     </row>
   </sheetData>
@@ -7651,6 +7889,45 @@
     <hyperlink ref="E34" r:id="rId36" location="Czech" xr:uid="{F0DF73B3-7BC6-497F-8E2E-7ED4E75C1E28}"/>
     <hyperlink ref="E20" r:id="rId37" location="Czech" xr:uid="{49774962-6028-496C-860D-EE9E6E1EF54C}"/>
     <hyperlink ref="E8" r:id="rId38" location="Czech" xr:uid="{5EAEE623-8274-4002-9D7B-105304776E58}"/>
+    <hyperlink ref="F2" r:id="rId39" xr:uid="{848CA005-AB88-455D-98C3-1CEAC84865FB}"/>
+    <hyperlink ref="F3" r:id="rId40" xr:uid="{45AF1CD9-2226-4BC9-AC51-F67211C8AAC1}"/>
+    <hyperlink ref="F4" r:id="rId41" xr:uid="{A409BEA8-4228-4960-B9F2-E116867B379D}"/>
+    <hyperlink ref="F5" r:id="rId42" xr:uid="{D92C0DFF-FCDB-457E-9EF8-1504E50C4B40}"/>
+    <hyperlink ref="F6" r:id="rId43" xr:uid="{B480FA19-4A92-4FE6-8DC6-E2770660A3EA}"/>
+    <hyperlink ref="F7" r:id="rId44" xr:uid="{7B281F87-ADD6-4FD2-B8A0-71AC411DA7B0}"/>
+    <hyperlink ref="F8" r:id="rId45" xr:uid="{CAE7D724-F5BC-432B-9C84-0B53AD7455FF}"/>
+    <hyperlink ref="F9" r:id="rId46" xr:uid="{CD565EE9-033A-4565-90A6-30F716071F77}"/>
+    <hyperlink ref="F10" r:id="rId47" xr:uid="{471F5768-0829-4CEF-A522-FA39BA5F5EE2}"/>
+    <hyperlink ref="F12" r:id="rId48" xr:uid="{1FA22728-C587-4A22-9481-9CBCC4E51089}"/>
+    <hyperlink ref="F11" r:id="rId49" xr:uid="{5B137EC4-F81A-4B00-A362-FA8224B889F6}"/>
+    <hyperlink ref="F13" r:id="rId50" xr:uid="{B43A2A52-59D5-4F7A-964E-07F90E0C91DD}"/>
+    <hyperlink ref="F14" r:id="rId51" xr:uid="{7DBFD75F-6275-4085-9EC2-E28F6BA6F2BF}"/>
+    <hyperlink ref="F15" r:id="rId52" xr:uid="{D47388E8-8D39-4137-A17D-3979FFC960DA}"/>
+    <hyperlink ref="F16" r:id="rId53" xr:uid="{BB1F3EF0-32F0-4194-958C-E4C3346408FC}"/>
+    <hyperlink ref="F17" r:id="rId54" xr:uid="{F2DAC8C7-9633-449F-AA57-9516344543A1}"/>
+    <hyperlink ref="F18" r:id="rId55" xr:uid="{7C0D8AB0-3265-4246-81FE-C35CBA4D9DA9}"/>
+    <hyperlink ref="F20" r:id="rId56" xr:uid="{F8C25553-CD78-4C7A-8E01-A614E025CF8A}"/>
+    <hyperlink ref="F19" r:id="rId57" xr:uid="{3B812E5A-F336-459B-B599-05D1B2CC0D25}"/>
+    <hyperlink ref="F21" r:id="rId58" xr:uid="{6C4EC7D6-E3A8-41A0-97C5-26B5D0695873}"/>
+    <hyperlink ref="F22" r:id="rId59" xr:uid="{51BFA554-CEBA-4E7F-A467-DA1DF26DB4B9}"/>
+    <hyperlink ref="F23" r:id="rId60" xr:uid="{EC78ED7F-999D-4C1B-AABC-F94FE5064109}"/>
+    <hyperlink ref="F24" r:id="rId61" xr:uid="{46B1BBB3-F237-4EC9-A0D4-EF7EC84FBF6E}"/>
+    <hyperlink ref="F25" r:id="rId62" xr:uid="{8D683CA9-4AB3-45C0-81CE-58F82581FA95}"/>
+    <hyperlink ref="F26" r:id="rId63" xr:uid="{165753FE-6E76-4F65-ADB0-3C0598689D9E}"/>
+    <hyperlink ref="F27" r:id="rId64" xr:uid="{EA9CB9A5-1796-45D8-BF72-2FB5DC634265}"/>
+    <hyperlink ref="F28" r:id="rId65" xr:uid="{9684DA43-6441-4294-A859-DB3C97CE1228}"/>
+    <hyperlink ref="F29" r:id="rId66" xr:uid="{DD22E862-92F8-4299-9AA9-DA617D61B8A2}"/>
+    <hyperlink ref="F30" r:id="rId67" xr:uid="{DF6D44AA-94BF-44D3-A48A-3444B463F2F7}"/>
+    <hyperlink ref="F31" r:id="rId68" xr:uid="{DDE009AF-EDFA-4657-A038-49FD7E209F7F}"/>
+    <hyperlink ref="F32" r:id="rId69" xr:uid="{CA703502-E512-4F14-AC28-E29855310BCD}"/>
+    <hyperlink ref="F33" r:id="rId70" xr:uid="{D9959C68-4F76-400F-9A97-25C94CF61DFD}"/>
+    <hyperlink ref="F34" r:id="rId71" xr:uid="{486E112D-6716-40D6-8176-F9350DC19DE4}"/>
+    <hyperlink ref="F35" r:id="rId72" xr:uid="{D45E0FCD-B2AD-4326-922C-866A98C53C36}"/>
+    <hyperlink ref="F36" r:id="rId73" xr:uid="{16CB97F9-4518-4009-A4DE-CEDDD1B75F66}"/>
+    <hyperlink ref="F37" r:id="rId74" xr:uid="{80A390BD-EA40-437C-955B-386CA21755F1}"/>
+    <hyperlink ref="F38" r:id="rId75" xr:uid="{30B58AF3-6257-4AD1-A756-CC04EAA66BA7}"/>
+    <hyperlink ref="F39" r:id="rId76" xr:uid="{0780753F-EF44-4886-B750-3D84C6F27521}"/>
+    <hyperlink ref="F40" r:id="rId77" xr:uid="{E77524E5-DE37-4687-A7EC-E01254B77C04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added House topic and image urls for house topic
</commit_message>
<xml_diff>
--- a/data/vocab.xlsx
+++ b/data/vocab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\Czech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632D1267-2F9B-4391-A22A-957A7D077A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B40B9E4-CD89-4B32-8DEB-A135DC0047E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="1274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="1330">
   <si>
     <t>English</t>
   </si>
@@ -3872,6 +3872,174 @@
   </si>
   <si>
     <t>https://free-images.com/lg/1826/dinner_table_fancy_dinner.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/6354/homes_for_sale_attic.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/2357/basement_walls_interior_room.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/086e/bathroom_luxury_luxury_bathroom.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/0b34/bed_double_bed_hotel.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/7ed4/bedroom_bed_pillows_headboard.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/5049/recycling_bins_3_refuse.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/44b9/heating_tankless_water_heater.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/9f3f/books_tcp_ip_network.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/db05/book_bookcase_reading_254048.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/9ace/bowl_mixing_bowl_dirty_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/c1a2/box_wooden_box_casket.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1efa/cabinet_70th_old_wallpaper.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/221a/calendar_2016_2016_calendar_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/79f7/chair_garden_green_hedge.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/7f60/computer_student_students_491760.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/0d23/cup_tea_coffee_tea.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/7692/cushion_cushions_fabric_sofa.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/dbcf/apple_desk_office_technology.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b50d/dining_room_dining_table.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a00e/fork_cutlery_metal_fork_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/073b/tiefkuhlschublade_jpeg.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3203/missing_fridge_light_makes.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a7ed/garden_garden_door_cottage.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/6400/glass_wine_glass_wine_2.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/42f2/home_blue_home_blue.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/4623/house_10.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d92e/kettle_glass_body_stainless.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a69a/kitchen_open_home_house.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3728/knife_serrated_kitchen_slice.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/71d4/laptop_at_night_laptop_5.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/6cb9/oven_stove_fireplace_doors_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b134/pan_cook_sear_frying.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/2bec/picture_instant_polaroid_vintage.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/58ef/pillows_bed_bedding_bedroom_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/c57b/plate_stack_plate_stack.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1509/pot_boiling_water_heiss.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/f23f/radiator_heating_flat_radiators.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/md/fab4/radio_vintage_retro_music.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/8892/family_room_living_room.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/e68e/shower_bathroom_large_spa.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/ebf6/basin_sink_kitchen_sink_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a37e/leather_sofa_recliner_sofa.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/5ff4/soup_spoon_cutlery_metal.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/6120/staircase_stairs_architecture_643121.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b6c1/tables_chairs_table_restaurant.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d581/tv_lcd_television_screen.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/bb9c/wc_toilet_purely_public_1.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/display/towels_bath_towels_bath.html</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b764/wall_bricks_bricks_wall_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/8644/dressing_room_wardrobe_design.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b52a/window_grilles_window_grid.jpg</t>
+  </si>
+  <si>
+    <t>blackberry</t>
+  </si>
+  <si>
+    <t>ostružina</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/ostru%C5%BEina#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3455/blackberry_bramble_berry_fruit.jpg</t>
+  </si>
+  <si>
+    <t>ostružiny</t>
   </si>
 </sst>
 </file>
@@ -3935,13 +4103,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4280,27 +4448,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>554</v>
       </c>
@@ -4325,16 +4493,16 @@
       <c r="I2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="J2" s="8"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>552</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="8"/>
       <c r="D3" t="s">
         <v>560</v>
       </c>
@@ -4344,10 +4512,10 @@
       <c r="F3" t="s">
         <v>562</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="8"/>
       <c r="I3" t="s">
         <v>560</v>
       </c>
@@ -4359,10 +4527,10 @@
       <c r="A4" t="s">
         <v>564</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="8"/>
       <c r="D4" t="s">
         <v>567</v>
       </c>
@@ -4372,10 +4540,10 @@
       <c r="F4" t="s">
         <v>569</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>567</v>
       </c>
@@ -4387,10 +4555,10 @@
       <c r="A5" t="s">
         <v>666</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>667</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>668</v>
       </c>
@@ -4400,10 +4568,10 @@
       <c r="F5" t="s">
         <v>670</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>668</v>
       </c>
@@ -4415,10 +4583,10 @@
       <c r="A6" t="s">
         <v>672</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>674</v>
       </c>
@@ -4428,10 +4596,10 @@
       <c r="F6" t="s">
         <v>676</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>675</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>674</v>
       </c>
@@ -4443,10 +4611,10 @@
       <c r="A7" t="s">
         <v>677</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="8"/>
       <c r="D7" t="s">
         <v>680</v>
       </c>
@@ -4456,10 +4624,10 @@
       <c r="F7" t="s">
         <v>682</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>681</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>680</v>
       </c>
@@ -4471,10 +4639,10 @@
       <c r="A8" t="s">
         <v>685</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>684</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="8"/>
       <c r="D8" t="s">
         <v>686</v>
       </c>
@@ -4484,10 +4652,10 @@
       <c r="F8" t="s">
         <v>688</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="8"/>
       <c r="I8" t="s">
         <v>686</v>
       </c>
@@ -4499,10 +4667,10 @@
       <c r="A9" t="s">
         <v>690</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="8"/>
       <c r="D9" t="s">
         <v>692</v>
       </c>
@@ -4512,10 +4680,10 @@
       <c r="F9" t="s">
         <v>694</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="8" t="s">
         <v>693</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="8"/>
       <c r="I9" t="s">
         <v>692</v>
       </c>
@@ -4527,10 +4695,10 @@
       <c r="A10" t="s">
         <v>699</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>696</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="8"/>
       <c r="D10" t="s">
         <v>697</v>
       </c>
@@ -4540,10 +4708,10 @@
       <c r="F10" t="s">
         <v>700</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="8"/>
       <c r="I10" t="s">
         <v>697</v>
       </c>
@@ -4555,10 +4723,10 @@
       <c r="A11" t="s">
         <v>702</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="8"/>
       <c r="D11" t="s">
         <v>701</v>
       </c>
@@ -4568,10 +4736,10 @@
       <c r="F11" t="s">
         <v>701</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="8"/>
       <c r="I11" t="s">
         <v>701</v>
       </c>
@@ -4583,10 +4751,10 @@
       <c r="A12" t="s">
         <v>704</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="8"/>
       <c r="D12" t="s">
         <v>707</v>
       </c>
@@ -4596,10 +4764,10 @@
       <c r="F12" t="s">
         <v>709</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="8" t="s">
         <v>708</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="8"/>
       <c r="I12" t="s">
         <v>707</v>
       </c>
@@ -4611,10 +4779,10 @@
       <c r="A13" t="s">
         <v>710</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="8"/>
       <c r="D13" t="s">
         <v>713</v>
       </c>
@@ -4624,10 +4792,10 @@
       <c r="F13" t="s">
         <v>715</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>714</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="8"/>
       <c r="I13" t="s">
         <v>713</v>
       </c>
@@ -4636,134 +4804,114 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="B19:C19"/>
@@ -4780,17 +4928,37 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" location="Czech" xr:uid="{5941DCB9-FDEB-4587-B027-375759EB9DA4}"/>
@@ -8913,10 +9081,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3081E238-0A75-4CCA-BCD2-D049DAB6C4FD}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9031,1151 +9199,1173 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>466</v>
+        <v>1325</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>465</v>
+        <v>1326</v>
       </c>
       <c r="D6" t="s">
-        <v>467</v>
+        <v>1329</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>468</v>
+        <v>1327</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1213</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1261</v>
+        <v>466</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>1262</v>
+        <v>465</v>
       </c>
       <c r="D7" t="s">
-        <v>1262</v>
+        <v>467</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1263</v>
+        <v>468</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1271</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>530</v>
+        <v>1261</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>531</v>
+        <v>1262</v>
       </c>
       <c r="D8" t="s">
-        <v>531</v>
+        <v>1262</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>532</v>
+        <v>1263</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1214</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>511</v>
+        <v>530</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>512</v>
+        <v>531</v>
       </c>
       <c r="D9" t="s">
-        <v>514</v>
+        <v>531</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>513</v>
+        <v>532</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>570</v>
+        <v>511</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>571</v>
+        <v>512</v>
       </c>
       <c r="D10" t="s">
-        <v>570</v>
+        <v>514</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>572</v>
+        <v>513</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>660</v>
+        <v>570</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C11" t="s">
-        <v>658</v>
+        <v>571</v>
       </c>
       <c r="D11" t="s">
-        <v>658</v>
+        <v>570</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>659</v>
+        <v>572</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>502</v>
+        <v>660</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>501</v>
+        <v>658</v>
       </c>
       <c r="D12" t="s">
-        <v>504</v>
+        <v>658</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>503</v>
+        <v>659</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>604</v>
+        <v>502</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>605</v>
+        <v>501</v>
       </c>
       <c r="D13" t="s">
-        <v>607</v>
+        <v>504</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>606</v>
+        <v>503</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1269</v>
+        <v>604</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>1268</v>
+        <v>605</v>
       </c>
       <c r="D14" t="s">
-        <v>1268</v>
+        <v>607</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1270</v>
+        <v>606</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1273</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>534</v>
+        <v>1269</v>
       </c>
       <c r="B15" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>533</v>
+        <v>1268</v>
       </c>
       <c r="D15" t="s">
-        <v>535</v>
+        <v>1268</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>536</v>
+        <v>1270</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1220</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>638</v>
+        <v>534</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="C16" t="s">
-        <v>639</v>
+        <v>533</v>
       </c>
       <c r="D16" t="s">
-        <v>639</v>
+        <v>535</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>637</v>
+        <v>536</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>810</v>
+        <v>638</v>
       </c>
       <c r="B17" t="s">
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>811</v>
+        <v>639</v>
       </c>
       <c r="D17" t="s">
-        <v>811</v>
+        <v>639</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>812</v>
+        <v>637</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>648</v>
+        <v>810</v>
       </c>
       <c r="B18" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>647</v>
+        <v>811</v>
       </c>
       <c r="D18" t="s">
-        <v>650</v>
+        <v>811</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>649</v>
+        <v>812</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="B19" t="s">
         <v>263</v>
       </c>
       <c r="C19" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="D19" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>636</v>
+        <v>643</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C20" t="s">
-        <v>596</v>
+        <v>645</v>
       </c>
       <c r="D20" t="s">
-        <v>599</v>
+        <v>646</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>598</v>
+        <v>644</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>620</v>
+        <v>636</v>
       </c>
       <c r="B21" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>621</v>
+        <v>596</v>
       </c>
       <c r="D21" t="s">
-        <v>622</v>
+        <v>599</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>623</v>
+        <v>598</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="B22" t="s">
         <v>263</v>
       </c>
       <c r="C22" t="s">
-        <v>633</v>
+        <v>621</v>
       </c>
       <c r="D22" t="s">
-        <v>635</v>
+        <v>622</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>634</v>
+        <v>623</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>505</v>
+        <v>632</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="C23" t="s">
-        <v>505</v>
+        <v>633</v>
       </c>
       <c r="D23" t="s">
-        <v>505</v>
+        <v>635</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>506</v>
+        <v>634</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>505</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>505</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
+        <v>505</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>56</v>
+        <v>506</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>489</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>490</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>492</v>
+        <v>92</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>491</v>
+        <v>56</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>574</v>
+        <v>489</v>
       </c>
       <c r="B26" t="s">
         <v>263</v>
       </c>
       <c r="C26" t="s">
-        <v>573</v>
+        <v>490</v>
       </c>
       <c r="D26" t="s">
-        <v>575</v>
+        <v>492</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>576</v>
+        <v>491</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>493</v>
+        <v>574</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C27" t="s">
-        <v>496</v>
+        <v>573</v>
       </c>
       <c r="D27" t="s">
-        <v>495</v>
+        <v>575</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>494</v>
+        <v>576</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1265</v>
+        <v>493</v>
       </c>
       <c r="B28" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>1264</v>
+        <v>496</v>
       </c>
       <c r="D28" t="s">
-        <v>1267</v>
+        <v>495</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>1266</v>
+        <v>494</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1272</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>631</v>
+        <v>1265</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="C29" t="s">
-        <v>628</v>
+        <v>1264</v>
       </c>
       <c r="D29" t="s">
-        <v>629</v>
+        <v>1267</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>630</v>
+        <v>1266</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1233</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>578</v>
+        <v>631</v>
       </c>
       <c r="B30" t="s">
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>579</v>
+        <v>628</v>
       </c>
       <c r="D30" t="s">
-        <v>581</v>
+        <v>629</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>580</v>
+        <v>630</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1145</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>473</v>
+        <v>578</v>
       </c>
       <c r="B31" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>474</v>
+        <v>579</v>
       </c>
       <c r="D31" t="s">
-        <v>476</v>
+        <v>581</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>475</v>
+        <v>580</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1234</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>640</v>
+        <v>473</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C32" t="s">
-        <v>641</v>
+        <v>474</v>
       </c>
       <c r="D32" t="s">
-        <v>641</v>
+        <v>476</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>642</v>
+        <v>475</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>541</v>
+        <v>640</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>542</v>
+        <v>641</v>
       </c>
       <c r="D33" t="s">
-        <v>542</v>
+        <v>641</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>543</v>
+        <v>642</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>613</v>
+        <v>541</v>
       </c>
       <c r="B34" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>615</v>
+        <v>542</v>
       </c>
       <c r="D34" t="s">
-        <v>614</v>
+        <v>542</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>612</v>
+        <v>543</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C35" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="D35" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>515</v>
+        <v>608</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>516</v>
+        <v>609</v>
       </c>
       <c r="D36" t="s">
-        <v>516</v>
+        <v>610</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>517</v>
+        <v>611</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>470</v>
+        <v>515</v>
       </c>
       <c r="B37" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>469</v>
+        <v>516</v>
       </c>
       <c r="D37" t="s">
-        <v>472</v>
+        <v>516</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>471</v>
+        <v>517</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>537</v>
+        <v>470</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C38" t="s">
-        <v>539</v>
+        <v>469</v>
       </c>
       <c r="D38" t="s">
-        <v>538</v>
+        <v>472</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>540</v>
+        <v>471</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>451</v>
+        <v>537</v>
       </c>
       <c r="B39" t="s">
         <v>25</v>
       </c>
       <c r="C39" t="s">
-        <v>450</v>
+        <v>539</v>
       </c>
       <c r="D39" t="s">
-        <v>452</v>
+        <v>538</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>453</v>
+        <v>540</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>519</v>
+        <v>451</v>
       </c>
       <c r="B40" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>518</v>
+        <v>450</v>
       </c>
       <c r="D40" t="s">
-        <v>520</v>
+        <v>452</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>521</v>
+        <v>453</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>586</v>
+        <v>519</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="C41" t="s">
-        <v>585</v>
+        <v>518</v>
       </c>
       <c r="D41" t="s">
-        <v>585</v>
+        <v>520</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>587</v>
+        <v>521</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>507</v>
+        <v>586</v>
       </c>
       <c r="B42" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>509</v>
+        <v>585</v>
       </c>
       <c r="D42" t="s">
-        <v>510</v>
+        <v>585</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>508</v>
+        <v>587</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>507</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>509</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>510</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>38</v>
+        <v>508</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1247</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>462</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>463</v>
+        <v>37</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>464</v>
+        <v>38</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>545</v>
+        <v>1247</v>
       </c>
       <c r="B45" t="s">
         <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>544</v>
+        <v>462</v>
       </c>
       <c r="D45" t="s">
-        <v>547</v>
+        <v>463</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>546</v>
+        <v>464</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>577</v>
+        <v>545</v>
       </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
-        <v>573</v>
+        <v>544</v>
       </c>
       <c r="D46" t="s">
-        <v>575</v>
+        <v>547</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>576</v>
+        <v>546</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>523</v>
+        <v>577</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C47" t="s">
-        <v>522</v>
+        <v>573</v>
       </c>
       <c r="D47" t="s">
-        <v>525</v>
+        <v>575</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>524</v>
+        <v>576</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>597</v>
+        <v>523</v>
       </c>
       <c r="B48" t="s">
         <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>596</v>
+        <v>522</v>
       </c>
       <c r="D48" t="s">
-        <v>599</v>
+        <v>525</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>598</v>
+        <v>524</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>588</v>
+        <v>597</v>
       </c>
       <c r="B49" t="s">
         <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>589</v>
+        <v>596</v>
       </c>
       <c r="D49" t="s">
-        <v>591</v>
+        <v>599</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>459</v>
+        <v>588</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>458</v>
+        <v>589</v>
       </c>
       <c r="D50" t="s">
-        <v>461</v>
+        <v>591</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>460</v>
+        <v>590</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>526</v>
+        <v>459</v>
       </c>
       <c r="B51" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C51" t="s">
-        <v>527</v>
+        <v>458</v>
       </c>
       <c r="D51" t="s">
-        <v>529</v>
+        <v>461</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>528</v>
+        <v>460</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>624</v>
+        <v>526</v>
       </c>
       <c r="B52" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C52" t="s">
-        <v>625</v>
+        <v>527</v>
       </c>
       <c r="D52" t="s">
-        <v>626</v>
+        <v>529</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>627</v>
+        <v>528</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>600</v>
+        <v>624</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C53" t="s">
-        <v>601</v>
+        <v>625</v>
       </c>
       <c r="D53" t="s">
-        <v>602</v>
+        <v>626</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>603</v>
+        <v>627</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>816</v>
+        <v>600</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
-        <v>813</v>
+        <v>601</v>
       </c>
       <c r="D54" t="s">
-        <v>815</v>
+        <v>602</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>814</v>
+        <v>603</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>617</v>
+        <v>816</v>
       </c>
       <c r="B55" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C55" t="s">
-        <v>616</v>
+        <v>813</v>
       </c>
       <c r="D55" t="s">
-        <v>619</v>
+        <v>815</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>618</v>
+        <v>814</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>617</v>
+      </c>
+      <c r="B56" t="s">
+        <v>263</v>
+      </c>
+      <c r="C56" t="s">
+        <v>616</v>
+      </c>
+      <c r="D56" t="s">
+        <v>619</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>655</v>
       </c>
-      <c r="B56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" t="s">
         <v>657</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>657</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>1260</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F56">
-    <sortCondition ref="A40:A56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F57">
+    <sortCondition ref="A1:A57"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" location="Czech" xr:uid="{A1D23F1B-FDA8-43C5-AAB6-C117CE1D1E54}"/>
-    <hyperlink ref="E39" r:id="rId2" location="Czech" xr:uid="{09F13A92-D8D4-4C33-86EB-F8EDCDA9E93B}"/>
+    <hyperlink ref="E40" r:id="rId2" location="Czech" xr:uid="{09F13A92-D8D4-4C33-86EB-F8EDCDA9E93B}"/>
     <hyperlink ref="E4" r:id="rId3" location="Czech" xr:uid="{BD4126AA-7C0B-4B16-B348-CECE2614A744}"/>
-    <hyperlink ref="E50" r:id="rId4" location="Czech" xr:uid="{826C4AE5-DC96-45AF-9AF1-89E8DEA24FF6}"/>
-    <hyperlink ref="E44" r:id="rId5" location="Czech" xr:uid="{E507F6E6-5BA7-46FE-9855-5A950753A897}"/>
-    <hyperlink ref="E6" r:id="rId6" location="Czech" xr:uid="{875D18B0-F469-4A76-AD52-119E27E36D5A}"/>
-    <hyperlink ref="E37" r:id="rId7" location="Czech" xr:uid="{915A7180-FAFB-4DDC-8CA3-4AA7316128C8}"/>
-    <hyperlink ref="E31" r:id="rId8" location="Czech" xr:uid="{005A1F8A-8182-4540-B3D4-A0C5D65C5FF3}"/>
-    <hyperlink ref="E25" r:id="rId9" location="Czech" xr:uid="{CA703896-AFE2-4E28-BF97-CCF4AE6545BB}"/>
-    <hyperlink ref="E27" r:id="rId10" location="Czech" xr:uid="{65E8F5C1-BE4A-450C-8239-1706127CA745}"/>
-    <hyperlink ref="E12" r:id="rId11" location="Czech" xr:uid="{E033C4DF-9D6B-487B-98CF-11706215CD89}"/>
-    <hyperlink ref="E23" r:id="rId12" location="Czech" xr:uid="{3919C6E2-259A-4926-A059-4A2FD34C36B0}"/>
-    <hyperlink ref="E42" r:id="rId13" location="Czech" xr:uid="{A56EE458-C3A2-4BB7-B928-FB984564837A}"/>
-    <hyperlink ref="E9" r:id="rId14" location="Czech" xr:uid="{A024442B-A7CF-4006-80C9-0A972DEC0D28}"/>
-    <hyperlink ref="E36" r:id="rId15" xr:uid="{874C2BD1-F639-48CB-9200-61871B21CCBD}"/>
-    <hyperlink ref="E40" r:id="rId16" location="Czech" xr:uid="{ABF0AD9D-20B4-4C19-9F19-DDE7755B82DA}"/>
-    <hyperlink ref="E47" r:id="rId17" location="Czech" xr:uid="{44EABECC-6856-45C3-80E9-D7275091641B}"/>
-    <hyperlink ref="E51" r:id="rId18" location="Czech" xr:uid="{846E6719-F2A7-4BAA-8A91-8EA0B3A5EA84}"/>
-    <hyperlink ref="E8" r:id="rId19" location="Czech" xr:uid="{0F18DABB-587E-4E71-944A-CA84F59592EC}"/>
-    <hyperlink ref="E15" r:id="rId20" location="Czech" xr:uid="{CAF54C10-3BF5-438C-8D62-FAF128C6831C}"/>
-    <hyperlink ref="E38" r:id="rId21" location="Czech" xr:uid="{68A1565A-0245-4FA2-9959-DAD43B747129}"/>
-    <hyperlink ref="E33" r:id="rId22" location="Czech" xr:uid="{4445173F-5165-4668-B186-F6FA1131C024}"/>
-    <hyperlink ref="E45" r:id="rId23" location="Czech" xr:uid="{5ED5ECCF-995D-438A-AE90-63D59F359E7C}"/>
-    <hyperlink ref="E10" r:id="rId24" location="Czech" xr:uid="{75FBDD0E-F09B-4054-8534-A14D95201648}"/>
-    <hyperlink ref="E26" r:id="rId25" location="Czech" xr:uid="{AE7ABCCD-0E4E-4B7C-90B9-A3694887AF1C}"/>
-    <hyperlink ref="E46" r:id="rId26" location="Czech" xr:uid="{DEE0A69F-5A79-427D-ADCE-2043CC497C8B}"/>
-    <hyperlink ref="E30" r:id="rId27" location="Czech" xr:uid="{8027C2E0-4B1B-4839-A04D-9C5889D6F471}"/>
+    <hyperlink ref="E51" r:id="rId4" location="Czech" xr:uid="{826C4AE5-DC96-45AF-9AF1-89E8DEA24FF6}"/>
+    <hyperlink ref="E45" r:id="rId5" location="Czech" xr:uid="{E507F6E6-5BA7-46FE-9855-5A950753A897}"/>
+    <hyperlink ref="E7" r:id="rId6" location="Czech" xr:uid="{875D18B0-F469-4A76-AD52-119E27E36D5A}"/>
+    <hyperlink ref="E38" r:id="rId7" location="Czech" xr:uid="{915A7180-FAFB-4DDC-8CA3-4AA7316128C8}"/>
+    <hyperlink ref="E32" r:id="rId8" location="Czech" xr:uid="{005A1F8A-8182-4540-B3D4-A0C5D65C5FF3}"/>
+    <hyperlink ref="E26" r:id="rId9" location="Czech" xr:uid="{CA703896-AFE2-4E28-BF97-CCF4AE6545BB}"/>
+    <hyperlink ref="E28" r:id="rId10" location="Czech" xr:uid="{65E8F5C1-BE4A-450C-8239-1706127CA745}"/>
+    <hyperlink ref="E13" r:id="rId11" location="Czech" xr:uid="{E033C4DF-9D6B-487B-98CF-11706215CD89}"/>
+    <hyperlink ref="E24" r:id="rId12" location="Czech" xr:uid="{3919C6E2-259A-4926-A059-4A2FD34C36B0}"/>
+    <hyperlink ref="E43" r:id="rId13" location="Czech" xr:uid="{A56EE458-C3A2-4BB7-B928-FB984564837A}"/>
+    <hyperlink ref="E10" r:id="rId14" location="Czech" xr:uid="{A024442B-A7CF-4006-80C9-0A972DEC0D28}"/>
+    <hyperlink ref="E37" r:id="rId15" xr:uid="{874C2BD1-F639-48CB-9200-61871B21CCBD}"/>
+    <hyperlink ref="E41" r:id="rId16" location="Czech" xr:uid="{ABF0AD9D-20B4-4C19-9F19-DDE7755B82DA}"/>
+    <hyperlink ref="E48" r:id="rId17" location="Czech" xr:uid="{44EABECC-6856-45C3-80E9-D7275091641B}"/>
+    <hyperlink ref="E52" r:id="rId18" location="Czech" xr:uid="{846E6719-F2A7-4BAA-8A91-8EA0B3A5EA84}"/>
+    <hyperlink ref="E9" r:id="rId19" location="Czech" xr:uid="{0F18DABB-587E-4E71-944A-CA84F59592EC}"/>
+    <hyperlink ref="E16" r:id="rId20" location="Czech" xr:uid="{CAF54C10-3BF5-438C-8D62-FAF128C6831C}"/>
+    <hyperlink ref="E39" r:id="rId21" location="Czech" xr:uid="{68A1565A-0245-4FA2-9959-DAD43B747129}"/>
+    <hyperlink ref="E34" r:id="rId22" location="Czech" xr:uid="{4445173F-5165-4668-B186-F6FA1131C024}"/>
+    <hyperlink ref="E46" r:id="rId23" location="Czech" xr:uid="{5ED5ECCF-995D-438A-AE90-63D59F359E7C}"/>
+    <hyperlink ref="E11" r:id="rId24" location="Czech" xr:uid="{75FBDD0E-F09B-4054-8534-A14D95201648}"/>
+    <hyperlink ref="E27" r:id="rId25" location="Czech" xr:uid="{AE7ABCCD-0E4E-4B7C-90B9-A3694887AF1C}"/>
+    <hyperlink ref="E47" r:id="rId26" location="Czech" xr:uid="{DEE0A69F-5A79-427D-ADCE-2043CC497C8B}"/>
+    <hyperlink ref="E31" r:id="rId27" location="Czech" xr:uid="{8027C2E0-4B1B-4839-A04D-9C5889D6F471}"/>
     <hyperlink ref="E5" r:id="rId28" xr:uid="{BA3EF3D6-AAAD-47B5-8B18-608AEEA711AF}"/>
-    <hyperlink ref="E41" r:id="rId29" location="Czech" xr:uid="{D74E85B4-CF38-4510-8321-CEF7AE65EDB1}"/>
-    <hyperlink ref="E49" r:id="rId30" location="Czech" xr:uid="{FA89C244-9977-446F-9F7B-F4C4A50A4B62}"/>
+    <hyperlink ref="E42" r:id="rId29" location="Czech" xr:uid="{D74E85B4-CF38-4510-8321-CEF7AE65EDB1}"/>
+    <hyperlink ref="E50" r:id="rId30" location="Czech" xr:uid="{FA89C244-9977-446F-9F7B-F4C4A50A4B62}"/>
     <hyperlink ref="E3" r:id="rId31" location="Czech" xr:uid="{A3117963-915E-426F-87F4-0ECCA8561421}"/>
-    <hyperlink ref="E48" r:id="rId32" location="Czech" xr:uid="{903AB6E7-665D-45FE-B41F-C5A4837850EA}"/>
-    <hyperlink ref="E53" r:id="rId33" location="Czech" xr:uid="{B1C096AF-1D81-4A2D-8D49-6CB376837167}"/>
-    <hyperlink ref="E13" r:id="rId34" location="Czech" xr:uid="{CCD3BD32-82A3-4BE1-A2E7-4FD101B85CCE}"/>
-    <hyperlink ref="E35" r:id="rId35" location="Czech" xr:uid="{49C8086D-E40C-4F7D-818D-D116E7FE9D4F}"/>
-    <hyperlink ref="E34" r:id="rId36" location="Czech" xr:uid="{61EA7DAF-217B-4B06-ABD0-FE715B249E77}"/>
-    <hyperlink ref="E55" r:id="rId37" location="Czech" xr:uid="{745C737C-07CA-4C51-8818-4C606487EABB}"/>
-    <hyperlink ref="E21" r:id="rId38" location="Czech" xr:uid="{571E29AD-F37C-4DDE-BEBB-DFCDF490BBA6}"/>
-    <hyperlink ref="E52" r:id="rId39" location="Czech" xr:uid="{DAD12AE5-5530-4133-8B92-9B6529F187C6}"/>
-    <hyperlink ref="E29" r:id="rId40" location="Czech" xr:uid="{52219598-D330-4A36-874F-B30B39DD3A6E}"/>
-    <hyperlink ref="E22" r:id="rId41" location="Czech" xr:uid="{1121D1DE-F079-4EA9-A097-EFAAAF79BC0E}"/>
-    <hyperlink ref="E20" r:id="rId42" location="Czech" xr:uid="{90676ACC-B807-4F74-BCD6-FA0C8D8DF2AA}"/>
-    <hyperlink ref="E16" r:id="rId43" location="Czech" xr:uid="{DEA496E0-0E8D-46F2-B276-65E0785BCFFF}"/>
-    <hyperlink ref="E32" r:id="rId44" location="Czech" xr:uid="{340D3731-0B3D-4728-9DB0-B6687A1B0A70}"/>
-    <hyperlink ref="E19" r:id="rId45" location="Czech" xr:uid="{B1F10C08-7D8A-4B00-85B3-177A2FD2BBBD}"/>
-    <hyperlink ref="E18" r:id="rId46" location="Czech" xr:uid="{AA795A16-C980-464F-AEF3-F664CD01B82E}"/>
-    <hyperlink ref="E56" r:id="rId47" location="Czech" xr:uid="{3F06F30A-9A25-4F35-93F4-27D72FD68DB8}"/>
-    <hyperlink ref="E11" r:id="rId48" location="Czech" xr:uid="{EE02CC40-0253-4A6A-AC33-5CE85C8CCEC6}"/>
-    <hyperlink ref="E43" r:id="rId49" location="Czech" xr:uid="{3D38AD09-C41A-4C80-A00B-4115BE4289ED}"/>
-    <hyperlink ref="E24" r:id="rId50" location="Czech" xr:uid="{5135D70C-EEFF-4AA4-B597-7BE4D31B8141}"/>
-    <hyperlink ref="E17" r:id="rId51" location="Czech" xr:uid="{12E41639-99E0-4A62-B45D-93D524D0703C}"/>
-    <hyperlink ref="E54" r:id="rId52" location="Czech" xr:uid="{27683485-CCF5-46C5-A2E8-663A9D73CA68}"/>
+    <hyperlink ref="E49" r:id="rId32" location="Czech" xr:uid="{903AB6E7-665D-45FE-B41F-C5A4837850EA}"/>
+    <hyperlink ref="E54" r:id="rId33" location="Czech" xr:uid="{B1C096AF-1D81-4A2D-8D49-6CB376837167}"/>
+    <hyperlink ref="E14" r:id="rId34" location="Czech" xr:uid="{CCD3BD32-82A3-4BE1-A2E7-4FD101B85CCE}"/>
+    <hyperlink ref="E36" r:id="rId35" location="Czech" xr:uid="{49C8086D-E40C-4F7D-818D-D116E7FE9D4F}"/>
+    <hyperlink ref="E35" r:id="rId36" location="Czech" xr:uid="{61EA7DAF-217B-4B06-ABD0-FE715B249E77}"/>
+    <hyperlink ref="E56" r:id="rId37" location="Czech" xr:uid="{745C737C-07CA-4C51-8818-4C606487EABB}"/>
+    <hyperlink ref="E22" r:id="rId38" location="Czech" xr:uid="{571E29AD-F37C-4DDE-BEBB-DFCDF490BBA6}"/>
+    <hyperlink ref="E53" r:id="rId39" location="Czech" xr:uid="{DAD12AE5-5530-4133-8B92-9B6529F187C6}"/>
+    <hyperlink ref="E30" r:id="rId40" location="Czech" xr:uid="{52219598-D330-4A36-874F-B30B39DD3A6E}"/>
+    <hyperlink ref="E23" r:id="rId41" location="Czech" xr:uid="{1121D1DE-F079-4EA9-A097-EFAAAF79BC0E}"/>
+    <hyperlink ref="E21" r:id="rId42" location="Czech" xr:uid="{90676ACC-B807-4F74-BCD6-FA0C8D8DF2AA}"/>
+    <hyperlink ref="E17" r:id="rId43" location="Czech" xr:uid="{DEA496E0-0E8D-46F2-B276-65E0785BCFFF}"/>
+    <hyperlink ref="E33" r:id="rId44" location="Czech" xr:uid="{340D3731-0B3D-4728-9DB0-B6687A1B0A70}"/>
+    <hyperlink ref="E20" r:id="rId45" location="Czech" xr:uid="{B1F10C08-7D8A-4B00-85B3-177A2FD2BBBD}"/>
+    <hyperlink ref="E19" r:id="rId46" location="Czech" xr:uid="{AA795A16-C980-464F-AEF3-F664CD01B82E}"/>
+    <hyperlink ref="E57" r:id="rId47" location="Czech" xr:uid="{3F06F30A-9A25-4F35-93F4-27D72FD68DB8}"/>
+    <hyperlink ref="E12" r:id="rId48" location="Czech" xr:uid="{EE02CC40-0253-4A6A-AC33-5CE85C8CCEC6}"/>
+    <hyperlink ref="E44" r:id="rId49" location="Czech" xr:uid="{3D38AD09-C41A-4C80-A00B-4115BE4289ED}"/>
+    <hyperlink ref="E25" r:id="rId50" location="Czech" xr:uid="{5135D70C-EEFF-4AA4-B597-7BE4D31B8141}"/>
+    <hyperlink ref="E18" r:id="rId51" location="Czech" xr:uid="{12E41639-99E0-4A62-B45D-93D524D0703C}"/>
+    <hyperlink ref="E55" r:id="rId52" location="Czech" xr:uid="{27683485-CCF5-46C5-A2E8-663A9D73CA68}"/>
     <hyperlink ref="F2" r:id="rId53" xr:uid="{E6D52F15-D79A-4B16-809F-7004DFBB63C8}"/>
     <hyperlink ref="F3" r:id="rId54" xr:uid="{30E09585-9F56-414D-920F-FC2C88D294FA}"/>
     <hyperlink ref="F4" r:id="rId55" xr:uid="{F008EE77-14EB-44F5-8F38-2A7B21A57769}"/>
     <hyperlink ref="F5" r:id="rId56" xr:uid="{BEE7EBD8-60B4-4955-BB19-7D5B68840431}"/>
-    <hyperlink ref="F6" r:id="rId57" xr:uid="{45D8E5B0-32D9-408A-B8E3-DB1A50D035AD}"/>
-    <hyperlink ref="F8" r:id="rId58" xr:uid="{B8177C16-A65E-4CC8-8112-681DD74666D9}"/>
-    <hyperlink ref="F9" r:id="rId59" xr:uid="{0FED9746-98FD-4A62-A35F-088F9C9830C4}"/>
-    <hyperlink ref="F10" r:id="rId60" xr:uid="{C7DA4B24-0C25-40B0-A442-5E36ECB86EEF}"/>
-    <hyperlink ref="F11" r:id="rId61" xr:uid="{D2AB1889-82B1-4C32-A916-BC3DE316496A}"/>
-    <hyperlink ref="F12" r:id="rId62" xr:uid="{74C2E99A-FE27-4AE5-97C3-9E98FEC69875}"/>
-    <hyperlink ref="F13" r:id="rId63" xr:uid="{752970C7-5AF0-4100-86A5-3DC0EBD54189}"/>
-    <hyperlink ref="F15" r:id="rId64" xr:uid="{12CA1679-CF67-4A5A-B6D5-150A2419C76C}"/>
-    <hyperlink ref="F16" r:id="rId65" xr:uid="{781DEFFC-083C-440C-A6DE-E6E10683798B}"/>
-    <hyperlink ref="F17" r:id="rId66" xr:uid="{1068ECEA-93F1-44C3-AA64-6A3BF7F38683}"/>
-    <hyperlink ref="F18" r:id="rId67" xr:uid="{49C54B5C-546F-4F15-823E-EEB0CE06B471}"/>
-    <hyperlink ref="F19" r:id="rId68" xr:uid="{FE4AB093-E1D4-4289-9CB2-0B7024DEDE22}"/>
-    <hyperlink ref="F20" r:id="rId69" xr:uid="{62E5A290-1326-4109-986F-8C39C8DA84B6}"/>
-    <hyperlink ref="F21" r:id="rId70" xr:uid="{0DF3A5CA-AE17-4435-8A40-C397B22C5C91}"/>
-    <hyperlink ref="F22" r:id="rId71" xr:uid="{D1475536-6C93-4FC0-9750-6A90992DEA45}"/>
-    <hyperlink ref="F23" r:id="rId72" xr:uid="{A9CC5FB2-8167-49C1-9C8E-2873B5346D41}"/>
-    <hyperlink ref="F24" r:id="rId73" xr:uid="{C306F08E-C969-4162-99A0-154D1103DBEE}"/>
-    <hyperlink ref="F25" r:id="rId74" xr:uid="{8C9ACC97-BE52-4915-8E33-2A980A49C005}"/>
-    <hyperlink ref="F26" r:id="rId75" xr:uid="{85FE31C2-A753-4CF7-B6C1-9B3B920C940D}"/>
-    <hyperlink ref="F27" r:id="rId76" xr:uid="{9C63CAA7-B2E5-4205-A4C0-837F71C58867}"/>
-    <hyperlink ref="F29" r:id="rId77" xr:uid="{B891269D-B892-41D2-AAE2-3A62F81413EF}"/>
-    <hyperlink ref="F30" r:id="rId78" xr:uid="{2956577E-6209-4C18-9638-CD84DDEA4F9E}"/>
-    <hyperlink ref="F31" r:id="rId79" xr:uid="{0724377C-FE8B-49A4-92B6-B9CB83ED0B00}"/>
-    <hyperlink ref="F32" r:id="rId80" xr:uid="{2E6201DB-2F6D-4BB6-8780-6723B3D6DA2B}"/>
-    <hyperlink ref="F33" r:id="rId81" xr:uid="{9899A66B-A27C-4A61-B303-84DB6BFD8A99}"/>
-    <hyperlink ref="F34" r:id="rId82" xr:uid="{A66E0D8A-935B-42D6-B70C-8DCE86FFE78A}"/>
-    <hyperlink ref="F35" r:id="rId83" xr:uid="{C8C6FDC7-1B9D-4E12-AB02-9CE90AAF88BD}"/>
-    <hyperlink ref="F36" r:id="rId84" xr:uid="{6ECFA8E9-9EC5-4A63-A8C1-44CB846F51CE}"/>
-    <hyperlink ref="F37" r:id="rId85" xr:uid="{C0D9C6AA-4041-4370-BD5F-7B1197B7E854}"/>
-    <hyperlink ref="F38" r:id="rId86" xr:uid="{2D9ACFFC-688C-4AB3-89A7-5EB151BA4EA2}"/>
-    <hyperlink ref="F39" r:id="rId87" xr:uid="{07E0BC01-BFC8-4A3E-9130-CEBBD76E42AE}"/>
-    <hyperlink ref="F40" r:id="rId88" xr:uid="{274258B3-76B1-461E-9C6A-40BD35A3A2FF}"/>
-    <hyperlink ref="F41" r:id="rId89" xr:uid="{4D4340B8-E8E0-4806-AA88-FEA49A01AF33}"/>
-    <hyperlink ref="F42" r:id="rId90" xr:uid="{B9D80B07-DAFC-4374-AB19-957C94291EA7}"/>
-    <hyperlink ref="F43" r:id="rId91" xr:uid="{22A6DF69-2B57-4DAC-8F8C-35C7E2170862}"/>
-    <hyperlink ref="F44" r:id="rId92" xr:uid="{CBFAFD4E-D5B5-4790-895E-2F85F12E41B5}"/>
-    <hyperlink ref="F45" r:id="rId93" xr:uid="{2E896B42-9841-4048-88D9-B090A55E29E0}"/>
-    <hyperlink ref="F46" r:id="rId94" xr:uid="{5236C4FF-BC15-4D99-A94A-E82667E1CABC}"/>
-    <hyperlink ref="F47" r:id="rId95" xr:uid="{C142DD7B-584A-4BAE-A9A2-C961B72728A0}"/>
-    <hyperlink ref="F48" r:id="rId96" xr:uid="{45AAF83F-B23C-4D25-952C-72BDF5B216B4}"/>
-    <hyperlink ref="F49" r:id="rId97" xr:uid="{17999536-F814-4FBA-81AB-468A5EEF7699}"/>
-    <hyperlink ref="F50" r:id="rId98" xr:uid="{606F78CD-057C-4CE5-951A-90332C5D8773}"/>
-    <hyperlink ref="F51" r:id="rId99" xr:uid="{DA367059-8E02-466B-B51D-B60835BB8524}"/>
-    <hyperlink ref="F52" r:id="rId100" xr:uid="{296FB6F7-F2CE-495E-8D69-A6C1AA4226CD}"/>
-    <hyperlink ref="F53" r:id="rId101" xr:uid="{8AB9E978-49B3-47EF-B841-340B0387DC33}"/>
-    <hyperlink ref="F54" r:id="rId102" xr:uid="{877DC3BE-DFBC-4867-BF92-6C6D190CC216}"/>
-    <hyperlink ref="F55" r:id="rId103" xr:uid="{B28A879D-6345-489C-BF70-E315342E86C1}"/>
-    <hyperlink ref="F56" r:id="rId104" xr:uid="{5F823D1E-E878-4ED9-826E-E6C7D7E96D4F}"/>
-    <hyperlink ref="E7" r:id="rId105" location="Czech" xr:uid="{1BE34E5D-A81F-46D5-9524-51E6C408FE8A}"/>
-    <hyperlink ref="E28" r:id="rId106" location="Czech" xr:uid="{C70889B9-2692-4A79-B51E-516A65017932}"/>
-    <hyperlink ref="E14" r:id="rId107" location="Czech" xr:uid="{1D58C86D-3D46-404A-8900-2AF505BF92D4}"/>
-    <hyperlink ref="F7" r:id="rId108" xr:uid="{D1B0E7F4-2372-4687-B33D-BCF7B365CE13}"/>
-    <hyperlink ref="F28" r:id="rId109" xr:uid="{E37AC33E-99BD-4AAA-A874-FB4DFB9A5032}"/>
-    <hyperlink ref="F14" r:id="rId110" xr:uid="{2EE222BD-D194-45EC-96F1-5356CA36052A}"/>
+    <hyperlink ref="F7" r:id="rId57" xr:uid="{45D8E5B0-32D9-408A-B8E3-DB1A50D035AD}"/>
+    <hyperlink ref="F9" r:id="rId58" xr:uid="{B8177C16-A65E-4CC8-8112-681DD74666D9}"/>
+    <hyperlink ref="F10" r:id="rId59" xr:uid="{0FED9746-98FD-4A62-A35F-088F9C9830C4}"/>
+    <hyperlink ref="F11" r:id="rId60" xr:uid="{C7DA4B24-0C25-40B0-A442-5E36ECB86EEF}"/>
+    <hyperlink ref="F12" r:id="rId61" xr:uid="{D2AB1889-82B1-4C32-A916-BC3DE316496A}"/>
+    <hyperlink ref="F13" r:id="rId62" xr:uid="{74C2E99A-FE27-4AE5-97C3-9E98FEC69875}"/>
+    <hyperlink ref="F14" r:id="rId63" xr:uid="{752970C7-5AF0-4100-86A5-3DC0EBD54189}"/>
+    <hyperlink ref="F16" r:id="rId64" xr:uid="{12CA1679-CF67-4A5A-B6D5-150A2419C76C}"/>
+    <hyperlink ref="F17" r:id="rId65" xr:uid="{781DEFFC-083C-440C-A6DE-E6E10683798B}"/>
+    <hyperlink ref="F18" r:id="rId66" xr:uid="{1068ECEA-93F1-44C3-AA64-6A3BF7F38683}"/>
+    <hyperlink ref="F19" r:id="rId67" xr:uid="{49C54B5C-546F-4F15-823E-EEB0CE06B471}"/>
+    <hyperlink ref="F20" r:id="rId68" xr:uid="{FE4AB093-E1D4-4289-9CB2-0B7024DEDE22}"/>
+    <hyperlink ref="F21" r:id="rId69" xr:uid="{62E5A290-1326-4109-986F-8C39C8DA84B6}"/>
+    <hyperlink ref="F22" r:id="rId70" xr:uid="{0DF3A5CA-AE17-4435-8A40-C397B22C5C91}"/>
+    <hyperlink ref="F23" r:id="rId71" xr:uid="{D1475536-6C93-4FC0-9750-6A90992DEA45}"/>
+    <hyperlink ref="F24" r:id="rId72" xr:uid="{A9CC5FB2-8167-49C1-9C8E-2873B5346D41}"/>
+    <hyperlink ref="F25" r:id="rId73" xr:uid="{C306F08E-C969-4162-99A0-154D1103DBEE}"/>
+    <hyperlink ref="F26" r:id="rId74" xr:uid="{8C9ACC97-BE52-4915-8E33-2A980A49C005}"/>
+    <hyperlink ref="F27" r:id="rId75" xr:uid="{85FE31C2-A753-4CF7-B6C1-9B3B920C940D}"/>
+    <hyperlink ref="F28" r:id="rId76" xr:uid="{9C63CAA7-B2E5-4205-A4C0-837F71C58867}"/>
+    <hyperlink ref="F30" r:id="rId77" xr:uid="{B891269D-B892-41D2-AAE2-3A62F81413EF}"/>
+    <hyperlink ref="F31" r:id="rId78" xr:uid="{2956577E-6209-4C18-9638-CD84DDEA4F9E}"/>
+    <hyperlink ref="F32" r:id="rId79" xr:uid="{0724377C-FE8B-49A4-92B6-B9CB83ED0B00}"/>
+    <hyperlink ref="F33" r:id="rId80" xr:uid="{2E6201DB-2F6D-4BB6-8780-6723B3D6DA2B}"/>
+    <hyperlink ref="F34" r:id="rId81" xr:uid="{9899A66B-A27C-4A61-B303-84DB6BFD8A99}"/>
+    <hyperlink ref="F35" r:id="rId82" xr:uid="{A66E0D8A-935B-42D6-B70C-8DCE86FFE78A}"/>
+    <hyperlink ref="F36" r:id="rId83" xr:uid="{C8C6FDC7-1B9D-4E12-AB02-9CE90AAF88BD}"/>
+    <hyperlink ref="F37" r:id="rId84" xr:uid="{6ECFA8E9-9EC5-4A63-A8C1-44CB846F51CE}"/>
+    <hyperlink ref="F38" r:id="rId85" xr:uid="{C0D9C6AA-4041-4370-BD5F-7B1197B7E854}"/>
+    <hyperlink ref="F39" r:id="rId86" xr:uid="{2D9ACFFC-688C-4AB3-89A7-5EB151BA4EA2}"/>
+    <hyperlink ref="F40" r:id="rId87" xr:uid="{07E0BC01-BFC8-4A3E-9130-CEBBD76E42AE}"/>
+    <hyperlink ref="F41" r:id="rId88" xr:uid="{274258B3-76B1-461E-9C6A-40BD35A3A2FF}"/>
+    <hyperlink ref="F42" r:id="rId89" xr:uid="{4D4340B8-E8E0-4806-AA88-FEA49A01AF33}"/>
+    <hyperlink ref="F43" r:id="rId90" xr:uid="{B9D80B07-DAFC-4374-AB19-957C94291EA7}"/>
+    <hyperlink ref="F44" r:id="rId91" xr:uid="{22A6DF69-2B57-4DAC-8F8C-35C7E2170862}"/>
+    <hyperlink ref="F45" r:id="rId92" xr:uid="{CBFAFD4E-D5B5-4790-895E-2F85F12E41B5}"/>
+    <hyperlink ref="F46" r:id="rId93" xr:uid="{2E896B42-9841-4048-88D9-B090A55E29E0}"/>
+    <hyperlink ref="F47" r:id="rId94" xr:uid="{5236C4FF-BC15-4D99-A94A-E82667E1CABC}"/>
+    <hyperlink ref="F48" r:id="rId95" xr:uid="{C142DD7B-584A-4BAE-A9A2-C961B72728A0}"/>
+    <hyperlink ref="F49" r:id="rId96" xr:uid="{45AAF83F-B23C-4D25-952C-72BDF5B216B4}"/>
+    <hyperlink ref="F50" r:id="rId97" xr:uid="{17999536-F814-4FBA-81AB-468A5EEF7699}"/>
+    <hyperlink ref="F51" r:id="rId98" xr:uid="{606F78CD-057C-4CE5-951A-90332C5D8773}"/>
+    <hyperlink ref="F52" r:id="rId99" xr:uid="{DA367059-8E02-466B-B51D-B60835BB8524}"/>
+    <hyperlink ref="F53" r:id="rId100" xr:uid="{296FB6F7-F2CE-495E-8D69-A6C1AA4226CD}"/>
+    <hyperlink ref="F54" r:id="rId101" xr:uid="{8AB9E978-49B3-47EF-B841-340B0387DC33}"/>
+    <hyperlink ref="F55" r:id="rId102" xr:uid="{877DC3BE-DFBC-4867-BF92-6C6D190CC216}"/>
+    <hyperlink ref="F56" r:id="rId103" xr:uid="{B28A879D-6345-489C-BF70-E315342E86C1}"/>
+    <hyperlink ref="F57" r:id="rId104" xr:uid="{5F823D1E-E878-4ED9-826E-E6C7D7E96D4F}"/>
+    <hyperlink ref="E8" r:id="rId105" location="Czech" xr:uid="{1BE34E5D-A81F-46D5-9524-51E6C408FE8A}"/>
+    <hyperlink ref="E29" r:id="rId106" location="Czech" xr:uid="{C70889B9-2692-4A79-B51E-516A65017932}"/>
+    <hyperlink ref="E15" r:id="rId107" location="Czech" xr:uid="{1D58C86D-3D46-404A-8900-2AF505BF92D4}"/>
+    <hyperlink ref="F8" r:id="rId108" xr:uid="{D1B0E7F4-2372-4687-B33D-BCF7B365CE13}"/>
+    <hyperlink ref="F29" r:id="rId109" xr:uid="{E37AC33E-99BD-4AAA-A874-FB4DFB9A5032}"/>
+    <hyperlink ref="F15" r:id="rId110" xr:uid="{2EE222BD-D194-45EC-96F1-5356CA36052A}"/>
+    <hyperlink ref="E6" r:id="rId111" location="Czech" xr:uid="{BCCE51DB-47B5-4B88-A747-0B58F7B5FCDE}"/>
+    <hyperlink ref="F6" r:id="rId112" xr:uid="{227F0F93-5B7E-4B17-8751-DD961084A7AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId111"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId113"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCD7ADF-A934-4B8C-90F5-000C68281CBC}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10185,9 +10375,10 @@
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -10203,8 +10394,11 @@
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>903</v>
       </c>
@@ -10220,8 +10414,11 @@
       <c r="E2" s="1" t="s">
         <v>904</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>905</v>
       </c>
@@ -10237,8 +10434,11 @@
       <c r="E3" s="1" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>738</v>
       </c>
@@ -10254,8 +10454,11 @@
       <c r="E4" s="1" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>756</v>
       </c>
@@ -10271,8 +10474,11 @@
       <c r="E5" s="1" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>741</v>
       </c>
@@ -10288,8 +10494,11 @@
       <c r="E6" s="1" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>859</v>
       </c>
@@ -10305,8 +10514,11 @@
       <c r="E7" s="1" t="s">
         <v>860</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>913</v>
       </c>
@@ -10322,8 +10534,11 @@
       <c r="E8" s="1" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>817</v>
       </c>
@@ -10339,8 +10554,11 @@
       <c r="E9" s="1" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>829</v>
       </c>
@@ -10356,8 +10574,11 @@
       <c r="E10" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>807</v>
       </c>
@@ -10373,8 +10594,11 @@
       <c r="E11" s="1" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>900</v>
       </c>
@@ -10390,8 +10614,11 @@
       <c r="E12" s="1" t="s">
         <v>899</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>883</v>
       </c>
@@ -10407,8 +10634,11 @@
       <c r="E13" s="1" t="s">
         <v>885</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>872</v>
       </c>
@@ -10424,8 +10654,11 @@
       <c r="E14" s="1" t="s">
         <v>873</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>766</v>
       </c>
@@ -10441,8 +10674,11 @@
       <c r="E15" s="1" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>850</v>
       </c>
@@ -10458,8 +10694,11 @@
       <c r="E16" s="1" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>803</v>
       </c>
@@ -10475,8 +10714,11 @@
       <c r="E17" s="1" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>866</v>
       </c>
@@ -10492,8 +10734,11 @@
       <c r="E18" s="1" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1100</v>
       </c>
@@ -10509,8 +10754,11 @@
       <c r="E19" s="1" t="s">
         <v>1101</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>750</v>
       </c>
@@ -10526,8 +10774,11 @@
       <c r="E20" s="1" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>792</v>
       </c>
@@ -10543,8 +10794,11 @@
       <c r="E21" s="1" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>841</v>
       </c>
@@ -10560,8 +10814,11 @@
       <c r="E22" s="1" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>835</v>
       </c>
@@ -10577,8 +10834,11 @@
       <c r="E23" s="1" t="s">
         <v>836</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>780</v>
       </c>
@@ -10594,8 +10854,11 @@
       <c r="E24" s="1" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>799</v>
       </c>
@@ -10611,8 +10874,11 @@
       <c r="E25" s="1" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>731</v>
       </c>
@@ -10628,8 +10894,11 @@
       <c r="E26" s="1" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="1" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>261</v>
       </c>
@@ -10645,8 +10914,11 @@
       <c r="E27" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="1" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>909</v>
       </c>
@@ -10662,8 +10934,11 @@
       <c r="E28" s="1" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="1" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>734</v>
       </c>
@@ -10679,8 +10954,11 @@
       <c r="E29" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" s="1" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>788</v>
       </c>
@@ -10696,8 +10974,11 @@
       <c r="E30" s="1" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" s="1" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>856</v>
       </c>
@@ -10713,8 +10994,11 @@
       <c r="E31" s="1" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="1" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>831</v>
       </c>
@@ -10730,8 +11014,11 @@
       <c r="E32" s="1" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="1" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>847</v>
       </c>
@@ -10747,8 +11034,11 @@
       <c r="E33" s="1" t="s">
         <v>848</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="1" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>825</v>
       </c>
@@ -10764,8 +11054,11 @@
       <c r="E34" s="1" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="1" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>862</v>
       </c>
@@ -10781,8 +11074,11 @@
       <c r="E35" s="1" t="s">
         <v>865</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" s="1" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>784</v>
       </c>
@@ -10798,8 +11094,11 @@
       <c r="E36" s="1" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" s="1" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>843</v>
       </c>
@@ -10815,8 +11114,11 @@
       <c r="E37" s="1" t="s">
         <v>844</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" s="1" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>870</v>
       </c>
@@ -10832,8 +11134,11 @@
       <c r="E38" s="1" t="s">
         <v>867</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" s="1" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>888</v>
       </c>
@@ -10849,8 +11154,11 @@
       <c r="E39" s="1" t="s">
         <v>889</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" s="1" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>746</v>
       </c>
@@ -10866,8 +11174,11 @@
       <c r="E40" s="1" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" s="1" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>772</v>
       </c>
@@ -10883,8 +11194,11 @@
       <c r="E41" s="1" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" s="1" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>893</v>
       </c>
@@ -10900,8 +11214,11 @@
       <c r="E42" s="1" t="s">
         <v>892</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" s="1" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>761</v>
       </c>
@@ -10917,8 +11234,11 @@
       <c r="E43" s="1" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" s="1" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>795</v>
       </c>
@@ -10934,8 +11254,11 @@
       <c r="E44" s="1" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" s="1" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>744</v>
       </c>
@@ -10951,8 +11274,11 @@
       <c r="E45" s="1" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" s="1" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>776</v>
       </c>
@@ -10968,8 +11294,11 @@
       <c r="E46" s="1" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" s="1" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>755</v>
       </c>
@@ -10985,8 +11314,11 @@
       <c r="E47" s="1" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" s="1" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>767</v>
       </c>
@@ -11002,8 +11334,11 @@
       <c r="E48" s="1" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" s="1" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>875</v>
       </c>
@@ -11019,8 +11354,11 @@
       <c r="E49" s="1" t="s">
         <v>876</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" s="1" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>895</v>
       </c>
@@ -11036,8 +11374,11 @@
       <c r="E50" s="1" t="s">
         <v>898</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" s="1" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>879</v>
       </c>
@@ -11053,8 +11394,11 @@
       <c r="E51" s="1" t="s">
         <v>882</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>822</v>
       </c>
@@ -11069,6 +11413,9 @@
       </c>
       <c r="E52" s="1" t="s">
         <v>823</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>1324</v>
       </c>
     </row>
   </sheetData>
@@ -11127,9 +11474,60 @@
     <hyperlink ref="E28" r:id="rId49" location="Czech" xr:uid="{D4152F8D-8835-4CDB-98F1-C09C729A36DE}"/>
     <hyperlink ref="E8" r:id="rId50" location="Czech" xr:uid="{91C31CEF-ED20-40A5-A4BF-8EAF8CEB0CB0}"/>
     <hyperlink ref="E19" r:id="rId51" location="Czech" xr:uid="{24B8314C-7FAE-42FF-B32D-DAC3650E5711}"/>
+    <hyperlink ref="F2" r:id="rId52" xr:uid="{7349BF2A-1CF9-4FF7-8640-A10ECC7F16B0}"/>
+    <hyperlink ref="F3" r:id="rId53" xr:uid="{A228D250-AC84-40A7-BCE4-9A9427BE1DE8}"/>
+    <hyperlink ref="F4" r:id="rId54" xr:uid="{39DACC5D-8CFB-4B06-8F42-130804F1C6B0}"/>
+    <hyperlink ref="F5" r:id="rId55" xr:uid="{3778AED1-01A4-4DF1-92A0-818D6CBFE66E}"/>
+    <hyperlink ref="F6" r:id="rId56" xr:uid="{FFB83AA4-0ED2-4B69-9D54-EAB22AE1BC17}"/>
+    <hyperlink ref="F7" r:id="rId57" xr:uid="{FF522957-2B5A-4672-9272-88F2AFC292F6}"/>
+    <hyperlink ref="F8" r:id="rId58" xr:uid="{EA8A73DF-686C-4121-B3E5-6C2C008C274B}"/>
+    <hyperlink ref="F9" r:id="rId59" xr:uid="{D17659BC-057F-4231-98AB-4613DE50139F}"/>
+    <hyperlink ref="F10" r:id="rId60" xr:uid="{4AF0E5D0-668A-4E53-A5B7-82CA9B7D5BC7}"/>
+    <hyperlink ref="F11" r:id="rId61" xr:uid="{DB1D716D-B733-44F6-9D35-00BE0A79DEF3}"/>
+    <hyperlink ref="F12" r:id="rId62" xr:uid="{3C3B54B6-3EDD-434F-B389-64FDC3EA1114}"/>
+    <hyperlink ref="F13" r:id="rId63" xr:uid="{E1C3A8AE-7DCB-434E-9A5C-089718B0AEB1}"/>
+    <hyperlink ref="F14" r:id="rId64" xr:uid="{50DEA5C8-F208-410C-8CB0-123632AF6BC2}"/>
+    <hyperlink ref="F15" r:id="rId65" xr:uid="{550426CA-719B-45B2-88C4-1487B1CA4020}"/>
+    <hyperlink ref="F16" r:id="rId66" xr:uid="{94C81662-9F67-4D7A-87AF-7ADF5AA7461B}"/>
+    <hyperlink ref="F17" r:id="rId67" xr:uid="{F0A11E35-3665-4E8F-B426-5EC2C938B0D1}"/>
+    <hyperlink ref="F18" r:id="rId68" xr:uid="{DF5891BE-136F-4B94-8ACA-CE06A2C21F7E}"/>
+    <hyperlink ref="F19" r:id="rId69" xr:uid="{A3C374D8-9359-4072-9CE2-F1414CA109DC}"/>
+    <hyperlink ref="F20" r:id="rId70" xr:uid="{8359BD25-F9A7-47CC-BE7F-E89B59F4E93B}"/>
+    <hyperlink ref="F21" r:id="rId71" xr:uid="{6C0201F9-712F-4713-8762-6115989E9D13}"/>
+    <hyperlink ref="F22" r:id="rId72" xr:uid="{4BF0A2FD-F6B7-48BB-A460-C7DC46CFC1C5}"/>
+    <hyperlink ref="F23" r:id="rId73" xr:uid="{7FD8380E-8438-4D86-9D2E-CD53171EBFE8}"/>
+    <hyperlink ref="F24" r:id="rId74" xr:uid="{7B87A74E-466D-439B-A756-7856E1BAAA88}"/>
+    <hyperlink ref="F25" r:id="rId75" xr:uid="{029D39CC-C1F2-4676-925B-7AD757C113AA}"/>
+    <hyperlink ref="F26" r:id="rId76" xr:uid="{B470E4C6-2592-462A-83F5-7D2A21C010A6}"/>
+    <hyperlink ref="F27" r:id="rId77" xr:uid="{7FD5E37D-33EC-4F4D-85D1-73D01754D068}"/>
+    <hyperlink ref="F28" r:id="rId78" xr:uid="{DFF521E5-6715-4C29-B30D-FD07F9852A0E}"/>
+    <hyperlink ref="F29" r:id="rId79" xr:uid="{6BAA2C7E-CFD3-4573-89CC-C44FD3246C80}"/>
+    <hyperlink ref="F30" r:id="rId80" xr:uid="{07B2DBF1-06BA-40D7-89FB-E174922671C2}"/>
+    <hyperlink ref="F31" r:id="rId81" xr:uid="{B7DC757A-BD71-48A1-B5CC-34BB0CDCCFF2}"/>
+    <hyperlink ref="F32" r:id="rId82" xr:uid="{74B6CD93-93DD-450B-BA99-CB541EBD2E7A}"/>
+    <hyperlink ref="F33" r:id="rId83" xr:uid="{4983453D-9F5D-45CB-8E8E-28DF2E8D9B56}"/>
+    <hyperlink ref="F34" r:id="rId84" xr:uid="{CB410BC5-2FB2-4C84-9E77-417F992B8CB2}"/>
+    <hyperlink ref="F35" r:id="rId85" xr:uid="{9DF6E28D-D72F-40A8-9FF3-680188943407}"/>
+    <hyperlink ref="F36" r:id="rId86" xr:uid="{71B6C3AF-B08D-441C-8F51-C57879F811B9}"/>
+    <hyperlink ref="F37" r:id="rId87" xr:uid="{B3B3FE99-020D-4B39-986C-E67308C59942}"/>
+    <hyperlink ref="F38" r:id="rId88" xr:uid="{BE62AF36-7AA6-4406-AFF8-9F3115F21F55}"/>
+    <hyperlink ref="F39" r:id="rId89" xr:uid="{F25BE1B9-1510-441A-AAFA-DF6891FF8B05}"/>
+    <hyperlink ref="F40" r:id="rId90" xr:uid="{11F96174-8B3C-4613-85E9-350625C89D71}"/>
+    <hyperlink ref="F41" r:id="rId91" xr:uid="{C7F3DFE2-6162-40CE-B017-111E00CFAD88}"/>
+    <hyperlink ref="F42" r:id="rId92" xr:uid="{B26C47F5-95B0-4CC6-B7C5-0FE5DE9F1D48}"/>
+    <hyperlink ref="F43" r:id="rId93" xr:uid="{E7E699D9-2D8A-4D90-95AE-279E34EA3635}"/>
+    <hyperlink ref="F44" r:id="rId94" xr:uid="{EA0D98A0-8359-4E91-B63A-C1C396B4852D}"/>
+    <hyperlink ref="F45" r:id="rId95" xr:uid="{34320072-4E10-45E9-8D5D-BF9565901E63}"/>
+    <hyperlink ref="F46" r:id="rId96" xr:uid="{71EEB8E7-415C-491D-ACDA-28BD6EC8DAB9}"/>
+    <hyperlink ref="F47" r:id="rId97" xr:uid="{F981C0FD-B38B-4960-8DBB-EC5EA32CA8E4}"/>
+    <hyperlink ref="F48" r:id="rId98" xr:uid="{CC47B797-0670-4FF9-AD9A-4358EB33B930}"/>
+    <hyperlink ref="F49" r:id="rId99" xr:uid="{F7B96616-D53A-4F58-B521-274BFA3DE2D4}"/>
+    <hyperlink ref="F50" r:id="rId100" xr:uid="{C5E1A3DC-4A02-46E5-B64F-3CBD1622553F}"/>
+    <hyperlink ref="F51" r:id="rId101" xr:uid="{1B3B5741-7720-4623-B744-D0AB9868A3BE}"/>
+    <hyperlink ref="F52" r:id="rId102" xr:uid="{BCB4D44C-B26F-4521-A900-DE2BFF96C039}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId52"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId103"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added image urls for Hobbies. People, Numbers and School
</commit_message>
<xml_diff>
--- a/data/vocab.xlsx
+++ b/data/vocab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\Czech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B40B9E4-CD89-4B32-8DEB-A135DC0047E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8D4F06-06BD-4A29-9D4B-6870CCB5EEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="10" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
   </bookViews>
   <sheets>
     <sheet name="Adjectives" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="1413">
   <si>
     <t>English</t>
   </si>
@@ -4040,6 +4040,255 @@
   </si>
   <si>
     <t>ostružiny</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/cc00/art_supplies_art_school.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/479e/art_therapy_therapeutic_discipline.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/30e7/concert_crowd_concert_crowd.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/0328/dance_stage_music_entertainment.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/4645/guitar_acoustic_guitar_1502742.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/0c97/photographer_photography_hobby_1240061.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3254/keyboard_piano_keys_music.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/f900/music_sheet_music_piano.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b971/party_hard_rock_cafe.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/7f61/fishing_in_mist_from.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/72f2/piano_piano_keys_wood.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/92ce/saxophone_player_music_performer.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1bd9/aunt_nephew_love_child.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/745d/boys_with_airgun_bird_3.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/e371/boyfriends_love_casal_kiss.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/77eb/brothers_children_boys_young.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/53f4/girls_buddy_friendship_beauty_2.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/da9b/child_holding_fish_on.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/cd63/little_girl_blonde_baby.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/8018/cousins_play_boy_girl.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/9fc7/daughter_with_her_father.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/cb4f/family_walk_in_wildness.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/6d58/fathers_day_father_with.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1644/friends_happy_fun_happy.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/39ff/girl_smiling_girl_girl.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/ba95/hugging_couple_covered_bridge.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/display/father_son_family_boy.html</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3901/mother_son_family_child.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/03b4/grandfather_advice_family_784512.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/27f6/grandmother_old_woman_child.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/359e/human_crowds_collection_people.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a63a/husbands_couples_man_women.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/98ce/baby_infant_girl_juliana.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/29ec/man_stylish_wall_brick.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/36e3/mother_son_maternity_canal.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/9825/wedding_family_fun_love.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/5c7a/girl_child_adorable_people.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/bd00/bike_partners_zoo_people.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/7874/person_top_mountian_view.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a37c/brothers_sisters_sisters_419429.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/aafc/father_son_islam_muslim.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/08c1/father_daughter_enjoy_magic.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/9daa/couple_husbend_wife_old.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/fad8/woman_working_business_woman.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a4c1/zero_electronic_digit_black.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/0e48/house_number_one_number.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/c181/number_two_paint_painting.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/fa5a/number_three_three_wood.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/29cd/four_number_four_civic.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/8c59/birthday_number_five_5.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/a48e/six_number_house_number.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/695d/seven_sign.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/765a/number_digit_eight_8.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/90b7/number_ad_yellow_color_4.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/319c/ten_number_figure_plate.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/db86/number_20_twenty_wall.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/50e5/number_thirty_number_street.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d2a8/number_50_fifty_wooden.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/67d5/sixty_number_sixty_civic.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d370/wood_orange_eighty_beach.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/0a41/route_ninety.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/ab50/student_biology_notes_think.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/088b/chair_butterfly_chair_sit.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d060/chemistry_scientific_chemical_421065.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/67c8/class_discussion_girls_study.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/0846/desk_chair_school_study.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/fb42/flag_english_english_flag.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/aaf8/test_testing_exam_sat.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/724c/geography_globe_blue_coloring.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/63c1/german_flag_germany_german.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/214d/history_city_street_arcade.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/652a/flag_irish_right_t.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/717f/fireman_talks_with_two.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/00f4/math_number_school_symbol.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/e102/music_nuts_music_notes_0.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/bb46/formula_mathematics_physics_594149.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3065/religion_christianity_islam_cross.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/d227/school_class_school_children.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/8d4d/science_chemistry_technology_736422.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/7f48/students_education_school_studying.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1032/kitchen_table_chairs_colorful.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1a89/teacher_female_education_woman.jpg</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/6c36/university_university_vermont_418973.jpg</t>
   </si>
 </sst>
 </file>
@@ -4092,7 +4341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4112,6 +4361,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4980,10 +5231,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72495061-B325-404B-BD6E-056CDCE7E104}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4993,9 +5244,10 @@
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5011,8 +5263,11 @@
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>211</v>
       </c>
@@ -5028,8 +5283,11 @@
       <c r="E2" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -5045,8 +5303,11 @@
       <c r="E3" s="1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -5062,8 +5323,11 @@
       <c r="E4" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -5079,8 +5343,11 @@
       <c r="E5" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>137</v>
       </c>
@@ -5096,8 +5363,11 @@
       <c r="E6" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -5113,8 +5383,11 @@
       <c r="E7" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -5130,8 +5403,11 @@
       <c r="E8" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>204</v>
       </c>
@@ -5147,8 +5423,11 @@
       <c r="E9" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>184</v>
       </c>
@@ -5164,8 +5443,11 @@
       <c r="E10" s="1" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -5181,8 +5463,11 @@
       <c r="E11" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>177</v>
       </c>
@@ -5198,8 +5483,11 @@
       <c r="E12" s="1" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>133</v>
       </c>
@@ -5215,8 +5503,11 @@
       <c r="E13" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>200</v>
       </c>
@@ -5232,8 +5523,11 @@
       <c r="E14" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -5249,8 +5543,11 @@
       <c r="E15" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>239</v>
       </c>
@@ -5266,8 +5563,11 @@
       <c r="E16" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -5283,8 +5583,11 @@
       <c r="E17" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>193</v>
       </c>
@@ -5300,8 +5603,11 @@
       <c r="E18" s="1" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -5317,8 +5623,11 @@
       <c r="E19" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>219</v>
       </c>
@@ -5334,8 +5643,11 @@
       <c r="E20" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>164</v>
       </c>
@@ -5351,8 +5663,11 @@
       <c r="E21" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -5368,8 +5683,11 @@
       <c r="E22" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -5385,8 +5703,11 @@
       <c r="E23" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -5402,8 +5723,11 @@
       <c r="E24" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>227</v>
       </c>
@@ -5419,8 +5743,11 @@
       <c r="E25" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>230</v>
       </c>
@@ -5436,8 +5763,11 @@
       <c r="E26" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="1" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>224</v>
       </c>
@@ -5453,8 +5783,11 @@
       <c r="E27" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="1" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>152</v>
       </c>
@@ -5470,8 +5803,11 @@
       <c r="E28" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="1" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>246</v>
       </c>
@@ -5487,8 +5823,11 @@
       <c r="E29" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" s="1" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>181</v>
       </c>
@@ -5504,8 +5843,11 @@
       <c r="E30" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" s="1" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>216</v>
       </c>
@@ -5521,8 +5863,11 @@
       <c r="E31" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="1" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>169</v>
       </c>
@@ -5538,8 +5883,11 @@
       <c r="E32" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="1" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -5554,6 +5902,9 @@
       </c>
       <c r="E33" s="1" t="s">
         <v>146</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>1373</v>
       </c>
     </row>
   </sheetData>
@@ -5593,26 +5944,58 @@
     <hyperlink ref="E16" r:id="rId30" location="Czech" xr:uid="{707FBED6-1241-498C-92D1-A91F8588F09D}"/>
     <hyperlink ref="E5" r:id="rId31" location="Czech" xr:uid="{2097113B-6B76-4D3D-A30A-7CF37B598414}"/>
     <hyperlink ref="E29" r:id="rId32" location="Czech" xr:uid="{05E9F102-CF14-41F7-BF4B-16F650608EE1}"/>
+    <hyperlink ref="F2" r:id="rId33" xr:uid="{A733EECB-5032-4005-8F80-25AD4FFB56CC}"/>
+    <hyperlink ref="F3" r:id="rId34" xr:uid="{B3B1E8E8-FAA1-4BFD-80A6-E46CF4F8C60E}"/>
+    <hyperlink ref="F4" r:id="rId35" xr:uid="{395312A8-B101-4A8C-A888-0191C1713CAE}"/>
+    <hyperlink ref="F5" r:id="rId36" xr:uid="{B5EB5799-A197-4848-B89A-0E13BA728F61}"/>
+    <hyperlink ref="F6" r:id="rId37" xr:uid="{0BFEADAA-3DD2-48EE-9BD1-9BEB280895F7}"/>
+    <hyperlink ref="F7" r:id="rId38" xr:uid="{A491F0C8-D6CC-4249-A24F-77DE50E4F303}"/>
+    <hyperlink ref="F9" r:id="rId39" xr:uid="{6C2F9952-CE09-476F-A84B-4A9AFB057420}"/>
+    <hyperlink ref="F8" r:id="rId40" xr:uid="{A0E6B86F-683C-401D-ABF8-96D2E69E4DFE}"/>
+    <hyperlink ref="F10" r:id="rId41" xr:uid="{3A5EAD61-0C3A-4DA2-A6B8-F22669724A12}"/>
+    <hyperlink ref="F11" r:id="rId42" xr:uid="{2FD097D8-A324-4074-97BA-D13DCBEF9395}"/>
+    <hyperlink ref="F12" r:id="rId43" xr:uid="{E17BA980-CF77-4359-8DAC-74748B244B5E}"/>
+    <hyperlink ref="F13" r:id="rId44" xr:uid="{30A4755C-CF06-45E5-B7D1-A4AA320A8714}"/>
+    <hyperlink ref="F14" r:id="rId45" xr:uid="{2799BB1C-A349-4598-BE6B-90AF83C6684A}"/>
+    <hyperlink ref="F15" r:id="rId46" xr:uid="{C82090DE-52F9-46EA-99AC-DC82B3A405A3}"/>
+    <hyperlink ref="F16" r:id="rId47" xr:uid="{570996C6-CEC3-4142-B7C5-C22C7299898B}"/>
+    <hyperlink ref="F17" r:id="rId48" xr:uid="{25258666-759E-4E7D-8CCE-5337101DD370}"/>
+    <hyperlink ref="F18" r:id="rId49" xr:uid="{393BC592-772E-490F-97AE-B7CF73FDBE49}"/>
+    <hyperlink ref="F19" r:id="rId50" xr:uid="{53F5ED32-35F5-45D6-A3D6-5A86256137C4}"/>
+    <hyperlink ref="F20" r:id="rId51" xr:uid="{44519846-7D8E-424F-9670-41D42721F7E9}"/>
+    <hyperlink ref="F21" r:id="rId52" xr:uid="{1BD3DC77-88EC-4DE7-BCAC-85FB53FF35C5}"/>
+    <hyperlink ref="F22" r:id="rId53" xr:uid="{D083192B-E8EF-48F3-844D-2F8DB0251926}"/>
+    <hyperlink ref="F23" r:id="rId54" xr:uid="{CC53F576-3320-45C2-B06E-199A4ED0BD56}"/>
+    <hyperlink ref="F24" r:id="rId55" xr:uid="{D5AAFC96-75EF-4AAA-92FD-D5EAC0A3F9CD}"/>
+    <hyperlink ref="F25" r:id="rId56" xr:uid="{3F015C09-8920-41A4-BDA1-BDFE313D18B3}"/>
+    <hyperlink ref="F26" r:id="rId57" xr:uid="{568DC4EF-D38F-42C9-8E35-C4752DAAF6FD}"/>
+    <hyperlink ref="F27" r:id="rId58" xr:uid="{3E8922F9-6D0F-4959-9ED6-0E00D607C69E}"/>
+    <hyperlink ref="F28" r:id="rId59" xr:uid="{8E09CF94-7BCF-4202-A984-FA4ED64A685C}"/>
+    <hyperlink ref="F29" r:id="rId60" xr:uid="{BFDA354C-0946-4C91-BBE9-AFE842AA3687}"/>
+    <hyperlink ref="F30" r:id="rId61" xr:uid="{8D4236D7-6F9D-41A3-A8F1-5F64F42EB045}"/>
+    <hyperlink ref="F31" r:id="rId62" xr:uid="{08B858BA-8E14-49DF-A46B-ACE2552BF918}"/>
+    <hyperlink ref="F32" r:id="rId63" xr:uid="{E987556D-227D-4A62-9A2B-99FA9724D119}"/>
+    <hyperlink ref="F33" r:id="rId64" xr:uid="{AF913E7E-1976-447C-91AB-C84826A84328}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId33"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId65"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD324FC-9653-4492-B751-94A43CE3C06A}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
@@ -5623,7 +6006,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>933</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>934</v>
@@ -5631,7 +6014,9 @@
       <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>1103</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -5652,7 +6037,9 @@
       <c r="C2" s="1" t="s">
         <v>936</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="9" t="s">
+        <v>1374</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5673,7 +6060,9 @@
       <c r="C3" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="9" t="s">
+        <v>1375</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -5694,7 +6083,9 @@
       <c r="C4" s="1" t="s">
         <v>929</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="1" t="s">
+        <v>1376</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5715,7 +6106,9 @@
       <c r="C5" s="1" t="s">
         <v>931</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="1" t="s">
+        <v>1377</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -5736,7 +6129,9 @@
       <c r="C6" s="1" t="s">
         <v>940</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="1" t="s">
+        <v>1378</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -5757,7 +6152,9 @@
       <c r="C7" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="1" t="s">
+        <v>1379</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -5778,7 +6175,9 @@
       <c r="C8" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="1" t="s">
+        <v>1380</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -5799,7 +6198,9 @@
       <c r="C9" s="1" t="s">
         <v>943</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="1" t="s">
+        <v>1381</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -5820,7 +6221,9 @@
       <c r="C10" s="1" t="s">
         <v>945</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="1" t="s">
+        <v>1382</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -5841,7 +6244,9 @@
       <c r="C11" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="1" t="s">
+        <v>1383</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -5862,7 +6267,9 @@
       <c r="C12" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="1" t="s">
+        <v>1384</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -5883,7 +6290,9 @@
       <c r="C13" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="1" t="s">
+        <v>1385</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -5904,7 +6313,9 @@
       <c r="C14" s="1" t="s">
         <v>955</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="1" t="s">
+        <v>1386</v>
+      </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -5925,7 +6336,7 @@
       <c r="C15" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -5946,7 +6357,9 @@
       <c r="C16" s="1" t="s">
         <v>961</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="1" t="s">
+        <v>1387</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -5967,7 +6380,9 @@
       <c r="C17" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="1" t="s">
+        <v>1388</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5988,7 +6403,7 @@
       <c r="C18" s="1" t="s">
         <v>967</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -6009,6 +6424,9 @@
       <c r="C19" s="1" t="s">
         <v>969</v>
       </c>
+      <c r="D19" s="1" t="s">
+        <v>1389</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -6020,6 +6438,12 @@
       <c r="C20" s="1" t="s">
         <v>973</v>
       </c>
+      <c r="D20" s="1" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D21" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6042,17 +6466,35 @@
     <hyperlink ref="C18" r:id="rId17" location="Czech" xr:uid="{5276FF4D-4D1F-4C27-9A0E-57C51C44A1ED}"/>
     <hyperlink ref="C19" r:id="rId18" location="Czech" xr:uid="{2C9E92A7-2248-4806-96A2-AD2E96875720}"/>
     <hyperlink ref="C20" r:id="rId19" location="Czech" xr:uid="{C19C8B23-BA27-4B0B-B8AC-9F9BCDC521B7}"/>
+    <hyperlink ref="D2" r:id="rId20" xr:uid="{F0BDE044-1A8F-4CF4-AACB-4630C322A2ED}"/>
+    <hyperlink ref="D3" r:id="rId21" xr:uid="{05481DE3-105B-4AF5-8A5E-E7759318892B}"/>
+    <hyperlink ref="D4" r:id="rId22" xr:uid="{37E8440F-D901-40BA-B510-B023D20867DE}"/>
+    <hyperlink ref="D5" r:id="rId23" xr:uid="{15BC1D47-CCE5-4B58-A2B9-6D09B9D1BE26}"/>
+    <hyperlink ref="D6" r:id="rId24" xr:uid="{C72544EB-4BA8-41C8-9473-3B1A0849DF2E}"/>
+    <hyperlink ref="D7" r:id="rId25" xr:uid="{1A04ED37-EB14-411A-8287-52E3963269CB}"/>
+    <hyperlink ref="D8" r:id="rId26" xr:uid="{F312E125-9DE7-419C-8CDA-1B02C16FCC40}"/>
+    <hyperlink ref="D9" r:id="rId27" xr:uid="{222A39D4-5015-4BB4-9915-86158874D9F4}"/>
+    <hyperlink ref="D10" r:id="rId28" xr:uid="{B048A639-6714-48CA-8BE8-BFE27FB206B7}"/>
+    <hyperlink ref="D11" r:id="rId29" xr:uid="{839B253F-92FC-48FA-BF9D-B6FA8BDB3358}"/>
+    <hyperlink ref="D12" r:id="rId30" xr:uid="{CFC7C849-0DC9-403C-B7BD-BFDCAA7613AF}"/>
+    <hyperlink ref="D13" r:id="rId31" xr:uid="{BC2ADF69-359C-4D5B-8F9C-AEFA6F7D66DE}"/>
+    <hyperlink ref="D14" r:id="rId32" xr:uid="{4709A1D2-067C-4075-8FF8-8D13BC7CEBF7}"/>
+    <hyperlink ref="D16" r:id="rId33" xr:uid="{0730EB0A-DF61-4295-9E30-4A916EA450C5}"/>
+    <hyperlink ref="D17" r:id="rId34" xr:uid="{511812B8-1CA2-4157-A0AA-A7670A20A653}"/>
+    <hyperlink ref="D19" r:id="rId35" xr:uid="{DB078DA7-33D2-4ADA-8BCF-D0C1DA9630B2}"/>
+    <hyperlink ref="D20" r:id="rId36" xr:uid="{176499E1-6475-415F-A1D8-628288BDF6DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId37"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEFB715-7639-4EA0-903C-A45601E83B0C}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6062,9 +6504,10 @@
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6080,8 +6523,11 @@
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1010</v>
       </c>
@@ -6097,8 +6543,11 @@
       <c r="E2" s="1" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1088</v>
       </c>
@@ -6114,8 +6563,11 @@
       <c r="E3" s="1" t="s">
         <v>1089</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>766</v>
       </c>
@@ -6131,8 +6583,11 @@
       <c r="E4" s="1" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1091</v>
       </c>
@@ -6148,8 +6603,11 @@
       <c r="E5" s="1" t="s">
         <v>1092</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1048</v>
       </c>
@@ -6165,8 +6623,11 @@
       <c r="E6" s="1" t="s">
         <v>1050</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1100</v>
       </c>
@@ -6182,8 +6643,11 @@
       <c r="E7" s="1" t="s">
         <v>1101</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1072</v>
       </c>
@@ -6199,8 +6663,11 @@
       <c r="E8" s="1" t="s">
         <v>1075</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1053</v>
       </c>
@@ -6216,8 +6683,11 @@
       <c r="E9" s="1" t="s">
         <v>1054</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1076</v>
       </c>
@@ -6233,8 +6703,11 @@
       <c r="E10" s="1" t="s">
         <v>1079</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1064</v>
       </c>
@@ -6250,8 +6723,11 @@
       <c r="E11" s="1" t="s">
         <v>1067</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1080</v>
       </c>
@@ -6267,8 +6743,11 @@
       <c r="E12" s="1" t="s">
         <v>1082</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1068</v>
       </c>
@@ -6284,8 +6763,11 @@
       <c r="E13" s="1" t="s">
         <v>1071</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1060</v>
       </c>
@@ -6301,8 +6783,11 @@
       <c r="E14" s="1" t="s">
         <v>1061</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1056</v>
       </c>
@@ -6318,8 +6803,11 @@
       <c r="E15" s="1" t="s">
         <v>1059</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>980</v>
       </c>
@@ -6335,8 +6823,11 @@
       <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1094</v>
       </c>
@@ -6352,8 +6843,11 @@
       <c r="E17" s="1" t="s">
         <v>1096</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="1" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1097</v>
       </c>
@@ -6369,8 +6863,11 @@
       <c r="E18" s="1" t="s">
         <v>1099</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>347</v>
       </c>
@@ -6386,8 +6883,11 @@
       <c r="E19" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1084</v>
       </c>
@@ -6403,8 +6903,11 @@
       <c r="E20" s="1" t="s">
         <v>1086</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1042</v>
       </c>
@@ -6420,8 +6923,11 @@
       <c r="E21" s="1" t="s">
         <v>1041</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>776</v>
       </c>
@@ -6437,8 +6943,11 @@
       <c r="E22" s="1" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1045</v>
       </c>
@@ -6454,8 +6963,11 @@
       <c r="E23" s="1" t="s">
         <v>1046</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="1" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>349</v>
       </c>
@@ -6470,6 +6982,9 @@
       </c>
       <c r="E24" s="1" t="s">
         <v>351</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>1412</v>
       </c>
     </row>
   </sheetData>
@@ -6500,9 +7015,32 @@
     <hyperlink ref="E4" r:id="rId21" location="Czech" xr:uid="{34C4E0F6-A3D9-4746-9C92-C8F83D3DF15E}"/>
     <hyperlink ref="E22" r:id="rId22" location="Czech" xr:uid="{FAEDDDA3-762C-40ED-89CF-102CB62E7CF2}"/>
     <hyperlink ref="E7" r:id="rId23" location="Czech" xr:uid="{C02FB070-4127-49F8-8456-7C9B3209F3BE}"/>
+    <hyperlink ref="F2" r:id="rId24" xr:uid="{652A5BB3-2A19-4253-84F0-8DA4239B6C05}"/>
+    <hyperlink ref="F3" r:id="rId25" xr:uid="{EA5245C2-EB11-47A8-AAD4-97A9FC4591E0}"/>
+    <hyperlink ref="F4" r:id="rId26" xr:uid="{7087630F-9DD8-40B4-B614-2154E7CAF729}"/>
+    <hyperlink ref="F5" r:id="rId27" xr:uid="{6C5BA987-6010-4718-84D9-A53293DA80DF}"/>
+    <hyperlink ref="F6" r:id="rId28" xr:uid="{A92FBC19-9C53-4810-9BED-6D3DD879ED54}"/>
+    <hyperlink ref="F7" r:id="rId29" xr:uid="{9A023231-E7A5-4F3F-9F28-2441DB17004C}"/>
+    <hyperlink ref="F8" r:id="rId30" xr:uid="{5B197407-2F44-40FB-944A-ED6DA43F35E4}"/>
+    <hyperlink ref="F9" r:id="rId31" xr:uid="{2D849C71-DF9F-48D2-8C86-4126185D29ED}"/>
+    <hyperlink ref="F10" r:id="rId32" xr:uid="{D426AC25-85DC-4A2B-8C15-B193E9D016B4}"/>
+    <hyperlink ref="F11" r:id="rId33" xr:uid="{0F08C970-C907-4FE5-B4D5-C72072F1A9D5}"/>
+    <hyperlink ref="F12" r:id="rId34" xr:uid="{DF7DBAD4-40D5-41B9-A3A0-D9F8DD54088F}"/>
+    <hyperlink ref="F13" r:id="rId35" xr:uid="{815F305B-4319-4083-84F7-11E2707A5810}"/>
+    <hyperlink ref="F14" r:id="rId36" xr:uid="{0527FFDB-D63C-4A91-AE23-F5ED2CD13421}"/>
+    <hyperlink ref="F15" r:id="rId37" xr:uid="{971331C2-966D-4CD7-AFAA-D56860C27987}"/>
+    <hyperlink ref="F16" r:id="rId38" xr:uid="{E6C1FDEA-B68A-4C12-B28C-1C5F945BA612}"/>
+    <hyperlink ref="F17" r:id="rId39" xr:uid="{10AA943B-9EDF-4E08-98A8-0351F38EF550}"/>
+    <hyperlink ref="F18" r:id="rId40" xr:uid="{6646BE0E-AA8A-4B13-B53F-C179A64B787B}"/>
+    <hyperlink ref="F19" r:id="rId41" xr:uid="{DC84B4D9-C722-417B-93E7-942935C08475}"/>
+    <hyperlink ref="F20" r:id="rId42" xr:uid="{EA458E9F-E963-4B4A-BA91-0EFF4F738D3B}"/>
+    <hyperlink ref="F21" r:id="rId43" xr:uid="{2F0FE915-72C5-4AFA-9211-DAAACCCB7061}"/>
+    <hyperlink ref="F22" r:id="rId44" xr:uid="{D60B4B6B-AA39-404F-9A5E-C79DB3E892D0}"/>
+    <hyperlink ref="F23" r:id="rId45" xr:uid="{B6915260-89B6-4DC1-B331-532F76A9A460}"/>
+    <hyperlink ref="F24" r:id="rId46" xr:uid="{6A15D661-E801-402B-9544-03FF54E53335}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId24"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -9083,7 +9621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3081E238-0A75-4CCA-BCD2-D049DAB6C4FD}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -10364,8 +10902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCD7ADF-A934-4B8C-90F5-000C68281CBC}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10375,7 +10913,7 @@
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -11533,10 +12071,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98745185-8E10-42AF-9471-9E6947DCA44E}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11546,9 +12084,10 @@
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -11564,8 +12103,11 @@
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1010</v>
       </c>
@@ -11581,8 +12123,11 @@
       <c r="E2" s="1" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>984</v>
       </c>
@@ -11598,8 +12143,11 @@
       <c r="E3" s="1" t="s">
         <v>986</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>989</v>
       </c>
@@ -11615,8 +12163,11 @@
       <c r="E4" s="1" t="s">
         <v>990</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="1" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>979</v>
       </c>
@@ -11632,8 +12183,11 @@
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>992</v>
       </c>
@@ -11649,8 +12203,11 @@
       <c r="E6" s="1" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="1" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1007</v>
       </c>
@@ -11666,8 +12223,11 @@
       <c r="E7" s="1" t="s">
         <v>1009</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>980</v>
       </c>
@@ -11683,8 +12243,11 @@
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1003</v>
       </c>
@@ -11700,8 +12263,11 @@
       <c r="E9" s="1" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>996</v>
       </c>
@@ -11717,8 +12283,11 @@
       <c r="E10" s="1" t="s">
         <v>998</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>978</v>
       </c>
@@ -11734,8 +12303,11 @@
       <c r="E11" s="1" t="s">
         <v>982</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>975</v>
       </c>
@@ -11750,6 +12322,9 @@
       </c>
       <c r="E12" s="1" t="s">
         <v>976</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>1341</v>
       </c>
     </row>
   </sheetData>
@@ -11768,8 +12343,19 @@
     <hyperlink ref="E9" r:id="rId9" location="Czech" xr:uid="{25410E82-2D7A-48B5-850B-E34B55C61C62}"/>
     <hyperlink ref="E7" r:id="rId10" location="Czech" xr:uid="{5D91D57B-B468-492F-A4D1-49BD44A37A67}"/>
     <hyperlink ref="E2" r:id="rId11" location="Czech" xr:uid="{D26896FD-CF79-4F40-9950-214F4CF020F4}"/>
+    <hyperlink ref="F2" r:id="rId12" xr:uid="{3B8988D0-0D97-43DB-89F2-0AF6F2084E7D}"/>
+    <hyperlink ref="F3" r:id="rId13" xr:uid="{7EBBCF48-9049-41FC-B63E-920A1419261B}"/>
+    <hyperlink ref="F4" r:id="rId14" xr:uid="{AC8A8DC3-D062-4654-93A2-B8C307E348D6}"/>
+    <hyperlink ref="F5" r:id="rId15" xr:uid="{431A19D1-8538-415A-832F-5C4B128527A8}"/>
+    <hyperlink ref="F6" r:id="rId16" xr:uid="{55191B17-D3BB-4BB9-BA0B-2BA68FABF358}"/>
+    <hyperlink ref="F7" r:id="rId17" xr:uid="{42D5BEEA-6929-4655-93C9-3C9180F0E1BD}"/>
+    <hyperlink ref="F8" r:id="rId18" xr:uid="{A9F8839A-8340-4C6C-80AA-2B091B8A8809}"/>
+    <hyperlink ref="F9" r:id="rId19" xr:uid="{116C6B14-2D7E-42C9-BAE3-925127A67EDA}"/>
+    <hyperlink ref="F10" r:id="rId20" xr:uid="{550C7506-1DF7-4910-9AE0-6F135EEA4B7F}"/>
+    <hyperlink ref="F11" r:id="rId21" xr:uid="{89A67A2E-9A67-43E6-9E56-98A7025F6405}"/>
+    <hyperlink ref="F12" r:id="rId22" xr:uid="{9CD0EB76-C1F8-4F54-ADF9-33107816F563}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added extra czech terms to school, city and home
</commit_message>
<xml_diff>
--- a/data/vocab.xlsx
+++ b/data/vocab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\Czech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8910A05-5F8E-4D27-AA2E-C65D1CC0F126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872E4536-6663-47B9-92FF-DD040D7C8318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
   </bookViews>
   <sheets>
     <sheet name="Adjectives" sheetId="14" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2176" uniqueCount="1614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2296" uniqueCount="1678">
   <si>
     <t>English</t>
   </si>
@@ -4893,6 +4893,198 @@
   </si>
   <si>
     <t>https://free-images.com/lg/391b/glasses_accessoirs_fashion_1333433.jpg</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testy</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/test#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/c5c6/quiz_test_exam_questionnaire.jpg</t>
+  </si>
+  <si>
+    <t>gym</t>
+  </si>
+  <si>
+    <t>tělocvična</t>
+  </si>
+  <si>
+    <t>tělocvičny</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/t%C4%9Blocvi%C4%8Dna#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/2ddd/ball_gym_ball_in.jpg</t>
+  </si>
+  <si>
+    <t>kaple</t>
+  </si>
+  <si>
+    <t>chapel</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/kaple#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/543c/chapel_church_house_chapel.jpg</t>
+  </si>
+  <si>
+    <t>pencil</t>
+  </si>
+  <si>
+    <t>tužka</t>
+  </si>
+  <si>
+    <t>tužky</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/tu%C5%BEka#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/e3c4/pencils_colored_drawing_school.jpg</t>
+  </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/pero#Czech</t>
+  </si>
+  <si>
+    <t>pero</t>
+  </si>
+  <si>
+    <t>pera</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/7f4b/pen_pens_close_up.jpg</t>
+  </si>
+  <si>
+    <t>pravítko</t>
+  </si>
+  <si>
+    <t>ruler</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/prav%C3%ADtko#Czech</t>
+  </si>
+  <si>
+    <t>pravítka</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/f125/school_ruler_measure_school.jpg</t>
+  </si>
+  <si>
+    <t>eraser</t>
+  </si>
+  <si>
+    <t>guma</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/guma#Czech</t>
+  </si>
+  <si>
+    <t>gumy</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/21bd/office_pink_erasers.jpg</t>
+  </si>
+  <si>
+    <t>zápisník</t>
+  </si>
+  <si>
+    <t>zápisníky</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/z%C3%A1pisn%C3%ADk#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1e96/notebook_pen_workplace_glasses.jpg</t>
+  </si>
+  <si>
+    <t>cafeteria</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/e45b/cafeteria_refectory_canteen_tables.jpg</t>
+  </si>
+  <si>
+    <t>carpark</t>
+  </si>
+  <si>
+    <t>parkoviště</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/parkovi%C5%A1t%C4%9B#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/f30c/carpark_0.jpg</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/auto#Czech</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>auta</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/9788/london_brighton_veteran_car_34.jpg</t>
+  </si>
+  <si>
+    <t>van</t>
+  </si>
+  <si>
+    <t>dodávka</t>
+  </si>
+  <si>
+    <t>dodávky</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/dod%C3%A1vka#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/3a07/white_van_ford_econoline.jpg</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>vlak</t>
+  </si>
+  <si>
+    <t>vlaky</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/vlak#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/32bc/new_train_station_at.jpg</t>
+  </si>
+  <si>
+    <t>subway</t>
+  </si>
+  <si>
+    <t>ship</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/lo%C4%8F#Czech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loď	</t>
+  </si>
+  <si>
+    <t>lodě, lodi</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/42a3/ship_passenger_ship_cruise.jpg</t>
   </si>
 </sst>
 </file>
@@ -4956,13 +5148,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5301,27 +5493,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>554</v>
       </c>
@@ -5346,16 +5538,16 @@
       <c r="I2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="J2" s="8"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>552</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="8"/>
       <c r="D3" t="s">
         <v>560</v>
       </c>
@@ -5365,10 +5557,10 @@
       <c r="F3" t="s">
         <v>562</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="8"/>
       <c r="I3" t="s">
         <v>560</v>
       </c>
@@ -5380,10 +5572,10 @@
       <c r="A4" t="s">
         <v>564</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="8"/>
       <c r="D4" t="s">
         <v>567</v>
       </c>
@@ -5393,10 +5585,10 @@
       <c r="F4" t="s">
         <v>569</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>567</v>
       </c>
@@ -5408,10 +5600,10 @@
       <c r="A5" t="s">
         <v>666</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>667</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>668</v>
       </c>
@@ -5421,10 +5613,10 @@
       <c r="F5" t="s">
         <v>670</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>668</v>
       </c>
@@ -5436,10 +5628,10 @@
       <c r="A6" t="s">
         <v>672</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>674</v>
       </c>
@@ -5449,10 +5641,10 @@
       <c r="F6" t="s">
         <v>676</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>675</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>674</v>
       </c>
@@ -5464,10 +5656,10 @@
       <c r="A7" t="s">
         <v>677</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="8"/>
       <c r="D7" t="s">
         <v>680</v>
       </c>
@@ -5477,10 +5669,10 @@
       <c r="F7" t="s">
         <v>682</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>681</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>680</v>
       </c>
@@ -5492,10 +5684,10 @@
       <c r="A8" t="s">
         <v>685</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>684</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="8"/>
       <c r="D8" t="s">
         <v>686</v>
       </c>
@@ -5505,10 +5697,10 @@
       <c r="F8" t="s">
         <v>688</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="8"/>
       <c r="I8" t="s">
         <v>686</v>
       </c>
@@ -5520,10 +5712,10 @@
       <c r="A9" t="s">
         <v>690</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="8"/>
       <c r="D9" t="s">
         <v>692</v>
       </c>
@@ -5533,10 +5725,10 @@
       <c r="F9" t="s">
         <v>694</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="8" t="s">
         <v>693</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="8"/>
       <c r="I9" t="s">
         <v>692</v>
       </c>
@@ -5548,10 +5740,10 @@
       <c r="A10" t="s">
         <v>699</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>696</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="8"/>
       <c r="D10" t="s">
         <v>697</v>
       </c>
@@ -5561,10 +5753,10 @@
       <c r="F10" t="s">
         <v>700</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="8"/>
       <c r="I10" t="s">
         <v>697</v>
       </c>
@@ -5576,10 +5768,10 @@
       <c r="A11" t="s">
         <v>702</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="8"/>
       <c r="D11" t="s">
         <v>701</v>
       </c>
@@ -5589,10 +5781,10 @@
       <c r="F11" t="s">
         <v>701</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="8"/>
       <c r="I11" t="s">
         <v>701</v>
       </c>
@@ -5604,10 +5796,10 @@
       <c r="A12" t="s">
         <v>704</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="8"/>
       <c r="D12" t="s">
         <v>707</v>
       </c>
@@ -5617,10 +5809,10 @@
       <c r="F12" t="s">
         <v>709</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="8" t="s">
         <v>708</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="8"/>
       <c r="I12" t="s">
         <v>707</v>
       </c>
@@ -5632,10 +5824,10 @@
       <c r="A13" t="s">
         <v>710</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="8"/>
       <c r="D13" t="s">
         <v>713</v>
       </c>
@@ -5645,10 +5837,10 @@
       <c r="F13" t="s">
         <v>715</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>714</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="8"/>
       <c r="I13" t="s">
         <v>713</v>
       </c>
@@ -5657,134 +5849,114 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="B19:C19"/>
@@ -5801,17 +5973,37 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" location="Czech" xr:uid="{5941DCB9-FDEB-4587-B027-375759EB9DA4}"/>
@@ -7379,10 +7571,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEFB715-7639-4EA0-903C-A45601E83B0C}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7392,7 +7584,7 @@
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -7457,478 +7649,720 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>766</v>
+        <v>817</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>764</v>
+        <v>818</v>
       </c>
       <c r="D4" t="s">
-        <v>764</v>
+        <v>820</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>765</v>
+        <v>819</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1392</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1091</v>
+        <v>1651</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>1090</v>
+        <v>751</v>
       </c>
       <c r="D5" t="s">
-        <v>1090</v>
+        <v>752</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1092</v>
+        <v>749</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1393</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1048</v>
+        <v>766</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>1049</v>
+        <v>764</v>
       </c>
       <c r="D6" t="s">
-        <v>1051</v>
+        <v>764</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1050</v>
+        <v>765</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1100</v>
+        <v>1624</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>1102</v>
+        <v>1623</v>
       </c>
       <c r="D7" t="s">
-        <v>1102</v>
+        <v>1623</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1101</v>
+        <v>1625</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1395</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1072</v>
+        <v>1091</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>1073</v>
+        <v>1090</v>
       </c>
       <c r="D8" t="s">
-        <v>1074</v>
+        <v>1090</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1075</v>
+        <v>1092</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1053</v>
+        <v>1048</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="D9" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1076</v>
+        <v>850</v>
       </c>
       <c r="B10" t="s">
         <v>263</v>
       </c>
       <c r="C10" t="s">
-        <v>1077</v>
+        <v>851</v>
       </c>
       <c r="D10" t="s">
-        <v>1078</v>
+        <v>853</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1079</v>
+        <v>852</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1398</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1064</v>
+        <v>1100</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>1066</v>
+        <v>1102</v>
       </c>
       <c r="D11" t="s">
-        <v>1065</v>
+        <v>1102</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1067</v>
+        <v>1101</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1080</v>
+        <v>1072</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>1081</v>
+        <v>1073</v>
       </c>
       <c r="D12" t="s">
-        <v>1081</v>
+        <v>1074</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1082</v>
+        <v>1075</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1068</v>
+        <v>1642</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>1069</v>
+        <v>1643</v>
       </c>
       <c r="D13" t="s">
-        <v>1070</v>
+        <v>1645</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1071</v>
+        <v>1644</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1401</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1060</v>
+        <v>1053</v>
       </c>
       <c r="B14" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>1063</v>
+        <v>1052</v>
       </c>
       <c r="D14" t="s">
-        <v>1062</v>
+        <v>1055</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1061</v>
+        <v>1054</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1402</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1056</v>
+        <v>1076</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C15" t="s">
-        <v>1057</v>
+        <v>1077</v>
       </c>
       <c r="D15" t="s">
-        <v>1058</v>
+        <v>1078</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1059</v>
+        <v>1079</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>980</v>
+        <v>1064</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>1066</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>1065</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>13</v>
+        <v>1067</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>1093</v>
+        <v>1081</v>
       </c>
       <c r="D17" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1097</v>
+        <v>1068</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>1098</v>
+        <v>1069</v>
       </c>
       <c r="D18" t="s">
-        <v>1098</v>
+        <v>1070</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>1099</v>
+        <v>1071</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>347</v>
+        <v>1060</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C19" t="s">
-        <v>345</v>
+        <v>1063</v>
       </c>
       <c r="D19" t="s">
-        <v>348</v>
+        <v>1062</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>346</v>
+        <v>1061</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1084</v>
+        <v>856</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C20" t="s">
-        <v>1083</v>
+        <v>854</v>
       </c>
       <c r="D20" t="s">
-        <v>1085</v>
+        <v>855</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1086</v>
+        <v>857</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1408</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1042</v>
+        <v>1056</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>1042</v>
+        <v>1057</v>
       </c>
       <c r="D21" t="s">
-        <v>1043</v>
+        <v>1058</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>1041</v>
+        <v>1059</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1409</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>776</v>
+        <v>980</v>
       </c>
       <c r="B22" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>775</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>778</v>
+        <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>777</v>
+        <v>13</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1410</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1045</v>
+        <v>854</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="C23" t="s">
-        <v>1044</v>
+        <v>1647</v>
       </c>
       <c r="D23" t="s">
-        <v>1047</v>
+        <v>1648</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>1046</v>
+        <v>1649</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1411</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1634</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1635</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1633</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>1636</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1628</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1629</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1630</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1098</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1640</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>347</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>345</v>
+      </c>
+      <c r="D29" t="s">
+        <v>348</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>776</v>
+      </c>
+      <c r="B32" t="s">
+        <v>263</v>
+      </c>
+      <c r="C32" t="s">
+        <v>775</v>
+      </c>
+      <c r="D32" t="s">
+        <v>778</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B34" t="s">
+        <v>263</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1614</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1615</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>1616</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>349</v>
       </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
         <v>350</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D35" t="s">
         <v>352</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>1412</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E24">
-    <sortCondition ref="A1:A24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F35">
+    <sortCondition ref="A11:A35"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E19" r:id="rId1" location="Czech" xr:uid="{D97F8FF0-5DDF-4BF6-8B75-56812833AFC4}"/>
-    <hyperlink ref="E21" r:id="rId2" location="Czech" xr:uid="{5ECCD1F0-6299-4497-81CE-85479F6D97BD}"/>
-    <hyperlink ref="E23" r:id="rId3" location="Czech" xr:uid="{98E0B637-1971-43ED-AB24-FEC7F8827688}"/>
-    <hyperlink ref="E24" r:id="rId4" location="Czech" xr:uid="{F27F07FF-6D47-490B-ACF8-7D7F118191BC}"/>
-    <hyperlink ref="E6" r:id="rId5" location="Czech" xr:uid="{40ED5768-D32F-4DC3-A6D1-59E668BC2EF3}"/>
-    <hyperlink ref="E9" r:id="rId6" location="Czech" xr:uid="{8CDB0446-3BE2-48ED-96C1-CC8A1BB918EB}"/>
-    <hyperlink ref="E15" r:id="rId7" location="Czech" xr:uid="{9ADDE44A-7C9E-4322-BA5C-29D6154547C3}"/>
-    <hyperlink ref="E16" r:id="rId8" location="Czech" xr:uid="{45DE09DF-A0F2-410A-8697-5EB4C73A92F9}"/>
+    <hyperlink ref="E29" r:id="rId1" location="Czech" xr:uid="{D97F8FF0-5DDF-4BF6-8B75-56812833AFC4}"/>
+    <hyperlink ref="E31" r:id="rId2" location="Czech" xr:uid="{5ECCD1F0-6299-4497-81CE-85479F6D97BD}"/>
+    <hyperlink ref="E33" r:id="rId3" location="Czech" xr:uid="{98E0B637-1971-43ED-AB24-FEC7F8827688}"/>
+    <hyperlink ref="E35" r:id="rId4" location="Czech" xr:uid="{F27F07FF-6D47-490B-ACF8-7D7F118191BC}"/>
+    <hyperlink ref="E9" r:id="rId5" location="Czech" xr:uid="{40ED5768-D32F-4DC3-A6D1-59E668BC2EF3}"/>
+    <hyperlink ref="E14" r:id="rId6" location="Czech" xr:uid="{8CDB0446-3BE2-48ED-96C1-CC8A1BB918EB}"/>
+    <hyperlink ref="E21" r:id="rId7" location="Czech" xr:uid="{9ADDE44A-7C9E-4322-BA5C-29D6154547C3}"/>
+    <hyperlink ref="E22" r:id="rId8" location="Czech" xr:uid="{45DE09DF-A0F2-410A-8697-5EB4C73A92F9}"/>
     <hyperlink ref="E2" r:id="rId9" location="Czech" xr:uid="{D4DB7691-3F43-4333-ACAB-CA253041DEE4}"/>
-    <hyperlink ref="E14" r:id="rId10" location="Czech" xr:uid="{9138BA5E-0808-4BB8-B9B6-0D558D0E998A}"/>
-    <hyperlink ref="E11" r:id="rId11" location="Czech" xr:uid="{7B9D727B-5297-445D-9AD3-489A63A0521F}"/>
-    <hyperlink ref="E13" r:id="rId12" location="Czech" xr:uid="{D3E55CC0-4E01-4AA6-BF7F-197F82CEB06D}"/>
-    <hyperlink ref="E8" r:id="rId13" location="Czech" xr:uid="{D37C10E0-4654-4B86-BECF-808A54E14FDF}"/>
-    <hyperlink ref="E10" r:id="rId14" location="Czech" xr:uid="{22A7CE5F-45D5-4F42-AB18-734E14BB07D3}"/>
-    <hyperlink ref="E12" r:id="rId15" location="Czech" xr:uid="{74D7E1BD-0CFC-4059-97AF-46D4B751DF00}"/>
-    <hyperlink ref="E20" r:id="rId16" location="Czech" xr:uid="{67A4A789-04F4-4613-89BA-71C7CC593D4C}"/>
+    <hyperlink ref="E19" r:id="rId10" location="Czech" xr:uid="{9138BA5E-0808-4BB8-B9B6-0D558D0E998A}"/>
+    <hyperlink ref="E16" r:id="rId11" location="Czech" xr:uid="{7B9D727B-5297-445D-9AD3-489A63A0521F}"/>
+    <hyperlink ref="E18" r:id="rId12" location="Czech" xr:uid="{D3E55CC0-4E01-4AA6-BF7F-197F82CEB06D}"/>
+    <hyperlink ref="E12" r:id="rId13" location="Czech" xr:uid="{D37C10E0-4654-4B86-BECF-808A54E14FDF}"/>
+    <hyperlink ref="E15" r:id="rId14" location="Czech" xr:uid="{22A7CE5F-45D5-4F42-AB18-734E14BB07D3}"/>
+    <hyperlink ref="E17" r:id="rId15" location="Czech" xr:uid="{74D7E1BD-0CFC-4059-97AF-46D4B751DF00}"/>
+    <hyperlink ref="E30" r:id="rId16" location="Czech" xr:uid="{67A4A789-04F4-4613-89BA-71C7CC593D4C}"/>
     <hyperlink ref="E3" r:id="rId17" location="Czech" xr:uid="{4DE75719-7B32-4B12-84D8-CA1B802F2F21}"/>
-    <hyperlink ref="E5" r:id="rId18" location="Czech" xr:uid="{2CFB094B-20B3-49F9-AFCD-1E5EFFDD14BB}"/>
-    <hyperlink ref="E17" r:id="rId19" location="Czech" xr:uid="{C04BB378-24ED-4BF3-8FE5-A06362B25D8C}"/>
-    <hyperlink ref="E18" r:id="rId20" location="Czech" xr:uid="{D38532B5-01C4-47DE-B5F7-F53E3B1B9090}"/>
-    <hyperlink ref="E4" r:id="rId21" location="Czech" xr:uid="{34C4E0F6-A3D9-4746-9C92-C8F83D3DF15E}"/>
-    <hyperlink ref="E22" r:id="rId22" location="Czech" xr:uid="{FAEDDDA3-762C-40ED-89CF-102CB62E7CF2}"/>
-    <hyperlink ref="E7" r:id="rId23" location="Czech" xr:uid="{C02FB070-4127-49F8-8456-7C9B3209F3BE}"/>
+    <hyperlink ref="E8" r:id="rId18" location="Czech" xr:uid="{2CFB094B-20B3-49F9-AFCD-1E5EFFDD14BB}"/>
+    <hyperlink ref="E26" r:id="rId19" location="Czech" xr:uid="{C04BB378-24ED-4BF3-8FE5-A06362B25D8C}"/>
+    <hyperlink ref="E27" r:id="rId20" location="Czech" xr:uid="{D38532B5-01C4-47DE-B5F7-F53E3B1B9090}"/>
+    <hyperlink ref="E6" r:id="rId21" location="Czech" xr:uid="{34C4E0F6-A3D9-4746-9C92-C8F83D3DF15E}"/>
+    <hyperlink ref="E32" r:id="rId22" location="Czech" xr:uid="{FAEDDDA3-762C-40ED-89CF-102CB62E7CF2}"/>
+    <hyperlink ref="E11" r:id="rId23" location="Czech" xr:uid="{C02FB070-4127-49F8-8456-7C9B3209F3BE}"/>
     <hyperlink ref="F2" r:id="rId24" xr:uid="{652A5BB3-2A19-4253-84F0-8DA4239B6C05}"/>
     <hyperlink ref="F3" r:id="rId25" xr:uid="{EA5245C2-EB11-47A8-AAD4-97A9FC4591E0}"/>
-    <hyperlink ref="F4" r:id="rId26" xr:uid="{7087630F-9DD8-40B4-B614-2154E7CAF729}"/>
-    <hyperlink ref="F5" r:id="rId27" xr:uid="{6C5BA987-6010-4718-84D9-A53293DA80DF}"/>
-    <hyperlink ref="F6" r:id="rId28" xr:uid="{A92FBC19-9C53-4810-9BED-6D3DD879ED54}"/>
-    <hyperlink ref="F7" r:id="rId29" xr:uid="{9A023231-E7A5-4F3F-9F28-2441DB17004C}"/>
-    <hyperlink ref="F8" r:id="rId30" xr:uid="{5B197407-2F44-40FB-944A-ED6DA43F35E4}"/>
-    <hyperlink ref="F9" r:id="rId31" xr:uid="{2D849C71-DF9F-48D2-8C86-4126185D29ED}"/>
-    <hyperlink ref="F10" r:id="rId32" xr:uid="{D426AC25-85DC-4A2B-8C15-B193E9D016B4}"/>
-    <hyperlink ref="F11" r:id="rId33" xr:uid="{0F08C970-C907-4FE5-B4D5-C72072F1A9D5}"/>
-    <hyperlink ref="F12" r:id="rId34" xr:uid="{DF7DBAD4-40D5-41B9-A3A0-D9F8DD54088F}"/>
-    <hyperlink ref="F13" r:id="rId35" xr:uid="{815F305B-4319-4083-84F7-11E2707A5810}"/>
-    <hyperlink ref="F14" r:id="rId36" xr:uid="{0527FFDB-D63C-4A91-AE23-F5ED2CD13421}"/>
-    <hyperlink ref="F15" r:id="rId37" xr:uid="{971331C2-966D-4CD7-AFAA-D56860C27987}"/>
-    <hyperlink ref="F16" r:id="rId38" xr:uid="{E6C1FDEA-B68A-4C12-B28C-1C5F945BA612}"/>
-    <hyperlink ref="F17" r:id="rId39" xr:uid="{10AA943B-9EDF-4E08-98A8-0351F38EF550}"/>
-    <hyperlink ref="F18" r:id="rId40" xr:uid="{6646BE0E-AA8A-4B13-B53F-C179A64B787B}"/>
-    <hyperlink ref="F19" r:id="rId41" xr:uid="{DC84B4D9-C722-417B-93E7-942935C08475}"/>
-    <hyperlink ref="F20" r:id="rId42" xr:uid="{EA458E9F-E963-4B4A-BA91-0EFF4F738D3B}"/>
-    <hyperlink ref="F21" r:id="rId43" xr:uid="{2F0FE915-72C5-4AFA-9211-DAAACCCB7061}"/>
-    <hyperlink ref="F22" r:id="rId44" xr:uid="{D60B4B6B-AA39-404F-9A5E-C79DB3E892D0}"/>
-    <hyperlink ref="F23" r:id="rId45" xr:uid="{B6915260-89B6-4DC1-B331-532F76A9A460}"/>
-    <hyperlink ref="F24" r:id="rId46" xr:uid="{6A15D661-E801-402B-9544-03FF54E53335}"/>
+    <hyperlink ref="F6" r:id="rId26" xr:uid="{7087630F-9DD8-40B4-B614-2154E7CAF729}"/>
+    <hyperlink ref="F8" r:id="rId27" xr:uid="{6C5BA987-6010-4718-84D9-A53293DA80DF}"/>
+    <hyperlink ref="F9" r:id="rId28" xr:uid="{A92FBC19-9C53-4810-9BED-6D3DD879ED54}"/>
+    <hyperlink ref="F11" r:id="rId29" xr:uid="{9A023231-E7A5-4F3F-9F28-2441DB17004C}"/>
+    <hyperlink ref="F12" r:id="rId30" xr:uid="{5B197407-2F44-40FB-944A-ED6DA43F35E4}"/>
+    <hyperlink ref="F14" r:id="rId31" xr:uid="{2D849C71-DF9F-48D2-8C86-4126185D29ED}"/>
+    <hyperlink ref="F15" r:id="rId32" xr:uid="{D426AC25-85DC-4A2B-8C15-B193E9D016B4}"/>
+    <hyperlink ref="F16" r:id="rId33" xr:uid="{0F08C970-C907-4FE5-B4D5-C72072F1A9D5}"/>
+    <hyperlink ref="F17" r:id="rId34" xr:uid="{DF7DBAD4-40D5-41B9-A3A0-D9F8DD54088F}"/>
+    <hyperlink ref="F18" r:id="rId35" xr:uid="{815F305B-4319-4083-84F7-11E2707A5810}"/>
+    <hyperlink ref="F19" r:id="rId36" xr:uid="{0527FFDB-D63C-4A91-AE23-F5ED2CD13421}"/>
+    <hyperlink ref="F21" r:id="rId37" xr:uid="{971331C2-966D-4CD7-AFAA-D56860C27987}"/>
+    <hyperlink ref="F22" r:id="rId38" xr:uid="{E6C1FDEA-B68A-4C12-B28C-1C5F945BA612}"/>
+    <hyperlink ref="F26" r:id="rId39" xr:uid="{10AA943B-9EDF-4E08-98A8-0351F38EF550}"/>
+    <hyperlink ref="F27" r:id="rId40" xr:uid="{6646BE0E-AA8A-4B13-B53F-C179A64B787B}"/>
+    <hyperlink ref="F29" r:id="rId41" xr:uid="{DC84B4D9-C722-417B-93E7-942935C08475}"/>
+    <hyperlink ref="F30" r:id="rId42" xr:uid="{EA458E9F-E963-4B4A-BA91-0EFF4F738D3B}"/>
+    <hyperlink ref="F31" r:id="rId43" xr:uid="{2F0FE915-72C5-4AFA-9211-DAAACCCB7061}"/>
+    <hyperlink ref="F32" r:id="rId44" xr:uid="{D60B4B6B-AA39-404F-9A5E-C79DB3E892D0}"/>
+    <hyperlink ref="F33" r:id="rId45" xr:uid="{B6915260-89B6-4DC1-B331-532F76A9A460}"/>
+    <hyperlink ref="F35" r:id="rId46" xr:uid="{6A15D661-E801-402B-9544-03FF54E53335}"/>
+    <hyperlink ref="E34" r:id="rId47" location="Czech" xr:uid="{91798AEA-5459-42DA-B6E4-2420766483A0}"/>
+    <hyperlink ref="F34" r:id="rId48" xr:uid="{EBCC9979-3371-4833-8364-E017C3EFB5D3}"/>
+    <hyperlink ref="E25" r:id="rId49" location="Czech" xr:uid="{B3062B39-A6FF-4B02-A2CE-969FBD98DAB7}"/>
+    <hyperlink ref="F25" r:id="rId50" xr:uid="{DBBA76E3-E87D-484B-BF41-2A6CA4B36D92}"/>
+    <hyperlink ref="E24" r:id="rId51" location="Czech" xr:uid="{DAF29236-41AB-4544-956A-F138ECD173B1}"/>
+    <hyperlink ref="F24" r:id="rId52" xr:uid="{2C31792E-F9AF-4809-B1DC-E1165E2A2C1A}"/>
+    <hyperlink ref="E28" r:id="rId53" location="Czech" xr:uid="{6105AD8C-B572-48E7-BD10-185FC66856B5}"/>
+    <hyperlink ref="F28" r:id="rId54" xr:uid="{39599B88-5EB9-4530-B12F-172E980A8AD1}"/>
+    <hyperlink ref="E13" r:id="rId55" location="Czech" xr:uid="{817AA916-C9F3-41CC-B2CD-FD84F4EDA4FC}"/>
+    <hyperlink ref="F13" r:id="rId56" xr:uid="{07252F6C-F61C-4479-8200-B992C7873255}"/>
+    <hyperlink ref="E23" r:id="rId57" location="Czech" xr:uid="{5D111A79-2AB3-4AAF-A665-415A239A32CA}"/>
+    <hyperlink ref="F23" r:id="rId58" xr:uid="{645B3A2D-44FD-4744-AECE-ED1F79C8C532}"/>
+    <hyperlink ref="E4" r:id="rId59" location="Czech" xr:uid="{471B3C75-447F-4648-BF8D-3547A5F9B6E6}"/>
+    <hyperlink ref="F4" r:id="rId60" xr:uid="{280AF2E1-B5C1-4538-A199-D85EE816B460}"/>
+    <hyperlink ref="E10" r:id="rId61" location="Czech" xr:uid="{E38FA3F7-1930-4559-BC6C-95930B1B4E94}"/>
+    <hyperlink ref="F10" r:id="rId62" xr:uid="{9BE16012-620C-4A9F-8B1D-EF4B9A0EE3F8}"/>
+    <hyperlink ref="E20" r:id="rId63" location="Czech" xr:uid="{A1294EB3-6F03-4E3C-BF1E-D171B00AEECB}"/>
+    <hyperlink ref="F20" r:id="rId64" xr:uid="{D7DACC4B-FB70-48E9-9BA9-C0F16516DB4D}"/>
+    <hyperlink ref="E5" r:id="rId65" location="Czech" xr:uid="{7300FC3F-FE29-4E36-B542-4CC693CEC8A2}"/>
+    <hyperlink ref="F5" r:id="rId66" xr:uid="{01B208BC-440B-4F65-B127-C76C23B8DF30}"/>
+    <hyperlink ref="E7" r:id="rId67" location="Czech" xr:uid="{459BEE16-B79E-4F25-BCF0-9F729AC399C7}"/>
+    <hyperlink ref="F7" r:id="rId68" xr:uid="{CEF11B34-4837-461E-8510-2A7D13E28C7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId47"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId69"/>
 </worksheet>
 </file>
 
@@ -8039,7 +8473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A83DE8-6398-4B6D-9AFD-F64AA71A004A}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -9608,10 +10042,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4FF4F7-C7FC-4558-887A-7BA51F1283D1}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9746,806 +10180,983 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>295</v>
+        <v>1657</v>
       </c>
       <c r="B7" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>294</v>
+        <v>1659</v>
       </c>
       <c r="D7" t="s">
-        <v>297</v>
+        <v>1660</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>296</v>
+        <v>1658</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1146</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1023</v>
+        <v>1653</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>1024</v>
+        <v>1654</v>
       </c>
       <c r="D8" t="s">
-        <v>1025</v>
+        <v>1654</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1026</v>
+        <v>1655</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1147</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="B9" t="s">
         <v>263</v>
       </c>
       <c r="C9" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="D9" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>251</v>
+        <v>1023</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>255</v>
+        <v>1024</v>
       </c>
       <c r="D10" t="s">
-        <v>256</v>
+        <v>1025</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>257</v>
+        <v>1026</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>370</v>
+        <v>1624</v>
       </c>
       <c r="B11" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>371</v>
+        <v>1623</v>
       </c>
       <c r="D11" t="s">
-        <v>372</v>
+        <v>1623</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>373</v>
+        <v>1625</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1151</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1000</v>
+        <v>276</v>
+      </c>
+      <c r="B12" t="s">
+        <v>263</v>
       </c>
       <c r="C12" t="s">
-        <v>1001</v>
+        <v>277</v>
       </c>
       <c r="D12" t="s">
-        <v>1002</v>
+        <v>278</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>279</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>343</v>
+        <v>251</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>344</v>
+        <v>255</v>
       </c>
       <c r="D13" t="s">
-        <v>344</v>
+        <v>256</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>342</v>
+        <v>257</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="B14" t="s">
         <v>263</v>
       </c>
       <c r="C14" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="D14" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>378</v>
-      </c>
-      <c r="B15" t="s">
-        <v>263</v>
+        <v>1000</v>
       </c>
       <c r="C15" t="s">
-        <v>378</v>
+        <v>1001</v>
       </c>
       <c r="D15" t="s">
-        <v>379</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>377</v>
+        <v>1002</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>261</v>
+        <v>1618</v>
       </c>
       <c r="B16" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>262</v>
+        <v>1619</v>
       </c>
       <c r="D16" t="s">
-        <v>264</v>
+        <v>1620</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>265</v>
+        <v>1621</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1155</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>320</v>
+        <v>343</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>319</v>
+        <v>344</v>
       </c>
       <c r="D17" t="s">
-        <v>321</v>
+        <v>344</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>315</v>
+        <v>382</v>
       </c>
       <c r="B18" t="s">
         <v>263</v>
       </c>
       <c r="C18" t="s">
-        <v>316</v>
+        <v>382</v>
       </c>
       <c r="D18" t="s">
-        <v>318</v>
+        <v>381</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>317</v>
+        <v>380</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>336</v>
+        <v>378</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="C19" t="s">
-        <v>336</v>
+        <v>378</v>
       </c>
       <c r="D19" t="s">
-        <v>337</v>
+        <v>379</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>335</v>
+        <v>377</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1159</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1013</v>
+        <v>261</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C20" t="s">
-        <v>1014</v>
+        <v>262</v>
       </c>
       <c r="D20" t="s">
-        <v>1014</v>
+        <v>264</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1015</v>
+        <v>265</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1192</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>651</v>
+        <v>320</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>652</v>
+        <v>319</v>
       </c>
       <c r="D21" t="s">
-        <v>653</v>
+        <v>321</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>654</v>
+        <v>322</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
       <c r="B22" t="s">
         <v>263</v>
       </c>
       <c r="C22" t="s">
-        <v>358</v>
+        <v>316</v>
       </c>
       <c r="D22" t="s">
-        <v>359</v>
+        <v>318</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>357</v>
+        <v>317</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>298</v>
+        <v>336</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>299</v>
+        <v>336</v>
       </c>
       <c r="D23" t="s">
-        <v>300</v>
+        <v>337</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>301</v>
+        <v>335</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>363</v>
+        <v>1013</v>
       </c>
       <c r="B24" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>364</v>
+        <v>1014</v>
       </c>
       <c r="D24" t="s">
-        <v>366</v>
+        <v>1014</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>365</v>
+        <v>1015</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1162</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>283</v>
+        <v>651</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>284</v>
+        <v>652</v>
       </c>
       <c r="D25" t="s">
-        <v>286</v>
+        <v>653</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>285</v>
+        <v>654</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1163</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C26" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="D26" t="s">
-        <v>1181</v>
+        <v>359</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>375</v>
+        <v>298</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>374</v>
+        <v>299</v>
       </c>
       <c r="D27" t="s">
-        <v>374</v>
+        <v>300</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>376</v>
+        <v>301</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1020</v>
+        <v>363</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C28" t="s">
-        <v>1021</v>
+        <v>364</v>
       </c>
       <c r="D28" t="s">
-        <v>1021</v>
+        <v>366</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>1022</v>
+        <v>365</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1196</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>347</v>
+        <v>283</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>345</v>
+        <v>284</v>
       </c>
       <c r="D29" t="s">
-        <v>348</v>
+        <v>286</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>346</v>
+        <v>285</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>272</v>
+        <v>367</v>
       </c>
       <c r="B30" t="s">
         <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>273</v>
+        <v>368</v>
       </c>
       <c r="D30" t="s">
-        <v>274</v>
+        <v>1181</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>275</v>
+        <v>369</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>269</v>
+        <v>375</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>270</v>
+        <v>374</v>
       </c>
       <c r="D31" t="s">
-        <v>270</v>
+        <v>374</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>271</v>
+        <v>376</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>306</v>
+        <v>1020</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>305</v>
+        <v>1021</v>
       </c>
       <c r="D32" t="s">
-        <v>305</v>
+        <v>1021</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>307</v>
+        <v>1022</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1169</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>390</v>
+        <v>347</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>388</v>
+        <v>345</v>
       </c>
       <c r="D33" t="s">
-        <v>389</v>
+        <v>348</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>387</v>
+        <v>346</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>331</v>
+        <v>1673</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>332</v>
+        <v>1675</v>
       </c>
       <c r="D34" t="s">
-        <v>333</v>
+        <v>1676</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>334</v>
+        <v>1674</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>1171</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="D35" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1172</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>392</v>
+        <v>269</v>
       </c>
       <c r="B36" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>391</v>
+        <v>270</v>
       </c>
       <c r="D36" t="s">
-        <v>391</v>
+        <v>270</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>393</v>
+        <v>271</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1173</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B37" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D37" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>1174</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>354</v>
+        <v>390</v>
       </c>
       <c r="B38" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>353</v>
+        <v>388</v>
       </c>
       <c r="D38" t="s">
-        <v>355</v>
+        <v>389</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>356</v>
+        <v>387</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1175</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="B39" t="s">
         <v>25</v>
       </c>
       <c r="C39" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="D39" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1176</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="D40" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>1177</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>339</v>
+        <v>392</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C41" t="s">
-        <v>338</v>
+        <v>391</v>
       </c>
       <c r="D41" t="s">
-        <v>341</v>
+        <v>391</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>340</v>
+        <v>393</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>1178</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>336</v>
+      </c>
+      <c r="D42" t="s">
+        <v>337</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>303</v>
+      </c>
+      <c r="B43" t="s">
+        <v>263</v>
+      </c>
+      <c r="C43" t="s">
+        <v>303</v>
+      </c>
+      <c r="D43" t="s">
+        <v>302</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>354</v>
+      </c>
+      <c r="B44" t="s">
+        <v>263</v>
+      </c>
+      <c r="C44" t="s">
+        <v>353</v>
+      </c>
+      <c r="D44" t="s">
+        <v>355</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>324</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>323</v>
+      </c>
+      <c r="D45" t="s">
+        <v>326</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>254</v>
+      </c>
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" t="s">
+        <v>250</v>
+      </c>
+      <c r="D46" t="s">
+        <v>253</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B47" t="s">
+        <v>263</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>339</v>
+      </c>
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>338</v>
+      </c>
+      <c r="D48" t="s">
+        <v>341</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>349</v>
       </c>
-      <c r="B42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
         <v>350</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D49" t="s">
         <v>352</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>1179</v>
       </c>
     </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1663</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1664</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>1666</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F42">
-    <sortCondition ref="A15:A42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F50">
+    <sortCondition ref="A25:A50"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1" location="Czech" xr:uid="{E8E8A843-7CC2-4265-B9C9-7C578FA6F1B3}"/>
-    <hyperlink ref="E40" r:id="rId2" location="Czech" xr:uid="{29E3E62B-267F-4E1E-A802-064587EF505B}"/>
-    <hyperlink ref="E16" r:id="rId3" location="Czech" xr:uid="{80E98C80-5593-4A83-A2A7-87A4EB1C1007}"/>
-    <hyperlink ref="E35" r:id="rId4" location="Czech" xr:uid="{BF8C09B8-5CB3-41B4-AC4D-D11D04BC02C0}"/>
-    <hyperlink ref="E31" r:id="rId5" location="Czech" xr:uid="{6C5393CC-A420-41FC-8FA8-5B9F03D3D33C}"/>
-    <hyperlink ref="E30" r:id="rId6" location="Czech" xr:uid="{75060718-EE0D-4E7B-893B-F51D43C5F47C}"/>
-    <hyperlink ref="E9" r:id="rId7" location="Czech" xr:uid="{0A1A2AF2-8380-417F-B569-BA17E5FF2DB5}"/>
+    <hyperlink ref="E13" r:id="rId1" location="Czech" xr:uid="{E8E8A843-7CC2-4265-B9C9-7C578FA6F1B3}"/>
+    <hyperlink ref="E46" r:id="rId2" location="Czech" xr:uid="{29E3E62B-267F-4E1E-A802-064587EF505B}"/>
+    <hyperlink ref="E20" r:id="rId3" location="Czech" xr:uid="{80E98C80-5593-4A83-A2A7-87A4EB1C1007}"/>
+    <hyperlink ref="E40" r:id="rId4" location="Czech" xr:uid="{BF8C09B8-5CB3-41B4-AC4D-D11D04BC02C0}"/>
+    <hyperlink ref="E36" r:id="rId5" location="Czech" xr:uid="{6C5393CC-A420-41FC-8FA8-5B9F03D3D33C}"/>
+    <hyperlink ref="E35" r:id="rId6" location="Czech" xr:uid="{75060718-EE0D-4E7B-893B-F51D43C5F47C}"/>
+    <hyperlink ref="E12" r:id="rId7" location="Czech" xr:uid="{0A1A2AF2-8380-417F-B569-BA17E5FF2DB5}"/>
     <hyperlink ref="E4" r:id="rId8" location="Czech" xr:uid="{8A7CCACB-3B7C-4913-8D8D-C9DC99D020F5}"/>
-    <hyperlink ref="E25" r:id="rId9" location="Czech" xr:uid="{96D89DC3-5D9A-43AF-8C2E-468D6C916A8E}"/>
+    <hyperlink ref="E29" r:id="rId9" location="Czech" xr:uid="{96D89DC3-5D9A-43AF-8C2E-468D6C916A8E}"/>
     <hyperlink ref="E3" r:id="rId10" location="Czech" xr:uid="{EDB4F91E-AEE7-4CCD-8396-9F41716C77D8}"/>
-    <hyperlink ref="E7" r:id="rId11" location="Czech" xr:uid="{C617EAF8-70FD-4FD5-B0AF-6AB6E909FC2A}"/>
-    <hyperlink ref="E23" r:id="rId12" location="Czech" xr:uid="{28D40E54-640C-4A82-A080-BBA9FA62F03E}"/>
-    <hyperlink ref="E37" r:id="rId13" location="Czech" xr:uid="{D141FF0B-EE96-4880-85F0-D8087C48F862}"/>
-    <hyperlink ref="E32" r:id="rId14" location="Czech" xr:uid="{112B474D-8350-4F16-9CC5-C8D11060BD5D}"/>
+    <hyperlink ref="E9" r:id="rId11" location="Czech" xr:uid="{C617EAF8-70FD-4FD5-B0AF-6AB6E909FC2A}"/>
+    <hyperlink ref="E27" r:id="rId12" location="Czech" xr:uid="{28D40E54-640C-4A82-A080-BBA9FA62F03E}"/>
+    <hyperlink ref="E43" r:id="rId13" location="Czech" xr:uid="{D141FF0B-EE96-4880-85F0-D8087C48F862}"/>
+    <hyperlink ref="E37" r:id="rId14" location="Czech" xr:uid="{112B474D-8350-4F16-9CC5-C8D11060BD5D}"/>
     <hyperlink ref="E5" r:id="rId15" location="Czech" xr:uid="{07FD535B-EB59-4C4B-8E68-0D99512B3041}"/>
     <hyperlink ref="E6" r:id="rId16" location="Czech" xr:uid="{A973B00A-0F15-478C-9FFE-9ED62A3D2B37}"/>
-    <hyperlink ref="E18" r:id="rId17" location="Czech" xr:uid="{6351909F-66B5-42E5-AF1F-1F940A14FAFB}"/>
-    <hyperlink ref="E17" r:id="rId18" location="Czech" xr:uid="{27FEB837-45BD-47D3-BEB1-126B2DC7404A}"/>
-    <hyperlink ref="E39" r:id="rId19" location="Czech" xr:uid="{C7E04CC5-27AF-4037-B58E-AAF3E591D244}"/>
-    <hyperlink ref="E34" r:id="rId20" location="Czech" xr:uid="{E3084264-159C-47B1-B581-425542C1D9FB}"/>
-    <hyperlink ref="E19" r:id="rId21" location="Czech" xr:uid="{DFEC6FB5-BCF3-4673-98A7-4C65D2444CB0}"/>
-    <hyperlink ref="E41" r:id="rId22" location="Czech" xr:uid="{7E2D7D06-8717-4D2C-A92E-045B23EBFA2B}"/>
-    <hyperlink ref="E13" r:id="rId23" location="Czech" xr:uid="{B960A189-7281-41C1-A30F-8B7F4DEF92D0}"/>
-    <hyperlink ref="E29" r:id="rId24" location="Czech" xr:uid="{5E7CDE06-64F5-4508-83F9-4FF602E27BF4}"/>
-    <hyperlink ref="E42" r:id="rId25" location="Czech" xr:uid="{E1713815-AA75-49D0-9539-BF687802643F}"/>
-    <hyperlink ref="E38" r:id="rId26" location="Czech" xr:uid="{8401D44B-03D8-489A-9169-9315E78B1375}"/>
-    <hyperlink ref="E22" r:id="rId27" location="Czech" xr:uid="{EF27B7C9-59D7-4234-B91F-02EE48EFE63C}"/>
+    <hyperlink ref="E22" r:id="rId17" location="Czech" xr:uid="{6351909F-66B5-42E5-AF1F-1F940A14FAFB}"/>
+    <hyperlink ref="E21" r:id="rId18" location="Czech" xr:uid="{27FEB837-45BD-47D3-BEB1-126B2DC7404A}"/>
+    <hyperlink ref="E45" r:id="rId19" location="Czech" xr:uid="{C7E04CC5-27AF-4037-B58E-AAF3E591D244}"/>
+    <hyperlink ref="E39" r:id="rId20" location="Czech" xr:uid="{E3084264-159C-47B1-B581-425542C1D9FB}"/>
+    <hyperlink ref="E23" r:id="rId21" location="Czech" xr:uid="{DFEC6FB5-BCF3-4673-98A7-4C65D2444CB0}"/>
+    <hyperlink ref="E48" r:id="rId22" location="Czech" xr:uid="{7E2D7D06-8717-4D2C-A92E-045B23EBFA2B}"/>
+    <hyperlink ref="E17" r:id="rId23" location="Czech" xr:uid="{B960A189-7281-41C1-A30F-8B7F4DEF92D0}"/>
+    <hyperlink ref="E33" r:id="rId24" location="Czech" xr:uid="{5E7CDE06-64F5-4508-83F9-4FF602E27BF4}"/>
+    <hyperlink ref="E49" r:id="rId25" location="Czech" xr:uid="{E1713815-AA75-49D0-9539-BF687802643F}"/>
+    <hyperlink ref="E44" r:id="rId26" location="Czech" xr:uid="{8401D44B-03D8-489A-9169-9315E78B1375}"/>
+    <hyperlink ref="E26" r:id="rId27" location="Czech" xr:uid="{EF27B7C9-59D7-4234-B91F-02EE48EFE63C}"/>
     <hyperlink ref="E2" r:id="rId28" location="Czech" xr:uid="{FC647918-864F-41DF-BB21-47296C9F74B1}"/>
-    <hyperlink ref="E24" r:id="rId29" location="Czech" xr:uid="{3F938700-E427-435F-8502-01CA89E59C22}"/>
-    <hyperlink ref="E26" r:id="rId30" location="Czech" xr:uid="{427CDB47-98D7-4146-8DD7-3DE6F7B4E300}"/>
-    <hyperlink ref="E11" r:id="rId31" location="Czech" xr:uid="{CE2F5C88-00CA-464B-A12D-EA831C68658E}"/>
-    <hyperlink ref="E27" r:id="rId32" location="Czech" xr:uid="{11BFEBF4-45A4-447B-B0B5-3906CF1A8D70}"/>
-    <hyperlink ref="E15" r:id="rId33" location="Czech" xr:uid="{D0C0F25F-3E91-4514-A4E6-80ADE113A939}"/>
-    <hyperlink ref="E14" r:id="rId34" location="Czech" xr:uid="{8A16B239-D26B-4907-BE6F-19A99D793E23}"/>
-    <hyperlink ref="E33" r:id="rId35" location="Czech" xr:uid="{D6EC7BE6-15DC-49FF-A912-D11DE24143B8}"/>
-    <hyperlink ref="E36" r:id="rId36" location="Czech" xr:uid="{F0DF73B3-7BC6-497F-8E2E-7ED4E75C1E28}"/>
-    <hyperlink ref="E21" r:id="rId37" location="Czech" xr:uid="{49774962-6028-496C-860D-EE9E6E1EF54C}"/>
-    <hyperlink ref="E8" r:id="rId38" location="Czech" xr:uid="{5EAEE623-8274-4002-9D7B-105304776E58}"/>
+    <hyperlink ref="E28" r:id="rId29" location="Czech" xr:uid="{3F938700-E427-435F-8502-01CA89E59C22}"/>
+    <hyperlink ref="E30" r:id="rId30" location="Czech" xr:uid="{427CDB47-98D7-4146-8DD7-3DE6F7B4E300}"/>
+    <hyperlink ref="E14" r:id="rId31" location="Czech" xr:uid="{CE2F5C88-00CA-464B-A12D-EA831C68658E}"/>
+    <hyperlink ref="E31" r:id="rId32" location="Czech" xr:uid="{11BFEBF4-45A4-447B-B0B5-3906CF1A8D70}"/>
+    <hyperlink ref="E19" r:id="rId33" location="Czech" xr:uid="{D0C0F25F-3E91-4514-A4E6-80ADE113A939}"/>
+    <hyperlink ref="E18" r:id="rId34" location="Czech" xr:uid="{8A16B239-D26B-4907-BE6F-19A99D793E23}"/>
+    <hyperlink ref="E38" r:id="rId35" location="Czech" xr:uid="{D6EC7BE6-15DC-49FF-A912-D11DE24143B8}"/>
+    <hyperlink ref="E41" r:id="rId36" location="Czech" xr:uid="{F0DF73B3-7BC6-497F-8E2E-7ED4E75C1E28}"/>
+    <hyperlink ref="E25" r:id="rId37" location="Czech" xr:uid="{49774962-6028-496C-860D-EE9E6E1EF54C}"/>
+    <hyperlink ref="E10" r:id="rId38" location="Czech" xr:uid="{5EAEE623-8274-4002-9D7B-105304776E58}"/>
     <hyperlink ref="F2" r:id="rId39" xr:uid="{848CA005-AB88-455D-98C3-1CEAC84865FB}"/>
     <hyperlink ref="F3" r:id="rId40" xr:uid="{45AF1CD9-2226-4BC9-AC51-F67211C8AAC1}"/>
     <hyperlink ref="F4" r:id="rId41" xr:uid="{A409BEA8-4228-4960-B9F2-E116867B379D}"/>
     <hyperlink ref="F5" r:id="rId42" xr:uid="{D92C0DFF-FCDB-457E-9EF8-1504E50C4B40}"/>
     <hyperlink ref="F6" r:id="rId43" xr:uid="{B480FA19-4A92-4FE6-8DC6-E2770660A3EA}"/>
-    <hyperlink ref="F7" r:id="rId44" xr:uid="{7B281F87-ADD6-4FD2-B8A0-71AC411DA7B0}"/>
-    <hyperlink ref="F8" r:id="rId45" xr:uid="{CAE7D724-F5BC-432B-9C84-0B53AD7455FF}"/>
-    <hyperlink ref="F9" r:id="rId46" xr:uid="{CD565EE9-033A-4565-90A6-30F716071F77}"/>
-    <hyperlink ref="F10" r:id="rId47" xr:uid="{471F5768-0829-4CEF-A522-FA39BA5F5EE2}"/>
-    <hyperlink ref="F12" r:id="rId48" xr:uid="{1FA22728-C587-4A22-9481-9CBCC4E51089}"/>
-    <hyperlink ref="F11" r:id="rId49" xr:uid="{5B137EC4-F81A-4B00-A362-FA8224B889F6}"/>
-    <hyperlink ref="F13" r:id="rId50" xr:uid="{B43A2A52-59D5-4F7A-964E-07F90E0C91DD}"/>
-    <hyperlink ref="F14" r:id="rId51" xr:uid="{7DBFD75F-6275-4085-9EC2-E28F6BA6F2BF}"/>
-    <hyperlink ref="F15" r:id="rId52" xr:uid="{D47388E8-8D39-4137-A17D-3979FFC960DA}"/>
-    <hyperlink ref="F16" r:id="rId53" xr:uid="{BB1F3EF0-32F0-4194-958C-E4C3346408FC}"/>
-    <hyperlink ref="F17" r:id="rId54" xr:uid="{F2DAC8C7-9633-449F-AA57-9516344543A1}"/>
-    <hyperlink ref="F18" r:id="rId55" xr:uid="{7C0D8AB0-3265-4246-81FE-C35CBA4D9DA9}"/>
-    <hyperlink ref="F21" r:id="rId56" xr:uid="{F8C25553-CD78-4C7A-8E01-A614E025CF8A}"/>
-    <hyperlink ref="F19" r:id="rId57" xr:uid="{3B812E5A-F336-459B-B599-05D1B2CC0D25}"/>
-    <hyperlink ref="F22" r:id="rId58" xr:uid="{6C4EC7D6-E3A8-41A0-97C5-26B5D0695873}"/>
-    <hyperlink ref="F23" r:id="rId59" xr:uid="{51BFA554-CEBA-4E7F-A467-DA1DF26DB4B9}"/>
-    <hyperlink ref="F24" r:id="rId60" xr:uid="{EC78ED7F-999D-4C1B-AABC-F94FE5064109}"/>
-    <hyperlink ref="F25" r:id="rId61" xr:uid="{46B1BBB3-F237-4EC9-A0D4-EF7EC84FBF6E}"/>
-    <hyperlink ref="F26" r:id="rId62" xr:uid="{8D683CA9-4AB3-45C0-81CE-58F82581FA95}"/>
-    <hyperlink ref="F27" r:id="rId63" xr:uid="{165753FE-6E76-4F65-ADB0-3C0598689D9E}"/>
-    <hyperlink ref="F29" r:id="rId64" xr:uid="{EA9CB9A5-1796-45D8-BF72-2FB5DC634265}"/>
-    <hyperlink ref="F30" r:id="rId65" xr:uid="{9684DA43-6441-4294-A859-DB3C97CE1228}"/>
-    <hyperlink ref="F31" r:id="rId66" xr:uid="{DD22E862-92F8-4299-9AA9-DA617D61B8A2}"/>
-    <hyperlink ref="F32" r:id="rId67" xr:uid="{DF6D44AA-94BF-44D3-A48A-3444B463F2F7}"/>
-    <hyperlink ref="F33" r:id="rId68" xr:uid="{DDE009AF-EDFA-4657-A038-49FD7E209F7F}"/>
-    <hyperlink ref="F34" r:id="rId69" xr:uid="{CA703502-E512-4F14-AC28-E29855310BCD}"/>
-    <hyperlink ref="F35" r:id="rId70" xr:uid="{D9959C68-4F76-400F-9A97-25C94CF61DFD}"/>
-    <hyperlink ref="F36" r:id="rId71" xr:uid="{486E112D-6716-40D6-8176-F9350DC19DE4}"/>
-    <hyperlink ref="F37" r:id="rId72" xr:uid="{D45E0FCD-B2AD-4326-922C-866A98C53C36}"/>
-    <hyperlink ref="F38" r:id="rId73" xr:uid="{16CB97F9-4518-4009-A4DE-CEDDD1B75F66}"/>
-    <hyperlink ref="F39" r:id="rId74" xr:uid="{80A390BD-EA40-437C-955B-386CA21755F1}"/>
-    <hyperlink ref="F40" r:id="rId75" xr:uid="{30B58AF3-6257-4AD1-A756-CC04EAA66BA7}"/>
-    <hyperlink ref="F41" r:id="rId76" xr:uid="{0780753F-EF44-4886-B750-3D84C6F27521}"/>
-    <hyperlink ref="F42" r:id="rId77" xr:uid="{E77524E5-DE37-4687-A7EC-E01254B77C04}"/>
-    <hyperlink ref="E20" r:id="rId78" location="Czech" xr:uid="{F2643207-E2F0-4864-BEB2-ECDFD6925BCF}"/>
-    <hyperlink ref="F20" r:id="rId79" xr:uid="{92307C42-E9C2-46CA-92F5-274617250F62}"/>
-    <hyperlink ref="E28" r:id="rId80" location="Czech" xr:uid="{02728391-8C85-4BE4-A57F-696911F17FDA}"/>
-    <hyperlink ref="F28" r:id="rId81" xr:uid="{83DAF3B0-028B-48E8-A7E8-60EFF591CA24}"/>
+    <hyperlink ref="F9" r:id="rId44" xr:uid="{7B281F87-ADD6-4FD2-B8A0-71AC411DA7B0}"/>
+    <hyperlink ref="F10" r:id="rId45" xr:uid="{CAE7D724-F5BC-432B-9C84-0B53AD7455FF}"/>
+    <hyperlink ref="F12" r:id="rId46" xr:uid="{CD565EE9-033A-4565-90A6-30F716071F77}"/>
+    <hyperlink ref="F13" r:id="rId47" xr:uid="{471F5768-0829-4CEF-A522-FA39BA5F5EE2}"/>
+    <hyperlink ref="F15" r:id="rId48" xr:uid="{1FA22728-C587-4A22-9481-9CBCC4E51089}"/>
+    <hyperlink ref="F14" r:id="rId49" xr:uid="{5B137EC4-F81A-4B00-A362-FA8224B889F6}"/>
+    <hyperlink ref="F17" r:id="rId50" xr:uid="{B43A2A52-59D5-4F7A-964E-07F90E0C91DD}"/>
+    <hyperlink ref="F18" r:id="rId51" xr:uid="{7DBFD75F-6275-4085-9EC2-E28F6BA6F2BF}"/>
+    <hyperlink ref="F19" r:id="rId52" xr:uid="{D47388E8-8D39-4137-A17D-3979FFC960DA}"/>
+    <hyperlink ref="F20" r:id="rId53" xr:uid="{BB1F3EF0-32F0-4194-958C-E4C3346408FC}"/>
+    <hyperlink ref="F21" r:id="rId54" xr:uid="{F2DAC8C7-9633-449F-AA57-9516344543A1}"/>
+    <hyperlink ref="F22" r:id="rId55" xr:uid="{7C0D8AB0-3265-4246-81FE-C35CBA4D9DA9}"/>
+    <hyperlink ref="F25" r:id="rId56" xr:uid="{F8C25553-CD78-4C7A-8E01-A614E025CF8A}"/>
+    <hyperlink ref="F23" r:id="rId57" xr:uid="{3B812E5A-F336-459B-B599-05D1B2CC0D25}"/>
+    <hyperlink ref="F26" r:id="rId58" xr:uid="{6C4EC7D6-E3A8-41A0-97C5-26B5D0695873}"/>
+    <hyperlink ref="F27" r:id="rId59" xr:uid="{51BFA554-CEBA-4E7F-A467-DA1DF26DB4B9}"/>
+    <hyperlink ref="F28" r:id="rId60" xr:uid="{EC78ED7F-999D-4C1B-AABC-F94FE5064109}"/>
+    <hyperlink ref="F29" r:id="rId61" xr:uid="{46B1BBB3-F237-4EC9-A0D4-EF7EC84FBF6E}"/>
+    <hyperlink ref="F30" r:id="rId62" xr:uid="{8D683CA9-4AB3-45C0-81CE-58F82581FA95}"/>
+    <hyperlink ref="F31" r:id="rId63" xr:uid="{165753FE-6E76-4F65-ADB0-3C0598689D9E}"/>
+    <hyperlink ref="F33" r:id="rId64" xr:uid="{EA9CB9A5-1796-45D8-BF72-2FB5DC634265}"/>
+    <hyperlink ref="F35" r:id="rId65" xr:uid="{9684DA43-6441-4294-A859-DB3C97CE1228}"/>
+    <hyperlink ref="F36" r:id="rId66" xr:uid="{DD22E862-92F8-4299-9AA9-DA617D61B8A2}"/>
+    <hyperlink ref="F37" r:id="rId67" xr:uid="{DF6D44AA-94BF-44D3-A48A-3444B463F2F7}"/>
+    <hyperlink ref="F38" r:id="rId68" xr:uid="{DDE009AF-EDFA-4657-A038-49FD7E209F7F}"/>
+    <hyperlink ref="F39" r:id="rId69" xr:uid="{CA703502-E512-4F14-AC28-E29855310BCD}"/>
+    <hyperlink ref="F40" r:id="rId70" xr:uid="{D9959C68-4F76-400F-9A97-25C94CF61DFD}"/>
+    <hyperlink ref="F41" r:id="rId71" xr:uid="{486E112D-6716-40D6-8176-F9350DC19DE4}"/>
+    <hyperlink ref="F43" r:id="rId72" xr:uid="{D45E0FCD-B2AD-4326-922C-866A98C53C36}"/>
+    <hyperlink ref="F44" r:id="rId73" xr:uid="{16CB97F9-4518-4009-A4DE-CEDDD1B75F66}"/>
+    <hyperlink ref="F45" r:id="rId74" xr:uid="{80A390BD-EA40-437C-955B-386CA21755F1}"/>
+    <hyperlink ref="F46" r:id="rId75" xr:uid="{30B58AF3-6257-4AD1-A756-CC04EAA66BA7}"/>
+    <hyperlink ref="F48" r:id="rId76" xr:uid="{0780753F-EF44-4886-B750-3D84C6F27521}"/>
+    <hyperlink ref="F49" r:id="rId77" xr:uid="{E77524E5-DE37-4687-A7EC-E01254B77C04}"/>
+    <hyperlink ref="E24" r:id="rId78" location="Czech" xr:uid="{F2643207-E2F0-4864-BEB2-ECDFD6925BCF}"/>
+    <hyperlink ref="F24" r:id="rId79" xr:uid="{92307C42-E9C2-46CA-92F5-274617250F62}"/>
+    <hyperlink ref="E32" r:id="rId80" location="Czech" xr:uid="{02728391-8C85-4BE4-A57F-696911F17FDA}"/>
+    <hyperlink ref="F32" r:id="rId81" xr:uid="{83DAF3B0-028B-48E8-A7E8-60EFF591CA24}"/>
+    <hyperlink ref="E16" r:id="rId82" location="Czech" xr:uid="{199C7183-0C81-4667-81CF-E688B3557B6E}"/>
+    <hyperlink ref="F16" r:id="rId83" xr:uid="{8E474FFE-5719-43F2-910A-55A2E4CF9B41}"/>
+    <hyperlink ref="E11" r:id="rId84" location="Czech" xr:uid="{6ED20886-9230-4036-8DEC-15189BD44817}"/>
+    <hyperlink ref="F11" r:id="rId85" xr:uid="{6D486564-1BEF-4D03-87A8-D95A1EBEF05F}"/>
+    <hyperlink ref="E8" r:id="rId86" location="Czech" xr:uid="{69917D66-5F91-4D56-82D5-9A35B9CDA28F}"/>
+    <hyperlink ref="F8" r:id="rId87" xr:uid="{4EF47456-C668-4274-812A-15C28C1CA2F4}"/>
+    <hyperlink ref="E7" r:id="rId88" location="Czech" xr:uid="{579837A4-600C-4C9F-96E1-7325B1092313}"/>
+    <hyperlink ref="F7" r:id="rId89" xr:uid="{805A349F-6D59-4C54-9634-C1957065889A}"/>
+    <hyperlink ref="E50" r:id="rId90" location="Czech" xr:uid="{226D4B96-35BA-4607-B91E-C98249AE79B7}"/>
+    <hyperlink ref="F50" r:id="rId91" xr:uid="{2CEAE8CD-38C4-485E-8EFF-B33DD1B0C85C}"/>
+    <hyperlink ref="E47" r:id="rId92" location="Czech" xr:uid="{63F4BDD4-1CB9-4741-9D6C-EC28C273BE46}"/>
+    <hyperlink ref="F47" r:id="rId93" xr:uid="{D6E2D60B-1F72-4C84-9439-262304E5416A}"/>
+    <hyperlink ref="E42" r:id="rId94" location="Czech" xr:uid="{7F5181B0-BEBF-4265-8D96-56C86EF17C9C}"/>
+    <hyperlink ref="F42" r:id="rId95" xr:uid="{DAF94A0E-8062-49A4-9B88-013F9EBBA58B}"/>
+    <hyperlink ref="E34" r:id="rId96" location="Czech" xr:uid="{05415563-4B9C-4CC9-9631-66CE94D30199}"/>
+    <hyperlink ref="F34" r:id="rId97" xr:uid="{A1A7E1DE-328E-4B75-B759-271DBFC3420D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId98"/>
 </worksheet>
 </file>
 
@@ -10593,7 +11204,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11148,7 +11759,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11223,145 +11834,145 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>485</v>
+        <v>1463</v>
       </c>
       <c r="B4" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>486</v>
+        <v>1464</v>
       </c>
       <c r="D4" t="s">
-        <v>488</v>
+        <v>1466</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>487</v>
+        <v>1465</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1203</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>664</v>
+        <v>485</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="C5" t="s">
-        <v>661</v>
+        <v>486</v>
       </c>
       <c r="D5" t="s">
-        <v>663</v>
+        <v>488</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>662</v>
+        <v>487</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>478</v>
+        <v>664</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>477</v>
+        <v>661</v>
       </c>
       <c r="D6" t="s">
-        <v>480</v>
+        <v>663</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>479</v>
+        <v>662</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>727</v>
+        <v>478</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>721</v>
+        <v>477</v>
       </c>
       <c r="D7" t="s">
-        <v>721</v>
+        <v>480</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>722</v>
+        <v>479</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1201</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>497</v>
+        <v>727</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>498</v>
+        <v>721</v>
       </c>
       <c r="D8" t="s">
-        <v>500</v>
+        <v>721</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>499</v>
+        <v>722</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1207</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1463</v>
+        <v>497</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>1464</v>
+        <v>498</v>
       </c>
       <c r="D9" t="s">
-        <v>1466</v>
+        <v>500</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1465</v>
+        <v>499</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1467</v>
+        <v>1207</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E8">
-    <sortCondition ref="A1:A8"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F9">
+    <sortCondition ref="A1:A9"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" location="Czech" xr:uid="{D08C6A78-C641-4A04-91FA-7DFC8121E4B1}"/>
-    <hyperlink ref="E6" r:id="rId2" location="Czech" xr:uid="{A9EEB33E-7F18-48EB-A28B-502990CCADD3}"/>
+    <hyperlink ref="E9" r:id="rId1" location="Czech" xr:uid="{D08C6A78-C641-4A04-91FA-7DFC8121E4B1}"/>
+    <hyperlink ref="E7" r:id="rId2" location="Czech" xr:uid="{A9EEB33E-7F18-48EB-A28B-502990CCADD3}"/>
     <hyperlink ref="E3" r:id="rId3" location="Czech" xr:uid="{B1C010BF-968A-42D9-8B9F-DC6405985AF0}"/>
-    <hyperlink ref="E4" r:id="rId4" location="Czech" xr:uid="{C010462B-E1BB-4415-9847-63CA7179E6BC}"/>
-    <hyperlink ref="E5" r:id="rId5" location="Czech" xr:uid="{6DF548CA-49AB-42B8-B810-D35D5B88A660}"/>
-    <hyperlink ref="E7" r:id="rId6" location="Czech" xr:uid="{094E0445-352E-473F-AF01-1051B531E551}"/>
+    <hyperlink ref="E5" r:id="rId4" location="Czech" xr:uid="{C010462B-E1BB-4415-9847-63CA7179E6BC}"/>
+    <hyperlink ref="E6" r:id="rId5" location="Czech" xr:uid="{6DF548CA-49AB-42B8-B810-D35D5B88A660}"/>
+    <hyperlink ref="E8" r:id="rId6" location="Czech" xr:uid="{094E0445-352E-473F-AF01-1051B531E551}"/>
     <hyperlink ref="E2" r:id="rId7" location="Czech" xr:uid="{36E6D160-7B61-4284-94EE-00272F0A46B5}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{1F83B336-51E2-4FED-8DE9-E7D6C121589D}"/>
+    <hyperlink ref="F8" r:id="rId8" xr:uid="{1F83B336-51E2-4FED-8DE9-E7D6C121589D}"/>
     <hyperlink ref="F3" r:id="rId9" xr:uid="{2F59FFE9-B0A1-44DF-A78C-201478508AFC}"/>
-    <hyperlink ref="F4" r:id="rId10" xr:uid="{4D8C4A2C-F138-4F58-9364-F9CD1EEB58B1}"/>
-    <hyperlink ref="F5" r:id="rId11" xr:uid="{4094A667-8753-49EC-9242-82EF2076EE31}"/>
-    <hyperlink ref="F6" r:id="rId12" xr:uid="{33E68306-1EDC-4E9F-94B0-5DC437EB5A56}"/>
+    <hyperlink ref="F5" r:id="rId10" xr:uid="{4D8C4A2C-F138-4F58-9364-F9CD1EEB58B1}"/>
+    <hyperlink ref="F6" r:id="rId11" xr:uid="{4094A667-8753-49EC-9242-82EF2076EE31}"/>
+    <hyperlink ref="F7" r:id="rId12" xr:uid="{33E68306-1EDC-4E9F-94B0-5DC437EB5A56}"/>
     <hyperlink ref="F2" r:id="rId13" xr:uid="{071524E1-1C12-4C13-BB42-DD6D4DAF49F2}"/>
-    <hyperlink ref="F8" r:id="rId14" xr:uid="{93AB0901-4009-4007-BF5C-1EE76F33C63F}"/>
-    <hyperlink ref="E9" r:id="rId15" location="Czech" xr:uid="{714E1DAF-CA55-48AB-9437-81F3ED4FAACE}"/>
-    <hyperlink ref="F9" r:id="rId16" xr:uid="{F4FCE0FE-8F33-4C96-9E7E-D73A4210D429}"/>
+    <hyperlink ref="F9" r:id="rId14" xr:uid="{93AB0901-4009-4007-BF5C-1EE76F33C63F}"/>
+    <hyperlink ref="E4" r:id="rId15" location="Czech" xr:uid="{714E1DAF-CA55-48AB-9437-81F3ED4FAACE}"/>
+    <hyperlink ref="F4" r:id="rId16" xr:uid="{F4FCE0FE-8F33-4C96-9E7E-D73A4210D429}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11371,7 +11982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3081E238-0A75-4CCA-BCD2-D049DAB6C4FD}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
@@ -12804,10 +13415,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCD7ADF-A934-4B8C-90F5-000C68281CBC}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13102,840 +13713,860 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>766</v>
+        <v>1657</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>764</v>
+        <v>1659</v>
       </c>
       <c r="D15" t="s">
-        <v>764</v>
+        <v>1660</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>765</v>
+        <v>1658</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1287</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>850</v>
+        <v>766</v>
       </c>
       <c r="B16" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>851</v>
+        <v>764</v>
       </c>
       <c r="D16" t="s">
-        <v>853</v>
+        <v>764</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>852</v>
+        <v>765</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>803</v>
+        <v>850</v>
       </c>
       <c r="B17" t="s">
         <v>263</v>
       </c>
       <c r="C17" t="s">
-        <v>802</v>
+        <v>851</v>
       </c>
       <c r="D17" t="s">
-        <v>805</v>
+        <v>853</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>804</v>
+        <v>852</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>866</v>
+        <v>803</v>
       </c>
       <c r="B18" t="s">
         <v>263</v>
       </c>
       <c r="C18" t="s">
-        <v>863</v>
+        <v>802</v>
       </c>
       <c r="D18" t="s">
-        <v>864</v>
+        <v>805</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>865</v>
+        <v>804</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1100</v>
+        <v>866</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C19" t="s">
-        <v>1102</v>
+        <v>863</v>
       </c>
       <c r="D19" t="s">
-        <v>1102</v>
+        <v>864</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>1101</v>
+        <v>865</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>750</v>
+        <v>1100</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>751</v>
+        <v>1102</v>
       </c>
       <c r="D20" t="s">
-        <v>752</v>
+        <v>1102</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>749</v>
+        <v>1101</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>792</v>
+        <v>750</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>793</v>
+        <v>751</v>
       </c>
       <c r="D21" t="s">
-        <v>794</v>
+        <v>752</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>791</v>
+        <v>749</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>841</v>
+        <v>792</v>
       </c>
       <c r="B22" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>839</v>
+        <v>793</v>
       </c>
       <c r="D22" t="s">
-        <v>840</v>
+        <v>794</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>838</v>
+        <v>791</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>835</v>
+        <v>841</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C23" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="D23" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>780</v>
+        <v>835</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>779</v>
+        <v>834</v>
       </c>
       <c r="D24" t="s">
-        <v>782</v>
+        <v>837</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>781</v>
+        <v>836</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>799</v>
+        <v>780</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>798</v>
+        <v>779</v>
       </c>
       <c r="D25" t="s">
-        <v>801</v>
+        <v>782</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>800</v>
+        <v>781</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>731</v>
+        <v>799</v>
       </c>
       <c r="B26" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>729</v>
+        <v>798</v>
       </c>
       <c r="D26" t="s">
-        <v>730</v>
+        <v>801</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>728</v>
+        <v>800</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>261</v>
+        <v>731</v>
       </c>
       <c r="B27" t="s">
         <v>263</v>
       </c>
       <c r="C27" t="s">
-        <v>262</v>
+        <v>729</v>
       </c>
       <c r="D27" t="s">
-        <v>264</v>
+        <v>730</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>265</v>
+        <v>728</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>909</v>
+        <v>261</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C28" t="s">
-        <v>910</v>
+        <v>262</v>
       </c>
       <c r="D28" t="s">
-        <v>910</v>
+        <v>264</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>911</v>
+        <v>265</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>734</v>
+        <v>909</v>
       </c>
       <c r="B29" t="s">
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>733</v>
+        <v>910</v>
       </c>
       <c r="D29" t="s">
-        <v>733</v>
+        <v>910</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>732</v>
+        <v>911</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>788</v>
+        <v>734</v>
       </c>
       <c r="B30" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>787</v>
+        <v>733</v>
       </c>
       <c r="D30" t="s">
-        <v>790</v>
+        <v>733</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>789</v>
+        <v>732</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>856</v>
+        <v>788</v>
       </c>
       <c r="B31" t="s">
         <v>263</v>
       </c>
       <c r="C31" t="s">
-        <v>854</v>
+        <v>787</v>
       </c>
       <c r="D31" t="s">
-        <v>855</v>
+        <v>790</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>857</v>
+        <v>789</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>831</v>
+        <v>856</v>
       </c>
       <c r="B32" t="s">
         <v>263</v>
       </c>
       <c r="C32" t="s">
-        <v>830</v>
+        <v>854</v>
       </c>
       <c r="D32" t="s">
-        <v>833</v>
+        <v>855</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>832</v>
+        <v>857</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>847</v>
+        <v>831</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C33" t="s">
-        <v>846</v>
+        <v>830</v>
       </c>
       <c r="D33" t="s">
-        <v>849</v>
+        <v>833</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>848</v>
+        <v>832</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>825</v>
+        <v>847</v>
       </c>
       <c r="B34" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>826</v>
+        <v>846</v>
       </c>
       <c r="D34" t="s">
-        <v>828</v>
+        <v>849</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>827</v>
+        <v>848</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>862</v>
+        <v>825</v>
       </c>
       <c r="B35" t="s">
         <v>263</v>
       </c>
       <c r="C35" t="s">
-        <v>863</v>
+        <v>826</v>
       </c>
       <c r="D35" t="s">
-        <v>864</v>
+        <v>828</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>865</v>
+        <v>827</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>784</v>
+        <v>862</v>
       </c>
       <c r="B36" t="s">
         <v>263</v>
       </c>
       <c r="C36" t="s">
-        <v>783</v>
+        <v>863</v>
       </c>
       <c r="D36" t="s">
-        <v>786</v>
+        <v>864</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>785</v>
+        <v>865</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>843</v>
+        <v>784</v>
       </c>
       <c r="B37" t="s">
         <v>263</v>
       </c>
       <c r="C37" t="s">
-        <v>842</v>
+        <v>783</v>
       </c>
       <c r="D37" t="s">
-        <v>845</v>
+        <v>786</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>844</v>
+        <v>785</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>870</v>
+        <v>843</v>
       </c>
       <c r="B38" t="s">
         <v>263</v>
       </c>
       <c r="C38" t="s">
-        <v>868</v>
+        <v>842</v>
       </c>
       <c r="D38" t="s">
-        <v>869</v>
+        <v>845</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>867</v>
+        <v>844</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>888</v>
+        <v>870</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="C39" t="s">
-        <v>887</v>
+        <v>868</v>
       </c>
       <c r="D39" t="s">
-        <v>890</v>
+        <v>869</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>889</v>
+        <v>867</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>746</v>
+        <v>888</v>
       </c>
       <c r="B40" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>745</v>
+        <v>887</v>
       </c>
       <c r="D40" t="s">
-        <v>747</v>
+        <v>890</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>748</v>
+        <v>889</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>772</v>
+        <v>746</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C41" t="s">
-        <v>771</v>
+        <v>745</v>
       </c>
       <c r="D41" t="s">
-        <v>774</v>
+        <v>747</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>773</v>
+        <v>748</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>893</v>
+        <v>772</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>891</v>
+        <v>771</v>
       </c>
       <c r="D42" t="s">
-        <v>894</v>
+        <v>774</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>892</v>
+        <v>773</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>761</v>
+        <v>893</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>760</v>
+        <v>891</v>
       </c>
       <c r="D43" t="s">
-        <v>763</v>
+        <v>894</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>762</v>
+        <v>892</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>795</v>
+        <v>1530</v>
       </c>
       <c r="B44" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>796</v>
+        <v>1532</v>
       </c>
       <c r="D44" t="s">
-        <v>796</v>
+        <v>1533</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>797</v>
+        <v>1531</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1316</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>744</v>
+        <v>761</v>
       </c>
       <c r="B45" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C45" t="s">
-        <v>742</v>
+        <v>760</v>
       </c>
       <c r="D45" t="s">
-        <v>742</v>
+        <v>763</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>743</v>
+        <v>762</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>776</v>
+        <v>795</v>
       </c>
       <c r="B46" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
-        <v>775</v>
+        <v>796</v>
       </c>
       <c r="D46" t="s">
-        <v>778</v>
+        <v>796</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>777</v>
+        <v>797</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>755</v>
+        <v>744</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>753</v>
+        <v>742</v>
       </c>
       <c r="D47" t="s">
-        <v>753</v>
+        <v>742</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>754</v>
+        <v>743</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C48" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
       <c r="D48" t="s">
-        <v>770</v>
+        <v>778</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>769</v>
+        <v>777</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>875</v>
+        <v>755</v>
       </c>
       <c r="B49" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>877</v>
+        <v>753</v>
       </c>
       <c r="D49" t="s">
-        <v>878</v>
+        <v>753</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>876</v>
+        <v>754</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>895</v>
+        <v>767</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>896</v>
+        <v>768</v>
       </c>
       <c r="D50" t="s">
-        <v>897</v>
+        <v>770</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>898</v>
+        <v>769</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="B51" t="s">
         <v>263</v>
       </c>
       <c r="C51" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
       <c r="D51" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>822</v>
+        <v>895</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C52" t="s">
-        <v>821</v>
+        <v>896</v>
       </c>
       <c r="D52" t="s">
-        <v>824</v>
+        <v>897</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>823</v>
+        <v>898</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1530</v>
+        <v>879</v>
       </c>
       <c r="B53" t="s">
+        <v>263</v>
+      </c>
+      <c r="C53" t="s">
+        <v>880</v>
+      </c>
+      <c r="D53" t="s">
+        <v>881</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>822</v>
+      </c>
+      <c r="B54" t="s">
         <v>27</v>
       </c>
-      <c r="C53" t="s">
-        <v>1532</v>
-      </c>
-      <c r="D53" t="s">
-        <v>1533</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>1531</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>1534</v>
+      <c r="C54" t="s">
+        <v>821</v>
+      </c>
+      <c r="D54" t="s">
+        <v>824</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>1324</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E52">
-    <sortCondition ref="A1:A52"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F54">
+    <sortCondition ref="A1:A54"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E27" r:id="rId1" location="Czech" xr:uid="{42D57DF4-42EF-42C1-AE8D-7AB606A19039}"/>
-    <hyperlink ref="E26" r:id="rId2" location="Czech" xr:uid="{93C6135E-76B5-4B09-98A2-42C47FB73DDC}"/>
-    <hyperlink ref="E29" r:id="rId3" location="Czech" xr:uid="{44A0C2AB-9696-48DA-97D4-F3A388641802}"/>
+    <hyperlink ref="E28" r:id="rId1" location="Czech" xr:uid="{42D57DF4-42EF-42C1-AE8D-7AB606A19039}"/>
+    <hyperlink ref="E27" r:id="rId2" location="Czech" xr:uid="{93C6135E-76B5-4B09-98A2-42C47FB73DDC}"/>
+    <hyperlink ref="E30" r:id="rId3" location="Czech" xr:uid="{44A0C2AB-9696-48DA-97D4-F3A388641802}"/>
     <hyperlink ref="E4" r:id="rId4" location="Czech" xr:uid="{7F571370-4E97-4C6F-83FF-A3B7E8A02DF7}"/>
     <hyperlink ref="E6" r:id="rId5" location="Czech" xr:uid="{301CD7C2-871E-4DF9-84B5-8E013577F084}"/>
-    <hyperlink ref="E45" r:id="rId6" location="Czech" xr:uid="{6C0E5A39-7B2B-44B5-A4AB-9124B80E365B}"/>
-    <hyperlink ref="E40" r:id="rId7" location="Czech" xr:uid="{C94E10F0-2FD4-43DA-AF43-2D9B52F183FD}"/>
-    <hyperlink ref="E20" r:id="rId8" location="Czech" xr:uid="{7562CF4F-3B2A-4649-891A-3C06E4FFC1B0}"/>
-    <hyperlink ref="E47" r:id="rId9" location="Czech" xr:uid="{4A4F43AC-3EEE-4254-AE7D-B9D28EA0C45F}"/>
+    <hyperlink ref="E47" r:id="rId6" location="Czech" xr:uid="{6C0E5A39-7B2B-44B5-A4AB-9124B80E365B}"/>
+    <hyperlink ref="E41" r:id="rId7" location="Czech" xr:uid="{C94E10F0-2FD4-43DA-AF43-2D9B52F183FD}"/>
+    <hyperlink ref="E21" r:id="rId8" location="Czech" xr:uid="{7562CF4F-3B2A-4649-891A-3C06E4FFC1B0}"/>
+    <hyperlink ref="E49" r:id="rId9" location="Czech" xr:uid="{4A4F43AC-3EEE-4254-AE7D-B9D28EA0C45F}"/>
     <hyperlink ref="E5" r:id="rId10" location="Czech" xr:uid="{788C0762-B3BB-4E83-885B-FD0617400C40}"/>
-    <hyperlink ref="E43" r:id="rId11" location="Czech" xr:uid="{02250CBB-AC5B-4E2A-9D63-10F060103603}"/>
-    <hyperlink ref="E15" r:id="rId12" location="Czech" xr:uid="{D641E7BD-D07F-4945-ACD0-270B0EF147FE}"/>
-    <hyperlink ref="E48" r:id="rId13" location="Czech" xr:uid="{96488995-F82D-4496-BCDE-21EC6E31B965}"/>
-    <hyperlink ref="E41" r:id="rId14" location="Czech" xr:uid="{7CE572C9-3864-4892-B1E7-D4C27E724B07}"/>
-    <hyperlink ref="E46" r:id="rId15" location="Czech" xr:uid="{448134AE-AFBB-420A-9C63-66606DBEE629}"/>
-    <hyperlink ref="E24" r:id="rId16" location="Czech" xr:uid="{81520B5E-B841-4B8F-9E8D-7B0DF45F12F4}"/>
-    <hyperlink ref="E36" r:id="rId17" location="Czech" xr:uid="{10E22225-EF52-488D-B6B5-625DB308957B}"/>
-    <hyperlink ref="E30" r:id="rId18" location="Czech" xr:uid="{9273397B-F045-4516-95BA-D02CBCC17A15}"/>
-    <hyperlink ref="E21" r:id="rId19" location="Czech" xr:uid="{EF9FA079-F46B-49B9-A28C-4CC94CDCF960}"/>
-    <hyperlink ref="E44" r:id="rId20" location="Czech" xr:uid="{28137938-693A-411B-9E2E-7840055BFC87}"/>
-    <hyperlink ref="E25" r:id="rId21" location="Czech" xr:uid="{00CC9396-8D10-4ECC-90FE-EA373B644027}"/>
-    <hyperlink ref="E17" r:id="rId22" location="Czech" xr:uid="{FEE6E685-A4FF-4713-9FF4-D4BC3272C7A5}"/>
+    <hyperlink ref="E45" r:id="rId11" location="Czech" xr:uid="{02250CBB-AC5B-4E2A-9D63-10F060103603}"/>
+    <hyperlink ref="E16" r:id="rId12" location="Czech" xr:uid="{D641E7BD-D07F-4945-ACD0-270B0EF147FE}"/>
+    <hyperlink ref="E50" r:id="rId13" location="Czech" xr:uid="{96488995-F82D-4496-BCDE-21EC6E31B965}"/>
+    <hyperlink ref="E42" r:id="rId14" location="Czech" xr:uid="{7CE572C9-3864-4892-B1E7-D4C27E724B07}"/>
+    <hyperlink ref="E48" r:id="rId15" location="Czech" xr:uid="{448134AE-AFBB-420A-9C63-66606DBEE629}"/>
+    <hyperlink ref="E25" r:id="rId16" location="Czech" xr:uid="{81520B5E-B841-4B8F-9E8D-7B0DF45F12F4}"/>
+    <hyperlink ref="E37" r:id="rId17" location="Czech" xr:uid="{10E22225-EF52-488D-B6B5-625DB308957B}"/>
+    <hyperlink ref="E31" r:id="rId18" location="Czech" xr:uid="{9273397B-F045-4516-95BA-D02CBCC17A15}"/>
+    <hyperlink ref="E22" r:id="rId19" location="Czech" xr:uid="{EF9FA079-F46B-49B9-A28C-4CC94CDCF960}"/>
+    <hyperlink ref="E46" r:id="rId20" location="Czech" xr:uid="{28137938-693A-411B-9E2E-7840055BFC87}"/>
+    <hyperlink ref="E26" r:id="rId21" location="Czech" xr:uid="{00CC9396-8D10-4ECC-90FE-EA373B644027}"/>
+    <hyperlink ref="E18" r:id="rId22" location="Czech" xr:uid="{FEE6E685-A4FF-4713-9FF4-D4BC3272C7A5}"/>
     <hyperlink ref="E11" r:id="rId23" location="Czech" xr:uid="{A3F9512D-CC56-4C3D-B405-0B61E035F2A2}"/>
     <hyperlink ref="E9" r:id="rId24" location="Czech" xr:uid="{2ECADC02-A521-4C1C-B055-B126B4BF45B3}"/>
-    <hyperlink ref="E52" r:id="rId25" location="Czech" xr:uid="{002F46B9-2313-43E5-AE80-41B1037D8F94}"/>
-    <hyperlink ref="E34" r:id="rId26" location="Czech" xr:uid="{7C11BBFB-34AC-40E0-8F30-E7B00E8504B1}"/>
+    <hyperlink ref="E54" r:id="rId25" location="Czech" xr:uid="{002F46B9-2313-43E5-AE80-41B1037D8F94}"/>
+    <hyperlink ref="E35" r:id="rId26" location="Czech" xr:uid="{7C11BBFB-34AC-40E0-8F30-E7B00E8504B1}"/>
     <hyperlink ref="E10" r:id="rId27" location="Czech" xr:uid="{E7B528EA-B4E6-4653-B978-63CBF121DA50}"/>
-    <hyperlink ref="E32" r:id="rId28" location="Czech" xr:uid="{DC6886CB-9B73-4CEA-B706-16DE84B570C9}"/>
-    <hyperlink ref="E23" r:id="rId29" location="Czech" xr:uid="{FC905C12-13F8-4882-99A4-BCEEA6F66C20}"/>
-    <hyperlink ref="E22" r:id="rId30" location="Czech" xr:uid="{9AF7662F-BC09-40F7-9A7F-286BF850CC88}"/>
-    <hyperlink ref="E37" r:id="rId31" location="Czech" xr:uid="{8FE8743F-1AFC-4A19-B244-FB2B01073DF5}"/>
-    <hyperlink ref="E33" r:id="rId32" location="Czech" xr:uid="{53EA3C45-A4B0-438A-AAC6-386775DA1300}"/>
-    <hyperlink ref="E16" r:id="rId33" location="Czech" xr:uid="{1F3D3165-59B4-4006-B26B-6D3756A38401}"/>
-    <hyperlink ref="E31" r:id="rId34" location="Czech" xr:uid="{40FBB35D-5E7D-4DDC-AD4E-7D6C060E51FB}"/>
+    <hyperlink ref="E33" r:id="rId28" location="Czech" xr:uid="{DC6886CB-9B73-4CEA-B706-16DE84B570C9}"/>
+    <hyperlink ref="E24" r:id="rId29" location="Czech" xr:uid="{FC905C12-13F8-4882-99A4-BCEEA6F66C20}"/>
+    <hyperlink ref="E23" r:id="rId30" location="Czech" xr:uid="{9AF7662F-BC09-40F7-9A7F-286BF850CC88}"/>
+    <hyperlink ref="E38" r:id="rId31" location="Czech" xr:uid="{8FE8743F-1AFC-4A19-B244-FB2B01073DF5}"/>
+    <hyperlink ref="E34" r:id="rId32" location="Czech" xr:uid="{53EA3C45-A4B0-438A-AAC6-386775DA1300}"/>
+    <hyperlink ref="E17" r:id="rId33" location="Czech" xr:uid="{1F3D3165-59B4-4006-B26B-6D3756A38401}"/>
+    <hyperlink ref="E32" r:id="rId34" location="Czech" xr:uid="{40FBB35D-5E7D-4DDC-AD4E-7D6C060E51FB}"/>
     <hyperlink ref="E7" r:id="rId35" location="Czech" xr:uid="{134B72CC-A9C7-41E4-AA73-3D3D754972B2}"/>
-    <hyperlink ref="E35" r:id="rId36" location="Czech" xr:uid="{B1FD1B6C-F427-4B2F-8363-837841828F43}"/>
-    <hyperlink ref="E18" r:id="rId37" location="Czech" xr:uid="{0E56D775-C75B-41DC-9F85-21CB10C1C081}"/>
-    <hyperlink ref="E38" r:id="rId38" location="Czech" xr:uid="{6F14A934-1E91-44DB-85DD-E21F9ACC6B2B}"/>
+    <hyperlink ref="E36" r:id="rId36" location="Czech" xr:uid="{B1FD1B6C-F427-4B2F-8363-837841828F43}"/>
+    <hyperlink ref="E19" r:id="rId37" location="Czech" xr:uid="{0E56D775-C75B-41DC-9F85-21CB10C1C081}"/>
+    <hyperlink ref="E39" r:id="rId38" location="Czech" xr:uid="{6F14A934-1E91-44DB-85DD-E21F9ACC6B2B}"/>
     <hyperlink ref="E14" r:id="rId39" location="Czech" xr:uid="{1599E9F5-072E-4A66-BBBF-44B744901DF5}"/>
-    <hyperlink ref="E49" r:id="rId40" location="Czech" xr:uid="{2BDA3736-BC83-4C6F-83F0-3322ED9B553A}"/>
-    <hyperlink ref="E51" r:id="rId41" location="Czech" xr:uid="{F53E68A0-237B-41BB-9960-B6650B8BA9E1}"/>
+    <hyperlink ref="E51" r:id="rId40" location="Czech" xr:uid="{2BDA3736-BC83-4C6F-83F0-3322ED9B553A}"/>
+    <hyperlink ref="E53" r:id="rId41" location="Czech" xr:uid="{F53E68A0-237B-41BB-9960-B6650B8BA9E1}"/>
     <hyperlink ref="E13" r:id="rId42" location="Czech" xr:uid="{4B2D7682-0A49-4CAC-988F-3E4E3A727D27}"/>
-    <hyperlink ref="E39" r:id="rId43" location="Czech" xr:uid="{B54C2F11-3995-44B8-B3BB-71CEA61766BF}"/>
-    <hyperlink ref="E42" r:id="rId44" location="Czech" xr:uid="{01A10AB9-B97C-466B-8E4C-577380F4C429}"/>
-    <hyperlink ref="E50" r:id="rId45" location="Czech" xr:uid="{A5124C8A-8893-4235-BD34-43A266E1073F}"/>
+    <hyperlink ref="E40" r:id="rId43" location="Czech" xr:uid="{B54C2F11-3995-44B8-B3BB-71CEA61766BF}"/>
+    <hyperlink ref="E43" r:id="rId44" location="Czech" xr:uid="{01A10AB9-B97C-466B-8E4C-577380F4C429}"/>
+    <hyperlink ref="E52" r:id="rId45" location="Czech" xr:uid="{A5124C8A-8893-4235-BD34-43A266E1073F}"/>
     <hyperlink ref="E12" r:id="rId46" location="Czech" xr:uid="{A33D02F7-F80E-4950-8345-39720EB31504}"/>
     <hyperlink ref="E2" r:id="rId47" location="Czech" xr:uid="{9AE5B971-FD6C-4B38-BD09-1D14C9221B85}"/>
     <hyperlink ref="E3" r:id="rId48" location="Czech" xr:uid="{5CB57FF0-FD6C-4B97-ABB0-85343D101768}"/>
-    <hyperlink ref="E28" r:id="rId49" location="Czech" xr:uid="{D4152F8D-8835-4CDB-98F1-C09C729A36DE}"/>
+    <hyperlink ref="E29" r:id="rId49" location="Czech" xr:uid="{D4152F8D-8835-4CDB-98F1-C09C729A36DE}"/>
     <hyperlink ref="E8" r:id="rId50" location="Czech" xr:uid="{91C31CEF-ED20-40A5-A4BF-8EAF8CEB0CB0}"/>
-    <hyperlink ref="E19" r:id="rId51" location="Czech" xr:uid="{24B8314C-7FAE-42FF-B32D-DAC3650E5711}"/>
+    <hyperlink ref="E20" r:id="rId51" location="Czech" xr:uid="{24B8314C-7FAE-42FF-B32D-DAC3650E5711}"/>
     <hyperlink ref="F2" r:id="rId52" xr:uid="{7349BF2A-1CF9-4FF7-8640-A10ECC7F16B0}"/>
     <hyperlink ref="F3" r:id="rId53" xr:uid="{A228D250-AC84-40A7-BCE4-9A9427BE1DE8}"/>
     <hyperlink ref="F4" r:id="rId54" xr:uid="{39DACC5D-8CFB-4B06-8F42-130804F1C6B0}"/>
@@ -13949,48 +14580,50 @@
     <hyperlink ref="F12" r:id="rId62" xr:uid="{3C3B54B6-3EDD-434F-B389-64FDC3EA1114}"/>
     <hyperlink ref="F13" r:id="rId63" xr:uid="{E1C3A8AE-7DCB-434E-9A5C-089718B0AEB1}"/>
     <hyperlink ref="F14" r:id="rId64" xr:uid="{50DEA5C8-F208-410C-8CB0-123632AF6BC2}"/>
-    <hyperlink ref="F15" r:id="rId65" xr:uid="{550426CA-719B-45B2-88C4-1487B1CA4020}"/>
-    <hyperlink ref="F16" r:id="rId66" xr:uid="{94C81662-9F67-4D7A-87AF-7ADF5AA7461B}"/>
-    <hyperlink ref="F17" r:id="rId67" xr:uid="{F0A11E35-3665-4E8F-B426-5EC2C938B0D1}"/>
-    <hyperlink ref="F18" r:id="rId68" xr:uid="{DF5891BE-136F-4B94-8ACA-CE06A2C21F7E}"/>
-    <hyperlink ref="F19" r:id="rId69" xr:uid="{A3C374D8-9359-4072-9CE2-F1414CA109DC}"/>
-    <hyperlink ref="F20" r:id="rId70" xr:uid="{8359BD25-F9A7-47CC-BE7F-E89B59F4E93B}"/>
-    <hyperlink ref="F21" r:id="rId71" xr:uid="{6C0201F9-712F-4713-8762-6115989E9D13}"/>
-    <hyperlink ref="F22" r:id="rId72" xr:uid="{4BF0A2FD-F6B7-48BB-A460-C7DC46CFC1C5}"/>
-    <hyperlink ref="F23" r:id="rId73" xr:uid="{7FD8380E-8438-4D86-9D2E-CD53171EBFE8}"/>
-    <hyperlink ref="F24" r:id="rId74" xr:uid="{7B87A74E-466D-439B-A756-7856E1BAAA88}"/>
-    <hyperlink ref="F25" r:id="rId75" xr:uid="{029D39CC-C1F2-4676-925B-7AD757C113AA}"/>
-    <hyperlink ref="F26" r:id="rId76" xr:uid="{B470E4C6-2592-462A-83F5-7D2A21C010A6}"/>
-    <hyperlink ref="F27" r:id="rId77" xr:uid="{7FD5E37D-33EC-4F4D-85D1-73D01754D068}"/>
-    <hyperlink ref="F28" r:id="rId78" xr:uid="{DFF521E5-6715-4C29-B30D-FD07F9852A0E}"/>
-    <hyperlink ref="F29" r:id="rId79" xr:uid="{6BAA2C7E-CFD3-4573-89CC-C44FD3246C80}"/>
-    <hyperlink ref="F30" r:id="rId80" xr:uid="{07B2DBF1-06BA-40D7-89FB-E174922671C2}"/>
-    <hyperlink ref="F31" r:id="rId81" xr:uid="{B7DC757A-BD71-48A1-B5CC-34BB0CDCCFF2}"/>
-    <hyperlink ref="F32" r:id="rId82" xr:uid="{74B6CD93-93DD-450B-BA99-CB541EBD2E7A}"/>
-    <hyperlink ref="F33" r:id="rId83" xr:uid="{4983453D-9F5D-45CB-8E8E-28DF2E8D9B56}"/>
-    <hyperlink ref="F34" r:id="rId84" xr:uid="{CB410BC5-2FB2-4C84-9E77-417F992B8CB2}"/>
-    <hyperlink ref="F35" r:id="rId85" xr:uid="{9DF6E28D-D72F-40A8-9FF3-680188943407}"/>
-    <hyperlink ref="F36" r:id="rId86" xr:uid="{71B6C3AF-B08D-441C-8F51-C57879F811B9}"/>
-    <hyperlink ref="F37" r:id="rId87" xr:uid="{B3B3FE99-020D-4B39-986C-E67308C59942}"/>
-    <hyperlink ref="F38" r:id="rId88" xr:uid="{BE62AF36-7AA6-4406-AFF8-9F3115F21F55}"/>
-    <hyperlink ref="F39" r:id="rId89" xr:uid="{F25BE1B9-1510-441A-AAFA-DF6891FF8B05}"/>
-    <hyperlink ref="F40" r:id="rId90" xr:uid="{11F96174-8B3C-4613-85E9-350625C89D71}"/>
-    <hyperlink ref="F41" r:id="rId91" xr:uid="{C7F3DFE2-6162-40CE-B017-111E00CFAD88}"/>
-    <hyperlink ref="F42" r:id="rId92" xr:uid="{B26C47F5-95B0-4CC6-B7C5-0FE5DE9F1D48}"/>
-    <hyperlink ref="F43" r:id="rId93" xr:uid="{E7E699D9-2D8A-4D90-95AE-279E34EA3635}"/>
-    <hyperlink ref="F44" r:id="rId94" xr:uid="{EA0D98A0-8359-4E91-B63A-C1C396B4852D}"/>
-    <hyperlink ref="F45" r:id="rId95" xr:uid="{34320072-4E10-45E9-8D5D-BF9565901E63}"/>
-    <hyperlink ref="F46" r:id="rId96" xr:uid="{71EEB8E7-415C-491D-ACDA-28BD6EC8DAB9}"/>
-    <hyperlink ref="F47" r:id="rId97" xr:uid="{F981C0FD-B38B-4960-8DBB-EC5EA32CA8E4}"/>
-    <hyperlink ref="F48" r:id="rId98" xr:uid="{CC47B797-0670-4FF9-AD9A-4358EB33B930}"/>
-    <hyperlink ref="F49" r:id="rId99" xr:uid="{F7B96616-D53A-4F58-B521-274BFA3DE2D4}"/>
-    <hyperlink ref="F50" r:id="rId100" xr:uid="{C5E1A3DC-4A02-46E5-B64F-3CBD1622553F}"/>
-    <hyperlink ref="F51" r:id="rId101" xr:uid="{1B3B5741-7720-4623-B744-D0AB9868A3BE}"/>
-    <hyperlink ref="F52" r:id="rId102" xr:uid="{BCB4D44C-B26F-4521-A900-DE2BFF96C039}"/>
-    <hyperlink ref="E53" r:id="rId103" location="Czech" xr:uid="{7F9BF6E5-10D6-4AB2-B055-BFE1534EF9EA}"/>
-    <hyperlink ref="F53" r:id="rId104" xr:uid="{F1E6A50C-E7E7-4374-88E6-E7BA966011B4}"/>
+    <hyperlink ref="F16" r:id="rId65" xr:uid="{550426CA-719B-45B2-88C4-1487B1CA4020}"/>
+    <hyperlink ref="F17" r:id="rId66" xr:uid="{94C81662-9F67-4D7A-87AF-7ADF5AA7461B}"/>
+    <hyperlink ref="F18" r:id="rId67" xr:uid="{F0A11E35-3665-4E8F-B426-5EC2C938B0D1}"/>
+    <hyperlink ref="F19" r:id="rId68" xr:uid="{DF5891BE-136F-4B94-8ACA-CE06A2C21F7E}"/>
+    <hyperlink ref="F20" r:id="rId69" xr:uid="{A3C374D8-9359-4072-9CE2-F1414CA109DC}"/>
+    <hyperlink ref="F21" r:id="rId70" xr:uid="{8359BD25-F9A7-47CC-BE7F-E89B59F4E93B}"/>
+    <hyperlink ref="F22" r:id="rId71" xr:uid="{6C0201F9-712F-4713-8762-6115989E9D13}"/>
+    <hyperlink ref="F23" r:id="rId72" xr:uid="{4BF0A2FD-F6B7-48BB-A460-C7DC46CFC1C5}"/>
+    <hyperlink ref="F24" r:id="rId73" xr:uid="{7FD8380E-8438-4D86-9D2E-CD53171EBFE8}"/>
+    <hyperlink ref="F25" r:id="rId74" xr:uid="{7B87A74E-466D-439B-A756-7856E1BAAA88}"/>
+    <hyperlink ref="F26" r:id="rId75" xr:uid="{029D39CC-C1F2-4676-925B-7AD757C113AA}"/>
+    <hyperlink ref="F27" r:id="rId76" xr:uid="{B470E4C6-2592-462A-83F5-7D2A21C010A6}"/>
+    <hyperlink ref="F28" r:id="rId77" xr:uid="{7FD5E37D-33EC-4F4D-85D1-73D01754D068}"/>
+    <hyperlink ref="F29" r:id="rId78" xr:uid="{DFF521E5-6715-4C29-B30D-FD07F9852A0E}"/>
+    <hyperlink ref="F30" r:id="rId79" xr:uid="{6BAA2C7E-CFD3-4573-89CC-C44FD3246C80}"/>
+    <hyperlink ref="F31" r:id="rId80" xr:uid="{07B2DBF1-06BA-40D7-89FB-E174922671C2}"/>
+    <hyperlink ref="F32" r:id="rId81" xr:uid="{B7DC757A-BD71-48A1-B5CC-34BB0CDCCFF2}"/>
+    <hyperlink ref="F33" r:id="rId82" xr:uid="{74B6CD93-93DD-450B-BA99-CB541EBD2E7A}"/>
+    <hyperlink ref="F34" r:id="rId83" xr:uid="{4983453D-9F5D-45CB-8E8E-28DF2E8D9B56}"/>
+    <hyperlink ref="F35" r:id="rId84" xr:uid="{CB410BC5-2FB2-4C84-9E77-417F992B8CB2}"/>
+    <hyperlink ref="F36" r:id="rId85" xr:uid="{9DF6E28D-D72F-40A8-9FF3-680188943407}"/>
+    <hyperlink ref="F37" r:id="rId86" xr:uid="{71B6C3AF-B08D-441C-8F51-C57879F811B9}"/>
+    <hyperlink ref="F38" r:id="rId87" xr:uid="{B3B3FE99-020D-4B39-986C-E67308C59942}"/>
+    <hyperlink ref="F39" r:id="rId88" xr:uid="{BE62AF36-7AA6-4406-AFF8-9F3115F21F55}"/>
+    <hyperlink ref="F40" r:id="rId89" xr:uid="{F25BE1B9-1510-441A-AAFA-DF6891FF8B05}"/>
+    <hyperlink ref="F41" r:id="rId90" xr:uid="{11F96174-8B3C-4613-85E9-350625C89D71}"/>
+    <hyperlink ref="F42" r:id="rId91" xr:uid="{C7F3DFE2-6162-40CE-B017-111E00CFAD88}"/>
+    <hyperlink ref="F43" r:id="rId92" xr:uid="{B26C47F5-95B0-4CC6-B7C5-0FE5DE9F1D48}"/>
+    <hyperlink ref="F45" r:id="rId93" xr:uid="{E7E699D9-2D8A-4D90-95AE-279E34EA3635}"/>
+    <hyperlink ref="F46" r:id="rId94" xr:uid="{EA0D98A0-8359-4E91-B63A-C1C396B4852D}"/>
+    <hyperlink ref="F47" r:id="rId95" xr:uid="{34320072-4E10-45E9-8D5D-BF9565901E63}"/>
+    <hyperlink ref="F48" r:id="rId96" xr:uid="{71EEB8E7-415C-491D-ACDA-28BD6EC8DAB9}"/>
+    <hyperlink ref="F49" r:id="rId97" xr:uid="{F981C0FD-B38B-4960-8DBB-EC5EA32CA8E4}"/>
+    <hyperlink ref="F50" r:id="rId98" xr:uid="{CC47B797-0670-4FF9-AD9A-4358EB33B930}"/>
+    <hyperlink ref="F51" r:id="rId99" xr:uid="{F7B96616-D53A-4F58-B521-274BFA3DE2D4}"/>
+    <hyperlink ref="F52" r:id="rId100" xr:uid="{C5E1A3DC-4A02-46E5-B64F-3CBD1622553F}"/>
+    <hyperlink ref="F53" r:id="rId101" xr:uid="{1B3B5741-7720-4623-B744-D0AB9868A3BE}"/>
+    <hyperlink ref="F54" r:id="rId102" xr:uid="{BCB4D44C-B26F-4521-A900-DE2BFF96C039}"/>
+    <hyperlink ref="E44" r:id="rId103" location="Czech" xr:uid="{7F9BF6E5-10D6-4AB2-B055-BFE1534EF9EA}"/>
+    <hyperlink ref="F44" r:id="rId104" xr:uid="{F1E6A50C-E7E7-4374-88E6-E7BA966011B4}"/>
+    <hyperlink ref="E15" r:id="rId105" location="Czech" xr:uid="{F9F8C814-645A-4735-BA5D-BAE32DB9FA72}"/>
+    <hyperlink ref="F15" r:id="rId106" xr:uid="{F0FFCB4D-A4EC-4E5C-8ECC-6663DEFFE439}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId105"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId107"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed footwear and sweater
</commit_message>
<xml_diff>
--- a/data/vocab.xlsx
+++ b/data/vocab.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oisin\Documents\Czech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CzechTutor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872E4536-6663-47B9-92FF-DD040D7C8318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC2DFD1-8E7C-4F80-A2E2-8F70269CA85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
   </bookViews>
   <sheets>
     <sheet name="Adjectives" sheetId="14" r:id="rId1"/>
@@ -4304,9 +4304,6 @@
     <t>https://free-images.com/lg/709d/clothes_line_clothes_dry.jpg</t>
   </si>
   <si>
-    <t>jumper</t>
-  </si>
-  <si>
     <t>svetr</t>
   </si>
   <si>
@@ -4781,9 +4778,6 @@
     <t>boot</t>
   </si>
   <si>
-    <t>shoe</t>
-  </si>
-  <si>
     <t>https://en.wiktionary.org/wiki/bota#Czech</t>
   </si>
   <si>
@@ -5085,6 +5079,12 @@
   </si>
   <si>
     <t>https://free-images.com/lg/42a3/ship_passenger_ship_cruise.jpg</t>
+  </si>
+  <si>
+    <t>footwear</t>
+  </si>
+  <si>
+    <t>sweater</t>
   </si>
 </sst>
 </file>
@@ -5148,13 +5148,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5493,27 +5493,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>558</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>559</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
         <v>554</v>
       </c>
@@ -5538,16 +5538,16 @@
       <c r="I2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="J2" s="7"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>552</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>553</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="6"/>
       <c r="D3" t="s">
         <v>560</v>
       </c>
@@ -5557,10 +5557,10 @@
       <c r="F3" t="s">
         <v>562</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>561</v>
       </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="6"/>
       <c r="I3" t="s">
         <v>560</v>
       </c>
@@ -5572,10 +5572,10 @@
       <c r="A4" t="s">
         <v>564</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>563</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="6"/>
       <c r="D4" t="s">
         <v>567</v>
       </c>
@@ -5585,10 +5585,10 @@
       <c r="F4" t="s">
         <v>569</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>568</v>
       </c>
-      <c r="H4" s="8"/>
+      <c r="H4" s="6"/>
       <c r="I4" t="s">
         <v>567</v>
       </c>
@@ -5600,10 +5600,10 @@
       <c r="A5" t="s">
         <v>666</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>667</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="6"/>
       <c r="D5" t="s">
         <v>668</v>
       </c>
@@ -5613,10 +5613,10 @@
       <c r="F5" t="s">
         <v>670</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>669</v>
       </c>
-      <c r="H5" s="8"/>
+      <c r="H5" s="6"/>
       <c r="I5" t="s">
         <v>668</v>
       </c>
@@ -5628,10 +5628,10 @@
       <c r="A6" t="s">
         <v>672</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>673</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="6"/>
       <c r="D6" t="s">
         <v>674</v>
       </c>
@@ -5641,10 +5641,10 @@
       <c r="F6" t="s">
         <v>676</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>675</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="6"/>
       <c r="I6" t="s">
         <v>674</v>
       </c>
@@ -5656,10 +5656,10 @@
       <c r="A7" t="s">
         <v>677</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>679</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="6"/>
       <c r="D7" t="s">
         <v>680</v>
       </c>
@@ -5669,10 +5669,10 @@
       <c r="F7" t="s">
         <v>682</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>681</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="6"/>
       <c r="I7" t="s">
         <v>680</v>
       </c>
@@ -5684,10 +5684,10 @@
       <c r="A8" t="s">
         <v>685</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>684</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="6"/>
       <c r="D8" t="s">
         <v>686</v>
       </c>
@@ -5697,10 +5697,10 @@
       <c r="F8" t="s">
         <v>688</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>687</v>
       </c>
-      <c r="H8" s="8"/>
+      <c r="H8" s="6"/>
       <c r="I8" t="s">
         <v>686</v>
       </c>
@@ -5712,10 +5712,10 @@
       <c r="A9" t="s">
         <v>690</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>691</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="6"/>
       <c r="D9" t="s">
         <v>692</v>
       </c>
@@ -5725,10 +5725,10 @@
       <c r="F9" t="s">
         <v>694</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>693</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="6"/>
       <c r="I9" t="s">
         <v>692</v>
       </c>
@@ -5740,10 +5740,10 @@
       <c r="A10" t="s">
         <v>699</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="6"/>
       <c r="D10" t="s">
         <v>697</v>
       </c>
@@ -5753,10 +5753,10 @@
       <c r="F10" t="s">
         <v>700</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="6" t="s">
         <v>698</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="6"/>
       <c r="I10" t="s">
         <v>697</v>
       </c>
@@ -5768,10 +5768,10 @@
       <c r="A11" t="s">
         <v>702</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="6"/>
       <c r="D11" t="s">
         <v>701</v>
       </c>
@@ -5781,10 +5781,10 @@
       <c r="F11" t="s">
         <v>701</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="H11" s="8"/>
+      <c r="H11" s="6"/>
       <c r="I11" t="s">
         <v>701</v>
       </c>
@@ -5796,10 +5796,10 @@
       <c r="A12" t="s">
         <v>704</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="6" t="s">
         <v>705</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="6"/>
       <c r="D12" t="s">
         <v>707</v>
       </c>
@@ -5809,10 +5809,10 @@
       <c r="F12" t="s">
         <v>709</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="6" t="s">
         <v>708</v>
       </c>
-      <c r="H12" s="8"/>
+      <c r="H12" s="6"/>
       <c r="I12" t="s">
         <v>707</v>
       </c>
@@ -5824,10 +5824,10 @@
       <c r="A13" t="s">
         <v>710</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>711</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="6"/>
       <c r="D13" t="s">
         <v>713</v>
       </c>
@@ -5837,10 +5837,10 @@
       <c r="F13" t="s">
         <v>715</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
         <v>714</v>
       </c>
-      <c r="H13" s="8"/>
+      <c r="H13" s="6"/>
       <c r="I13" t="s">
         <v>713</v>
       </c>
@@ -5849,114 +5849,134 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="B19:C19"/>
@@ -5973,37 +5993,17 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" location="Czech" xr:uid="{5941DCB9-FDEB-4587-B027-375759EB9DA4}"/>
@@ -7669,7 +7669,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -7684,7 +7684,7 @@
         <v>749</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -7709,22 +7709,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1621</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1621</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1623</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>1624</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1623</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1623</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1625</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>1626</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -7829,22 +7829,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1641</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>1642</v>
       </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1643</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1645</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>1644</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>1646</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -8035,56 +8035,56 @@
         <v>263</v>
       </c>
       <c r="C23" t="s">
+        <v>1645</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1646</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>1647</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" s="1" t="s">
         <v>1648</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>1649</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>1650</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24" t="s">
+        <v>1632</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1633</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1631</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>1634</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1635</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>1633</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>1636</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1626</v>
+      </c>
+      <c r="D25" t="s">
         <v>1627</v>
       </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E25" s="1" t="s">
         <v>1628</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" s="1" t="s">
         <v>1629</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>1630</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>1631</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -8129,22 +8129,22 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
       <c r="C28" t="s">
+        <v>1635</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1638</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>1637</v>
       </c>
-      <c r="D28" t="s">
-        <v>1640</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>1639</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>1641</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -8249,22 +8249,22 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="B34" t="s">
         <v>263</v>
       </c>
       <c r="C34" t="s">
+        <v>1612</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1613</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>1614</v>
       </c>
-      <c r="D34" t="s">
+      <c r="F34" s="1" t="s">
         <v>1615</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>1616</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>1617</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -8473,7 +8473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A83DE8-6398-4B6D-9AFD-F64AA71A004A}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -8569,22 +8569,22 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="D5" t="s">
+        <v>1490</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>1491</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1490</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>1492</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -8629,22 +8629,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D8" t="s">
         <v>1495</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
+        <v>1492</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>1496</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1493</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>1497</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -8669,22 +8669,22 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
       <c r="C10" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1480</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>1479</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" s="1" t="s">
         <v>1481</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1480</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>1482</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -8729,22 +8729,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
+        <v>1546</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1544</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>1547</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1546</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>1545</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>1548</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -8869,22 +8869,22 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>1482</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
         <v>1483</v>
       </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>1484</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" s="1" t="s">
         <v>1485</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>1486</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>1487</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -8929,22 +8929,22 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>1473</v>
       </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1475</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="F23" s="1" t="s">
         <v>1476</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>1474</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>1477</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -9129,22 +9129,22 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
         <v>1535</v>
       </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>1536</v>
       </c>
-      <c r="D33" t="s">
-        <v>1536</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>1537</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>1538</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -9189,22 +9189,22 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1540</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>1539</v>
       </c>
-      <c r="B36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="F36" s="1" t="s">
         <v>1542</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1541</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>1540</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>1543</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -9349,22 +9349,22 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="B44" t="s">
         <v>26</v>
       </c>
       <c r="C44" t="s">
+        <v>1468</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1470</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>1469</v>
       </c>
-      <c r="D44" t="s">
+      <c r="F44" s="1" t="s">
         <v>1471</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>1470</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>1472</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -9534,13 +9534,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02B6D68-A19F-4652-B7B7-7654A45BC946}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
@@ -9570,42 +9570,42 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1604</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1606</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1605</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1606</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1608</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>1607</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1609</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1576</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1577</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>1575</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" s="1" t="s">
         <v>1578</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1579</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1577</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1580</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -9630,362 +9630,362 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="B5" t="s">
         <v>263</v>
       </c>
       <c r="C5" t="s">
+        <v>1560</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>1561</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="1" t="s">
         <v>1563</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1562</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>1564</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="B6" t="s">
         <v>263</v>
       </c>
       <c r="C6" t="s">
+        <v>1600</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1600</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1601</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>1602</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1602</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>1603</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>1604</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1609</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1609</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>1610</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F7" s="1" t="s">
         <v>1611</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1611</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1612</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>1613</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>1521</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>1521</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>1522</v>
       </c>
-      <c r="D8" t="s">
-        <v>1522</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>1523</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>1524</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>1518</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1517</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1517</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>1519</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>1520</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="B10" t="s">
         <v>263</v>
       </c>
       <c r="C10" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D10" t="s">
         <v>1551</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="1" t="s">
         <v>1552</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>1553</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>1554</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>1565</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>1566</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="1" t="s">
         <v>1567</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>1568</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>1569</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>1430</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>1431</v>
       </c>
-      <c r="D12" t="s">
-        <v>1431</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>1432</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>1433</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1417</v>
+        <v>1677</v>
       </c>
       <c r="B13" t="s">
         <v>263</v>
       </c>
       <c r="C13" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>1418</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" s="1" t="s">
         <v>1420</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>1419</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>1421</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
         <v>1586</v>
       </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>1587</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1585</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>1588</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1589</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1587</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>1590</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>1427</v>
       </c>
-      <c r="D15" t="s">
-        <v>1427</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>1428</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>1429</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
         <v>1556</v>
       </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>1557</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="1" t="s">
+        <v>1554</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>1558</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>1555</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1559</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
         <v>1422</v>
       </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>1423</v>
       </c>
-      <c r="D17" t="s">
-        <v>1423</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>1424</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>1425</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1576</v>
+        <v>1676</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D18" t="s">
         <v>1439</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" s="1" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>1440</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>1442</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>1441</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
         <v>1435</v>
       </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>1436</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="1" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>1437</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>1434</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>1438</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="B20" t="s">
         <v>263</v>
       </c>
       <c r="C20" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="D20" t="s">
+        <v>1581</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>1583</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>1582</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>1585</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
         <v>1426</v>
       </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>1427</v>
       </c>
-      <c r="D21" t="s">
-        <v>1427</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>1428</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>1429</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="B22" t="s">
         <v>27</v>
       </c>
       <c r="C22" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D22" t="s">
         <v>1571</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" s="1" t="s">
         <v>1572</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>1573</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>1574</v>
       </c>
     </row>
   </sheetData>
@@ -10044,8 +10044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4FF4F7-C7FC-4558-887A-7BA51F1283D1}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10180,42 +10180,42 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
       </c>
       <c r="C7" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1658</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>1659</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1660</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1658</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>1661</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
       <c r="C8" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1652</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1653</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>1654</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1654</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1655</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>1656</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -10260,22 +10260,22 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1621</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1621</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1623</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>1624</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1623</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1623</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1625</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>1626</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -10354,22 +10354,22 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1617</v>
+      </c>
+      <c r="D16" t="s">
         <v>1618</v>
       </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="E16" s="1" t="s">
         <v>1619</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" s="1" t="s">
         <v>1620</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>1621</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>1622</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -10714,22 +10714,22 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
         <v>1673</v>
       </c>
-      <c r="B34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>1674</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>1675</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1676</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>1674</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>1677</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -10874,7 +10874,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="B42" t="s">
         <v>27</v>
@@ -10974,22 +10974,22 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="B47" t="s">
         <v>263</v>
       </c>
       <c r="C47" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1667</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>1668</v>
       </c>
-      <c r="D47" t="s">
+      <c r="F47" s="1" t="s">
         <v>1669</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>1670</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>1671</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -11034,22 +11034,22 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D50" t="s">
         <v>1662</v>
       </c>
-      <c r="B50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="E50" s="1" t="s">
         <v>1663</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F50" s="1" t="s">
         <v>1664</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>1665</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>1666</v>
       </c>
     </row>
   </sheetData>
@@ -11279,22 +11279,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B4" t="s">
         <v>263</v>
       </c>
       <c r="C4" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D4" t="s">
+        <v>1504</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>1505</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1504</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1506</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -11419,22 +11419,22 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>1513</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1512</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>1514</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1513</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1513</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>1515</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>1516</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -11539,22 +11539,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B17" t="s">
         <v>263</v>
       </c>
       <c r="C17" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1510</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>1509</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" s="1" t="s">
         <v>1511</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>1510</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>1512</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -11619,22 +11619,22 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
         <v>1498</v>
       </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>1499</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="1" t="s">
         <v>1500</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>1501</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -11834,22 +11834,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>1463</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>1465</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>1464</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" s="1" t="s">
         <v>1466</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1465</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1467</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -12038,22 +12038,22 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="B3" t="s">
         <v>263</v>
       </c>
       <c r="C3" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1450</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>1449</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="1" t="s">
         <v>1451</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1450</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>1452</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -12198,22 +12198,22 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B11" t="s">
         <v>263</v>
       </c>
       <c r="C11" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>1459</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" s="1" t="s">
         <v>1461</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1460</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>1462</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -12238,22 +12238,22 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="B13" t="s">
         <v>263</v>
       </c>
       <c r="C13" t="s">
+        <v>1595</v>
+      </c>
+      <c r="D13" t="s">
         <v>1597</v>
       </c>
-      <c r="D13" t="s">
-        <v>1599</v>
-      </c>
       <c r="E13" s="1" t="s">
+        <v>1596</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>1598</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>1600</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -12338,22 +12338,22 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B18" t="s">
         <v>263</v>
       </c>
       <c r="C18" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1455</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>1454</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" s="1" t="s">
         <v>1456</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>1455</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>1457</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -12518,22 +12518,22 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>1443</v>
       </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1445</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="F27" s="1" t="s">
         <v>1446</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>1444</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>1447</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -13098,22 +13098,22 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1527</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1526</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>1525</v>
       </c>
-      <c r="B56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="F56" s="1" t="s">
         <v>1528</v>
-      </c>
-      <c r="D56" t="s">
-        <v>1527</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>1526</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>1529</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -13258,22 +13258,22 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="B64" t="s">
         <v>263</v>
       </c>
       <c r="C64" t="s">
+        <v>1590</v>
+      </c>
+      <c r="D64" t="s">
         <v>1592</v>
       </c>
-      <c r="D64" t="s">
-        <v>1594</v>
-      </c>
       <c r="E64" s="1" t="s">
+        <v>1591</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>1593</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>1595</v>
       </c>
     </row>
   </sheetData>
@@ -13713,22 +13713,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1658</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>1659</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1660</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1658</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>1661</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -14293,22 +14293,22 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B44" t="s">
         <v>27</v>
       </c>
       <c r="C44" t="s">
+        <v>1531</v>
+      </c>
+      <c r="D44" t="s">
         <v>1532</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>1533</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>1531</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>1534</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added bikini and hoodie
</commit_message>
<xml_diff>
--- a/data/vocab.xlsx
+++ b/data/vocab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CzechTutor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC2DFD1-8E7C-4F80-A2E2-8F70269CA85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146BAAF9-865E-4D27-8DA1-B3645BA7EDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{52A82FCD-7763-4C45-82C3-9308E9D1C04C}"/>
   </bookViews>
   <sheets>
     <sheet name="Adjectives" sheetId="14" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2296" uniqueCount="1678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="1692">
   <si>
     <t>English</t>
   </si>
@@ -5085,6 +5085,48 @@
   </si>
   <si>
     <t>sweater</t>
+  </si>
+  <si>
+    <t>cocktail</t>
+  </si>
+  <si>
+    <t>koktejl</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/koktejl#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b6a5/cocktail_drink_beverage_1040857.jpg</t>
+  </si>
+  <si>
+    <t>koktejly</t>
+  </si>
+  <si>
+    <t>hoodie</t>
+  </si>
+  <si>
+    <t>mikina</t>
+  </si>
+  <si>
+    <t>mikiny</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/mikina#Czech</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/1a57/portrait_male_young_hoodie.jpg</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/bikiny#Czech</t>
+  </si>
+  <si>
+    <t>bikini</t>
+  </si>
+  <si>
+    <t>bikiny</t>
+  </si>
+  <si>
+    <t>https://free-images.com/lg/b59c/bikini_two_piece_swimwear.jpg</t>
   </si>
 </sst>
 </file>
@@ -5148,13 +5190,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5493,27 +5535,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>558</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>559</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
         <v>554</v>
       </c>
@@ -5538,16 +5580,16 @@
       <c r="I2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="J2" s="8"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>552</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="8"/>
       <c r="D3" t="s">
         <v>560</v>
       </c>
@@ -5557,10 +5599,10 @@
       <c r="F3" t="s">
         <v>562</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="8"/>
       <c r="I3" t="s">
         <v>560</v>
       </c>
@@ -5572,10 +5614,10 @@
       <c r="A4" t="s">
         <v>564</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="8"/>
       <c r="D4" t="s">
         <v>567</v>
       </c>
@@ -5585,10 +5627,10 @@
       <c r="F4" t="s">
         <v>569</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="8"/>
       <c r="I4" t="s">
         <v>567</v>
       </c>
@@ -5600,10 +5642,10 @@
       <c r="A5" t="s">
         <v>666</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>667</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="8"/>
       <c r="D5" t="s">
         <v>668</v>
       </c>
@@ -5613,10 +5655,10 @@
       <c r="F5" t="s">
         <v>670</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="8"/>
       <c r="I5" t="s">
         <v>668</v>
       </c>
@@ -5628,10 +5670,10 @@
       <c r="A6" t="s">
         <v>672</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>674</v>
       </c>
@@ -5641,10 +5683,10 @@
       <c r="F6" t="s">
         <v>676</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="8" t="s">
         <v>675</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="8"/>
       <c r="I6" t="s">
         <v>674</v>
       </c>
@@ -5656,10 +5698,10 @@
       <c r="A7" t="s">
         <v>677</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="8"/>
       <c r="D7" t="s">
         <v>680</v>
       </c>
@@ -5669,10 +5711,10 @@
       <c r="F7" t="s">
         <v>682</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="8" t="s">
         <v>681</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="8"/>
       <c r="I7" t="s">
         <v>680</v>
       </c>
@@ -5684,10 +5726,10 @@
       <c r="A8" t="s">
         <v>685</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>684</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="8"/>
       <c r="D8" t="s">
         <v>686</v>
       </c>
@@ -5697,10 +5739,10 @@
       <c r="F8" t="s">
         <v>688</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="8"/>
       <c r="I8" t="s">
         <v>686</v>
       </c>
@@ -5712,10 +5754,10 @@
       <c r="A9" t="s">
         <v>690</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="8"/>
       <c r="D9" t="s">
         <v>692</v>
       </c>
@@ -5725,10 +5767,10 @@
       <c r="F9" t="s">
         <v>694</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="8" t="s">
         <v>693</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="8"/>
       <c r="I9" t="s">
         <v>692</v>
       </c>
@@ -5740,10 +5782,10 @@
       <c r="A10" t="s">
         <v>699</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>696</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="8"/>
       <c r="D10" t="s">
         <v>697</v>
       </c>
@@ -5753,10 +5795,10 @@
       <c r="F10" t="s">
         <v>700</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="8"/>
       <c r="I10" t="s">
         <v>697</v>
       </c>
@@ -5768,10 +5810,10 @@
       <c r="A11" t="s">
         <v>702</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="8"/>
       <c r="D11" t="s">
         <v>701</v>
       </c>
@@ -5781,10 +5823,10 @@
       <c r="F11" t="s">
         <v>701</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="8" t="s">
         <v>701</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="8"/>
       <c r="I11" t="s">
         <v>701</v>
       </c>
@@ -5796,10 +5838,10 @@
       <c r="A12" t="s">
         <v>704</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="8"/>
       <c r="D12" t="s">
         <v>707</v>
       </c>
@@ -5809,10 +5851,10 @@
       <c r="F12" t="s">
         <v>709</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="8" t="s">
         <v>708</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="8"/>
       <c r="I12" t="s">
         <v>707</v>
       </c>
@@ -5824,10 +5866,10 @@
       <c r="A13" t="s">
         <v>710</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="8"/>
       <c r="D13" t="s">
         <v>713</v>
       </c>
@@ -5837,10 +5879,10 @@
       <c r="F13" t="s">
         <v>715</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="8" t="s">
         <v>714</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="8"/>
       <c r="I13" t="s">
         <v>713</v>
       </c>
@@ -5849,134 +5891,114 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="B19:C19"/>
@@ -5993,17 +6015,37 @@
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1" location="Czech" xr:uid="{5941DCB9-FDEB-4587-B027-375759EB9DA4}"/>
@@ -8473,8 +8515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A83DE8-6398-4B6D-9AFD-F64AA71A004A}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9532,10 +9574,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02B6D68-A19F-4652-B7B7-7654A45BC946}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9570,473 +9612,518 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1603</v>
+        <v>1689</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>1604</v>
+        <v>1690</v>
       </c>
       <c r="D2" t="s">
-        <v>1606</v>
+        <v>1690</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1605</v>
+        <v>1688</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1607</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1574</v>
+        <v>1603</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>1576</v>
+        <v>1604</v>
       </c>
       <c r="D3" t="s">
-        <v>1577</v>
+        <v>1606</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1575</v>
+        <v>1605</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1578</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1413</v>
+        <v>1574</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>1415</v>
+        <v>1576</v>
       </c>
       <c r="D4" t="s">
-        <v>1415</v>
+        <v>1577</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1414</v>
+        <v>1575</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1416</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1559</v>
+        <v>1413</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>1560</v>
+        <v>1415</v>
       </c>
       <c r="D5" t="s">
-        <v>1562</v>
+        <v>1415</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1561</v>
+        <v>1414</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1563</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>1599</v>
+        <v>1559</v>
       </c>
       <c r="B6" t="s">
         <v>263</v>
       </c>
       <c r="C6" t="s">
-        <v>1600</v>
+        <v>1560</v>
       </c>
       <c r="D6" t="s">
-        <v>1600</v>
+        <v>1562</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1601</v>
+        <v>1561</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1602</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1608</v>
+        <v>1599</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C7" t="s">
-        <v>1609</v>
+        <v>1600</v>
       </c>
       <c r="D7" t="s">
-        <v>1609</v>
+        <v>1600</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1610</v>
+        <v>1601</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1611</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1520</v>
+        <v>1676</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>1521</v>
+        <v>1438</v>
       </c>
       <c r="D8" t="s">
-        <v>1521</v>
+        <v>1439</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1522</v>
+        <v>1441</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1523</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>1517</v>
+        <v>1608</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>1516</v>
+        <v>1609</v>
       </c>
       <c r="D9" t="s">
-        <v>1516</v>
+        <v>1609</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1518</v>
+        <v>1610</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1519</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>1549</v>
+        <v>1520</v>
       </c>
       <c r="B10" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>1550</v>
+        <v>1521</v>
       </c>
       <c r="D10" t="s">
-        <v>1551</v>
+        <v>1521</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1552</v>
+        <v>1522</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1553</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>1564</v>
+        <v>1517</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>1565</v>
+        <v>1516</v>
       </c>
       <c r="D11" t="s">
-        <v>1566</v>
+        <v>1516</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1567</v>
+        <v>1518</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1568</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>1429</v>
+        <v>1549</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C12" t="s">
-        <v>1430</v>
+        <v>1550</v>
       </c>
       <c r="D12" t="s">
-        <v>1430</v>
+        <v>1551</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1431</v>
+        <v>1552</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1432</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>1677</v>
+        <v>1683</v>
       </c>
       <c r="B13" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>1417</v>
+        <v>1684</v>
       </c>
       <c r="D13" t="s">
-        <v>1419</v>
+        <v>1685</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1418</v>
+        <v>1686</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1420</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>1584</v>
+        <v>1564</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>1586</v>
+        <v>1565</v>
       </c>
       <c r="D14" t="s">
-        <v>1587</v>
+        <v>1566</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1585</v>
+        <v>1567</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1588</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>1548</v>
+        <v>1429</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>1426</v>
+        <v>1430</v>
       </c>
       <c r="D15" t="s">
-        <v>1426</v>
+        <v>1430</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1427</v>
+        <v>1431</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1428</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>1555</v>
+        <v>1584</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>1556</v>
+        <v>1586</v>
       </c>
       <c r="D16" t="s">
-        <v>1557</v>
+        <v>1587</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>1554</v>
+        <v>1585</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1558</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>1421</v>
+        <v>1548</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>1422</v>
+        <v>1426</v>
       </c>
       <c r="D17" t="s">
-        <v>1422</v>
+        <v>1426</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>1423</v>
+        <v>1427</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1424</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1676</v>
+        <v>1555</v>
       </c>
       <c r="B18" t="s">
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>1438</v>
+        <v>1556</v>
       </c>
       <c r="D18" t="s">
-        <v>1439</v>
+        <v>1557</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>1441</v>
+        <v>1554</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1440</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1434</v>
+        <v>1421</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>1435</v>
+        <v>1422</v>
       </c>
       <c r="D19" t="s">
-        <v>1436</v>
+        <v>1422</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>1433</v>
+        <v>1423</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1437</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1579</v>
+        <v>1434</v>
       </c>
       <c r="B20" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>1582</v>
+        <v>1435</v>
       </c>
       <c r="D20" t="s">
-        <v>1581</v>
+        <v>1436</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1580</v>
+        <v>1433</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1583</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1425</v>
+        <v>1579</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C21" t="s">
-        <v>1426</v>
+        <v>1582</v>
       </c>
       <c r="D21" t="s">
-        <v>1426</v>
+        <v>1581</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>1427</v>
+        <v>1580</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1428</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1417</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1418</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>1569</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>1570</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D24" t="s">
         <v>1571</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>1572</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>1573</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F22">
-    <sortCondition ref="A1:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
+    <sortCondition ref="A1:A24"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" location="Czech" xr:uid="{C8D8497D-6936-4602-A837-16F055153702}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{C558574F-D182-4A25-B3D3-C6E86CFE22B6}"/>
-    <hyperlink ref="E13" r:id="rId3" location="Czech" xr:uid="{F73E5D9B-0502-4A1F-A1BB-CCD4AF247DB2}"/>
-    <hyperlink ref="F13" r:id="rId4" xr:uid="{D1C3222C-EA71-42CD-BCC1-A152ACD54837}"/>
-    <hyperlink ref="E17" r:id="rId5" location="Czech" xr:uid="{368B4523-DC09-425D-B789-490AF67DAA66}"/>
-    <hyperlink ref="F17" r:id="rId6" xr:uid="{289473E4-EA0A-4E90-A737-60A105E61338}"/>
-    <hyperlink ref="E21" r:id="rId7" location="Czech" xr:uid="{ABC5B473-C91F-4FC1-9730-1B96F2A8F2E9}"/>
-    <hyperlink ref="F21" r:id="rId8" xr:uid="{914CDFDF-B196-4185-8354-74E4D63E44F2}"/>
-    <hyperlink ref="E12" r:id="rId9" location="Czech" xr:uid="{D4528106-044C-42B1-8648-7BB2ECFA53F1}"/>
-    <hyperlink ref="F12" r:id="rId10" xr:uid="{51B782D5-F726-43D7-97F8-5528F560F306}"/>
-    <hyperlink ref="E19" r:id="rId11" location="Czech" xr:uid="{484B463E-63EE-483A-B77B-60985370E3B9}"/>
-    <hyperlink ref="F19" r:id="rId12" xr:uid="{1C5EBBCE-FC4A-4F98-B9BD-38FEDE0D9C51}"/>
-    <hyperlink ref="F18" r:id="rId13" xr:uid="{A03237B3-9F5B-4EF1-8985-7EDBF61BF6DA}"/>
-    <hyperlink ref="E18" r:id="rId14" location="Czech" xr:uid="{D5EE9176-B88B-40B1-9EC2-5FECA94FF553}"/>
-    <hyperlink ref="E9" r:id="rId15" location="Czech" xr:uid="{1C2A5A82-0D54-41E2-9A1B-10EA7B15D3CD}"/>
-    <hyperlink ref="F9" r:id="rId16" xr:uid="{D8B11802-98C3-4790-8B17-4C0AD8CAD33C}"/>
-    <hyperlink ref="E8" r:id="rId17" location="Czech" xr:uid="{8ED7A855-0690-44A6-ABDD-2799AA47325E}"/>
-    <hyperlink ref="F8" r:id="rId18" xr:uid="{DF6D184D-1CBE-445E-8F82-D02E02F59F79}"/>
-    <hyperlink ref="E15" r:id="rId19" location="Czech" xr:uid="{43E92AB7-192F-4B95-883E-F4BFC0A084F6}"/>
-    <hyperlink ref="F15" r:id="rId20" xr:uid="{16A15844-6ACA-4E63-8FA2-D0EB2114986D}"/>
-    <hyperlink ref="E10" r:id="rId21" location="Czech" xr:uid="{35F81671-8E25-4B45-98AA-56A28D9A351A}"/>
-    <hyperlink ref="F10" r:id="rId22" xr:uid="{7E761A3A-920B-41A8-A05B-B4DAADE0650D}"/>
-    <hyperlink ref="E16" r:id="rId23" location="Czech" xr:uid="{28FD7126-C2B0-48E7-BBDE-7EFA78B36BE8}"/>
-    <hyperlink ref="F16" r:id="rId24" xr:uid="{77B44025-1D1A-432B-BBA6-83CD233D3057}"/>
-    <hyperlink ref="E5" r:id="rId25" location="Czech" xr:uid="{433A3175-9F6A-4FD8-992B-C511578D8FDE}"/>
-    <hyperlink ref="F5" r:id="rId26" xr:uid="{4B68679E-8427-48FB-99E4-0B0A69754D86}"/>
-    <hyperlink ref="E11" r:id="rId27" location="Czech" xr:uid="{0A5819DC-0FD8-417B-AA11-D88B9AFDCE42}"/>
-    <hyperlink ref="F11" r:id="rId28" xr:uid="{6E526287-7BF5-4644-B7F7-43A1F345C57C}"/>
-    <hyperlink ref="E22" r:id="rId29" location="Czech" xr:uid="{79AE5194-00B9-4249-BE4F-332D4D4FE237}"/>
-    <hyperlink ref="F22" r:id="rId30" xr:uid="{17A6ED69-69EA-4FB2-8D48-6084ED7FAFE0}"/>
-    <hyperlink ref="E3" r:id="rId31" location="Czech" xr:uid="{61463EB2-A9BE-475D-95E0-2B5D74E52640}"/>
-    <hyperlink ref="F3" r:id="rId32" xr:uid="{8FA6ECA0-EADE-42FC-BEFE-5FE408721FAA}"/>
-    <hyperlink ref="E20" r:id="rId33" xr:uid="{984F0467-C245-4204-8046-C512319F1DAC}"/>
-    <hyperlink ref="F20" r:id="rId34" xr:uid="{1A4CEE22-56B6-4B74-B9DA-58DA4F151F46}"/>
-    <hyperlink ref="E14" r:id="rId35" location="Czech" xr:uid="{E3208E71-8485-4F74-A69B-C03A0F883A5B}"/>
-    <hyperlink ref="F14" r:id="rId36" xr:uid="{D1F656E4-41CF-48D2-B5C4-2271C0428FDE}"/>
-    <hyperlink ref="E6" r:id="rId37" location="Czech" xr:uid="{AAFBFE56-1940-4E83-B3C4-91C4E625CBCA}"/>
-    <hyperlink ref="F6" r:id="rId38" xr:uid="{95E87E59-9499-4E50-962B-8E9431F9CFAE}"/>
-    <hyperlink ref="E2" r:id="rId39" location="Czech" xr:uid="{36F87DC1-17F6-441A-B77B-14315280BCE9}"/>
-    <hyperlink ref="F2" r:id="rId40" xr:uid="{FA750C57-CF30-4179-825D-FEABB91271DC}"/>
-    <hyperlink ref="E7" r:id="rId41" location="Czech" xr:uid="{7F57C436-6DCE-4DF6-8E41-85C4727BE8C6}"/>
-    <hyperlink ref="F7" r:id="rId42" xr:uid="{5DF7A61C-3A2B-4509-ADEC-A2E313C7DF0F}"/>
+    <hyperlink ref="E5" r:id="rId1" location="Czech" xr:uid="{C8D8497D-6936-4602-A837-16F055153702}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{C558574F-D182-4A25-B3D3-C6E86CFE22B6}"/>
+    <hyperlink ref="E22" r:id="rId3" location="Czech" xr:uid="{F73E5D9B-0502-4A1F-A1BB-CCD4AF247DB2}"/>
+    <hyperlink ref="F22" r:id="rId4" xr:uid="{D1C3222C-EA71-42CD-BCC1-A152ACD54837}"/>
+    <hyperlink ref="E19" r:id="rId5" location="Czech" xr:uid="{368B4523-DC09-425D-B789-490AF67DAA66}"/>
+    <hyperlink ref="F19" r:id="rId6" xr:uid="{289473E4-EA0A-4E90-A737-60A105E61338}"/>
+    <hyperlink ref="E23" r:id="rId7" location="Czech" xr:uid="{ABC5B473-C91F-4FC1-9730-1B96F2A8F2E9}"/>
+    <hyperlink ref="F23" r:id="rId8" xr:uid="{914CDFDF-B196-4185-8354-74E4D63E44F2}"/>
+    <hyperlink ref="E15" r:id="rId9" location="Czech" xr:uid="{D4528106-044C-42B1-8648-7BB2ECFA53F1}"/>
+    <hyperlink ref="F15" r:id="rId10" xr:uid="{51B782D5-F726-43D7-97F8-5528F560F306}"/>
+    <hyperlink ref="E20" r:id="rId11" location="Czech" xr:uid="{484B463E-63EE-483A-B77B-60985370E3B9}"/>
+    <hyperlink ref="F20" r:id="rId12" xr:uid="{1C5EBBCE-FC4A-4F98-B9BD-38FEDE0D9C51}"/>
+    <hyperlink ref="F8" r:id="rId13" xr:uid="{A03237B3-9F5B-4EF1-8985-7EDBF61BF6DA}"/>
+    <hyperlink ref="E8" r:id="rId14" location="Czech" xr:uid="{D5EE9176-B88B-40B1-9EC2-5FECA94FF553}"/>
+    <hyperlink ref="E11" r:id="rId15" location="Czech" xr:uid="{1C2A5A82-0D54-41E2-9A1B-10EA7B15D3CD}"/>
+    <hyperlink ref="F11" r:id="rId16" xr:uid="{D8B11802-98C3-4790-8B17-4C0AD8CAD33C}"/>
+    <hyperlink ref="E10" r:id="rId17" location="Czech" xr:uid="{8ED7A855-0690-44A6-ABDD-2799AA47325E}"/>
+    <hyperlink ref="F10" r:id="rId18" xr:uid="{DF6D184D-1CBE-445E-8F82-D02E02F59F79}"/>
+    <hyperlink ref="E17" r:id="rId19" location="Czech" xr:uid="{43E92AB7-192F-4B95-883E-F4BFC0A084F6}"/>
+    <hyperlink ref="F17" r:id="rId20" xr:uid="{16A15844-6ACA-4E63-8FA2-D0EB2114986D}"/>
+    <hyperlink ref="E12" r:id="rId21" location="Czech" xr:uid="{35F81671-8E25-4B45-98AA-56A28D9A351A}"/>
+    <hyperlink ref="F12" r:id="rId22" xr:uid="{7E761A3A-920B-41A8-A05B-B4DAADE0650D}"/>
+    <hyperlink ref="E18" r:id="rId23" location="Czech" xr:uid="{28FD7126-C2B0-48E7-BBDE-7EFA78B36BE8}"/>
+    <hyperlink ref="F18" r:id="rId24" xr:uid="{77B44025-1D1A-432B-BBA6-83CD233D3057}"/>
+    <hyperlink ref="E6" r:id="rId25" location="Czech" xr:uid="{433A3175-9F6A-4FD8-992B-C511578D8FDE}"/>
+    <hyperlink ref="F6" r:id="rId26" xr:uid="{4B68679E-8427-48FB-99E4-0B0A69754D86}"/>
+    <hyperlink ref="E14" r:id="rId27" location="Czech" xr:uid="{0A5819DC-0FD8-417B-AA11-D88B9AFDCE42}"/>
+    <hyperlink ref="F14" r:id="rId28" xr:uid="{6E526287-7BF5-4644-B7F7-43A1F345C57C}"/>
+    <hyperlink ref="E24" r:id="rId29" location="Czech" xr:uid="{79AE5194-00B9-4249-BE4F-332D4D4FE237}"/>
+    <hyperlink ref="F24" r:id="rId30" xr:uid="{17A6ED69-69EA-4FB2-8D48-6084ED7FAFE0}"/>
+    <hyperlink ref="E4" r:id="rId31" location="Czech" xr:uid="{61463EB2-A9BE-475D-95E0-2B5D74E52640}"/>
+    <hyperlink ref="F4" r:id="rId32" xr:uid="{8FA6ECA0-EADE-42FC-BEFE-5FE408721FAA}"/>
+    <hyperlink ref="E21" r:id="rId33" xr:uid="{984F0467-C245-4204-8046-C512319F1DAC}"/>
+    <hyperlink ref="F21" r:id="rId34" xr:uid="{1A4CEE22-56B6-4B74-B9DA-58DA4F151F46}"/>
+    <hyperlink ref="E16" r:id="rId35" location="Czech" xr:uid="{E3208E71-8485-4F74-A69B-C03A0F883A5B}"/>
+    <hyperlink ref="F16" r:id="rId36" xr:uid="{D1F656E4-41CF-48D2-B5C4-2271C0428FDE}"/>
+    <hyperlink ref="E7" r:id="rId37" location="Czech" xr:uid="{AAFBFE56-1940-4E83-B3C4-91C4E625CBCA}"/>
+    <hyperlink ref="F7" r:id="rId38" xr:uid="{95E87E59-9499-4E50-962B-8E9431F9CFAE}"/>
+    <hyperlink ref="E3" r:id="rId39" location="Czech" xr:uid="{36F87DC1-17F6-441A-B77B-14315280BCE9}"/>
+    <hyperlink ref="F3" r:id="rId40" xr:uid="{FA750C57-CF30-4179-825D-FEABB91271DC}"/>
+    <hyperlink ref="E9" r:id="rId41" location="Czech" xr:uid="{7F57C436-6DCE-4DF6-8E41-85C4727BE8C6}"/>
+    <hyperlink ref="F9" r:id="rId42" xr:uid="{5DF7A61C-3A2B-4509-ADEC-A2E313C7DF0F}"/>
+    <hyperlink ref="E13" r:id="rId43" location="Czech" xr:uid="{7245FE69-AA7D-4CF4-9333-BC3C4FB0BD64}"/>
+    <hyperlink ref="F13" r:id="rId44" xr:uid="{1ECC4A82-8179-4355-99A5-187FD7DCC1E2}"/>
+    <hyperlink ref="E2" r:id="rId45" location="Czech" xr:uid="{147868EB-8F8A-4D8A-BFE2-8506E6F8AB68}"/>
+    <hyperlink ref="F2" r:id="rId46" xr:uid="{AF6A9AB1-B1B8-47B0-9446-CB31E2CBF694}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId47"/>
 </worksheet>
 </file>
 
@@ -11756,15 +11843,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF50B53C-5CF5-4C27-A586-77DCF0E5F3F4}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
@@ -11834,145 +11921,167 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1462</v>
+        <v>1678</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>263</v>
       </c>
       <c r="C4" t="s">
-        <v>1463</v>
+        <v>1679</v>
       </c>
       <c r="D4" t="s">
-        <v>1465</v>
+        <v>1682</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1464</v>
+        <v>1680</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1466</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>485</v>
+        <v>1462</v>
       </c>
       <c r="B5" t="s">
-        <v>263</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>486</v>
+        <v>1463</v>
       </c>
       <c r="D5" t="s">
-        <v>488</v>
+        <v>1465</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>487</v>
+        <v>1464</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1203</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>664</v>
+        <v>485</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
-        <v>661</v>
+        <v>486</v>
       </c>
       <c r="D6" t="s">
-        <v>663</v>
+        <v>488</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>662</v>
+        <v>487</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>478</v>
+        <v>664</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>477</v>
+        <v>661</v>
       </c>
       <c r="D7" t="s">
-        <v>480</v>
+        <v>663</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>479</v>
+        <v>662</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>727</v>
+        <v>478</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>721</v>
+        <v>477</v>
       </c>
       <c r="D8" t="s">
-        <v>721</v>
+        <v>480</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>722</v>
+        <v>479</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1201</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>727</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>721</v>
+      </c>
+      <c r="D9" t="s">
+        <v>721</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>497</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>498</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>500</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>1207</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F9">
-    <sortCondition ref="A1:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F10">
+    <sortCondition ref="A1:A10"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" location="Czech" xr:uid="{D08C6A78-C641-4A04-91FA-7DFC8121E4B1}"/>
-    <hyperlink ref="E7" r:id="rId2" location="Czech" xr:uid="{A9EEB33E-7F18-48EB-A28B-502990CCADD3}"/>
+    <hyperlink ref="E10" r:id="rId1" location="Czech" xr:uid="{D08C6A78-C641-4A04-91FA-7DFC8121E4B1}"/>
+    <hyperlink ref="E8" r:id="rId2" location="Czech" xr:uid="{A9EEB33E-7F18-48EB-A28B-502990CCADD3}"/>
     <hyperlink ref="E3" r:id="rId3" location="Czech" xr:uid="{B1C010BF-968A-42D9-8B9F-DC6405985AF0}"/>
-    <hyperlink ref="E5" r:id="rId4" location="Czech" xr:uid="{C010462B-E1BB-4415-9847-63CA7179E6BC}"/>
-    <hyperlink ref="E6" r:id="rId5" location="Czech" xr:uid="{6DF548CA-49AB-42B8-B810-D35D5B88A660}"/>
-    <hyperlink ref="E8" r:id="rId6" location="Czech" xr:uid="{094E0445-352E-473F-AF01-1051B531E551}"/>
+    <hyperlink ref="E6" r:id="rId4" location="Czech" xr:uid="{C010462B-E1BB-4415-9847-63CA7179E6BC}"/>
+    <hyperlink ref="E7" r:id="rId5" location="Czech" xr:uid="{6DF548CA-49AB-42B8-B810-D35D5B88A660}"/>
+    <hyperlink ref="E9" r:id="rId6" location="Czech" xr:uid="{094E0445-352E-473F-AF01-1051B531E551}"/>
     <hyperlink ref="E2" r:id="rId7" location="Czech" xr:uid="{36E6D160-7B61-4284-94EE-00272F0A46B5}"/>
-    <hyperlink ref="F8" r:id="rId8" xr:uid="{1F83B336-51E2-4FED-8DE9-E7D6C121589D}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{1F83B336-51E2-4FED-8DE9-E7D6C121589D}"/>
     <hyperlink ref="F3" r:id="rId9" xr:uid="{2F59FFE9-B0A1-44DF-A78C-201478508AFC}"/>
-    <hyperlink ref="F5" r:id="rId10" xr:uid="{4D8C4A2C-F138-4F58-9364-F9CD1EEB58B1}"/>
-    <hyperlink ref="F6" r:id="rId11" xr:uid="{4094A667-8753-49EC-9242-82EF2076EE31}"/>
-    <hyperlink ref="F7" r:id="rId12" xr:uid="{33E68306-1EDC-4E9F-94B0-5DC437EB5A56}"/>
+    <hyperlink ref="F6" r:id="rId10" xr:uid="{4D8C4A2C-F138-4F58-9364-F9CD1EEB58B1}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{4094A667-8753-49EC-9242-82EF2076EE31}"/>
+    <hyperlink ref="F8" r:id="rId12" xr:uid="{33E68306-1EDC-4E9F-94B0-5DC437EB5A56}"/>
     <hyperlink ref="F2" r:id="rId13" xr:uid="{071524E1-1C12-4C13-BB42-DD6D4DAF49F2}"/>
-    <hyperlink ref="F9" r:id="rId14" xr:uid="{93AB0901-4009-4007-BF5C-1EE76F33C63F}"/>
-    <hyperlink ref="E4" r:id="rId15" location="Czech" xr:uid="{714E1DAF-CA55-48AB-9437-81F3ED4FAACE}"/>
-    <hyperlink ref="F4" r:id="rId16" xr:uid="{F4FCE0FE-8F33-4C96-9E7E-D73A4210D429}"/>
+    <hyperlink ref="F10" r:id="rId14" xr:uid="{93AB0901-4009-4007-BF5C-1EE76F33C63F}"/>
+    <hyperlink ref="E5" r:id="rId15" location="Czech" xr:uid="{714E1DAF-CA55-48AB-9437-81F3ED4FAACE}"/>
+    <hyperlink ref="F5" r:id="rId16" xr:uid="{F4FCE0FE-8F33-4C96-9E7E-D73A4210D429}"/>
+    <hyperlink ref="E4" r:id="rId17" location="Czech" xr:uid="{EED416D9-4DAF-4401-879C-BC84BCEA8ACA}"/>
+    <hyperlink ref="F4" r:id="rId18" xr:uid="{761A74A7-AB10-4ED4-BE6A-A24A680B2D1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>